<commit_message>
Fix parameter extraction and update test cases to XLSX
</commit_message>
<xml_diff>
--- a/harmony_test_results.xlsx
+++ b/harmony_test_results.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D178"/>
+  <dimension ref="A1:D180"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -451,7 +451,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>'s</t>
+          <t>parameter missing. URL: http://foxnews.hb.omtrdc.net/settings/foxnews.xml?r=1673312989724. Please add the</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -473,7 +473,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>'s</t>
+          <t>parameter missing. URL: http://foxnews.hb.omtrdc.net/settings/foxnews.xml?r=1673312989724. Please add the</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -483,7 +483,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Fail: 's:event:sid' parameter missing. URL: http://foxnews.hb.omtrdc.net/settings/foxnews.xml?r=1673312989724. Please add this parameter.</t>
+          <t>Fail: 's:event:type' parameter missing. URL: http://foxnews.hb.omtrdc.net/settings/foxnews.xml?r=1673312989724. Please add the 's:event:type' parameter.</t>
         </is>
       </c>
     </row>
@@ -495,7 +495,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>'l</t>
+          <t>parameter missing. URL: http://foxnews.hb.omtrdc.net/settings/foxnews.xml?r=1673312989724. Please add this parameter.</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -505,7 +505,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Fail: 'l:event:duration' parameter missing. Please add this parameter.</t>
+          <t>Fail: 's:event:sid' parameter missing. URL: http://foxnews.hb.omtrdc.net/settings/foxnews.xml?r=1673312989724. Please add this parameter.</t>
         </is>
       </c>
     </row>
@@ -517,7 +517,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>'l</t>
+          <t>parameter missing. Please add this parameter.</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -527,7 +527,7 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Fail: 'l:event:playhead' parameter missing. Please add this parameter.</t>
+          <t>Fail: 'l:event:duration' parameter missing. Please add this parameter.</t>
         </is>
       </c>
     </row>
@@ -539,7 +539,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>'l</t>
+          <t>parameter missing. Please add this parameter.</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -561,7 +561,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>'l</t>
+          <t>parameter missing. Please add this parameter.</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -583,7 +583,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>'s</t>
+          <t>parameter missing. Please add this parameter.</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -605,7 +605,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>'l</t>
+          <t>parameter missing. Please add this parameter.</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -627,7 +627,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>'s</t>
+          <t>parameter missing. Please add this parameter.</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -649,7 +649,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>'s</t>
+          <t>parameter missing. Please add this parameter.</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -671,7 +671,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>'s</t>
+          <t>parameter missing. URL: http://foxnews.hb.omtrdc.net/settings/foxnews.xml?r=1673312989724. Please add the</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -693,7 +693,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>'s</t>
+          <t>parameter found with value start. URL: http://foxnews.hb.omtrdc.net/?s:sc:rsid=foxnewsglobalproduction&amp;s:sc:tracking_server=smetrics.foxnews.com&amp;h:sc:ssl=1&amp;&amp;&amp;&amp;s:sp:ovp=Akamai&amp;s:sp:channel=Fox+News&amp;s:sp:player_name=Fox+News+Android+Player&amp;s:sp:hb_version=android-2.1.0.154-42fb90&amp;l:sp:hb_api_lvl=4&amp;s:event:sid=1673312989776217636246&amp;l:event:duration=0&amp;l:event:playhead=0&amp;l:event:prev_ts=-1&amp;s:event:type=start&amp;l:event:ts=1673312989797&amp;s:asset:name=Biden+accused+of+mishandling+classified+documents&amp;l:asset:length=200&amp;s:asset:publisher=foxnews&amp;s:asset:type=main&amp;s:asset:video_id=6318425658112&amp;s:stream:type=vod&amp;l:stream:startup_time=0&amp;l:stream:fps=0&amp;l:stream:bitrate=0&amp;l:stream:dropped_frames=0&amp;s:meta:a.media.asset=6318425658112&amp;s:meta:streamType=vod&amp;s:meta:length=200&amp;s:meta:app_id=Fox+News+amazon+tv+4.57.0+%282022121901%29&amp;s:meta:a.media.pass.mvpd=&amp;s:meta:s%3Aasset%3Aname=Biden+accused+of+mishandling+classified+documents&amp;s:meta:video_id=6318425658112&amp;s:meta:a.media.network=Fox+News.</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -715,7 +715,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>'s</t>
+          <t>parameter found with value start. URL: http://foxnews.hb.omtrdc.net/?s:sc:rsid=foxnewsglobalproduction&amp;s:sc:tracking_server=smetrics.foxnews.com&amp;h:sc:ssl=1&amp;&amp;&amp;&amp;s:sp:ovp=Akamai&amp;s:sp:channel=Fox+News&amp;s:sp:player_name=Fox+News+Android+Player&amp;s:sp:hb_version=android-2.1.0.154-42fb90&amp;l:sp:hb_api_lvl=4&amp;s:event:sid=1673312989776217636246&amp;l:event:duration=0&amp;l:event:playhead=0&amp;l:event:prev_ts=-1&amp;s:event:type=start&amp;l:event:ts=1673312989797&amp;s:asset:name=Biden+accused+of+mishandling+classified+documents&amp;l:asset:length=200&amp;s:asset:publisher=foxnews&amp;s:asset:type=main&amp;s:asset:video_id=6318425658112&amp;s:stream:type=vod&amp;l:stream:startup_time=0&amp;l:stream:fps=0&amp;l:stream:bitrate=0&amp;l:stream:dropped_frames=0&amp;s:meta:a.media.asset=6318425658112&amp;s:meta:streamType=vod&amp;s:meta:length=200&amp;s:meta:app_id=Fox+News+amazon+tv+4.57.0+%282022121901%29&amp;s:meta:a.media.pass.mvpd=&amp;s:meta:s%3Aasset%3Aname=Biden+accused+of+mishandling+classified+documents&amp;s:meta:video_id=6318425658112&amp;s:meta:a.media.network=Fox+News.</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -725,7 +725,7 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Pass: 's:event:sid' parameter found. URL: http://foxnews.hb.omtrdc.net/?s:sc:rsid=foxnewsglobalproduction&amp;s:sc:tracking_server=smetrics.foxnews.com&amp;h:sc:ssl=1&amp;&amp;&amp;&amp;s:sp:ovp=Akamai&amp;s:sp:channel=Fox+News&amp;s:sp:player_name=Fox+News+Android+Player&amp;s:sp:hb_version=android-2.1.0.154-42fb90&amp;l:sp:hb_api_lvl=4&amp;s:event:sid=1673312989776217636246&amp;l:event:duration=0&amp;l:event:playhead=0&amp;l:event:prev_ts=-1&amp;s:event:type=start&amp;l:event:ts=1673312989797&amp;s:asset:name=Biden+accused+of+mishandling+classified+documents&amp;l:asset:length=200&amp;s:asset:publisher=foxnews&amp;s:asset:type=main&amp;s:asset:video_id=6318425658112&amp;s:stream:type=vod&amp;l:stream:startup_time=0&amp;l:stream:fps=0&amp;l:stream:bitrate=0&amp;l:stream:dropped_frames=0&amp;s:meta:a.media.asset=6318425658112&amp;s:meta:streamType=vod&amp;s:meta:length=200&amp;s:meta:app_id=Fox+News+amazon+tv+4.57.0+%282022121901%29&amp;s:meta:a.media.pass.mvpd=&amp;s:meta:s%3Aasset%3Aname=Biden+accused+of+mishandling+classified+documents&amp;s:meta:video_id=6318425658112&amp;s:meta:a.media.network=Fox+News.</t>
+          <t>Pass: 's:event:type' parameter found with value start. URL: http://foxnews.hb.omtrdc.net/?s:sc:rsid=foxnewsglobalproduction&amp;s:sc:tracking_server=smetrics.foxnews.com&amp;h:sc:ssl=1&amp;&amp;&amp;&amp;s:sp:ovp=Akamai&amp;s:sp:channel=Fox+News&amp;s:sp:player_name=Fox+News+Android+Player&amp;s:sp:hb_version=android-2.1.0.154-42fb90&amp;l:sp:hb_api_lvl=4&amp;s:event:sid=1673312989776217636246&amp;l:event:duration=0&amp;l:event:playhead=0&amp;l:event:prev_ts=-1&amp;s:event:type=start&amp;l:event:ts=1673312989797&amp;s:asset:name=Biden+accused+of+mishandling+classified+documents&amp;l:asset:length=200&amp;s:asset:publisher=foxnews&amp;s:asset:type=main&amp;s:asset:video_id=6318425658112&amp;s:stream:type=vod&amp;l:stream:startup_time=0&amp;l:stream:fps=0&amp;l:stream:bitrate=0&amp;l:stream:dropped_frames=0&amp;s:meta:a.media.asset=6318425658112&amp;s:meta:streamType=vod&amp;s:meta:length=200&amp;s:meta:app_id=Fox+News+amazon+tv+4.57.0+%282022121901%29&amp;s:meta:a.media.pass.mvpd=&amp;s:meta:s%3Aasset%3Aname=Biden+accused+of+mishandling+classified+documents&amp;s:meta:video_id=6318425658112&amp;s:meta:a.media.network=Fox+News.</t>
         </is>
       </c>
     </row>
@@ -737,7 +737,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>'l</t>
+          <t>parameter found. URL: http://foxnews.hb.omtrdc.net/?s:sc:rsid=foxnewsglobalproduction&amp;s:sc:tracking_server=smetrics.foxnews.com&amp;h:sc:ssl=1&amp;&amp;&amp;&amp;s:sp:ovp=Akamai&amp;s:sp:channel=Fox+News&amp;s:sp:player_name=Fox+News+Android+Player&amp;s:sp:hb_version=android-2.1.0.154-42fb90&amp;l:sp:hb_api_lvl=4&amp;s:event:sid=1673312989776217636246&amp;l:event:duration=0&amp;l:event:playhead=0&amp;l:event:prev_ts=-1&amp;s:event:type=start&amp;l:event:ts=1673312989797&amp;s:asset:name=Biden+accused+of+mishandling+classified+documents&amp;l:asset:length=200&amp;s:asset:publisher=foxnews&amp;s:asset:type=main&amp;s:asset:video_id=6318425658112&amp;s:stream:type=vod&amp;l:stream:startup_time=0&amp;l:stream:fps=0&amp;l:stream:bitrate=0&amp;l:stream:dropped_frames=0&amp;s:meta:a.media.asset=6318425658112&amp;s:meta:streamType=vod&amp;s:meta:length=200&amp;s:meta:app_id=Fox+News+amazon+tv+4.57.0+%282022121901%29&amp;s:meta:a.media.pass.mvpd=&amp;s:meta:s%3Aasset%3Aname=Biden+accused+of+mishandling+classified+documents&amp;s:meta:video_id=6318425658112&amp;s:meta:a.media.network=Fox+News.</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -747,7 +747,7 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>Pass: 'l:event:duration' parameter found.</t>
+          <t>Pass: 's:event:sid' parameter found. URL: http://foxnews.hb.omtrdc.net/?s:sc:rsid=foxnewsglobalproduction&amp;s:sc:tracking_server=smetrics.foxnews.com&amp;h:sc:ssl=1&amp;&amp;&amp;&amp;s:sp:ovp=Akamai&amp;s:sp:channel=Fox+News&amp;s:sp:player_name=Fox+News+Android+Player&amp;s:sp:hb_version=android-2.1.0.154-42fb90&amp;l:sp:hb_api_lvl=4&amp;s:event:sid=1673312989776217636246&amp;l:event:duration=0&amp;l:event:playhead=0&amp;l:event:prev_ts=-1&amp;s:event:type=start&amp;l:event:ts=1673312989797&amp;s:asset:name=Biden+accused+of+mishandling+classified+documents&amp;l:asset:length=200&amp;s:asset:publisher=foxnews&amp;s:asset:type=main&amp;s:asset:video_id=6318425658112&amp;s:stream:type=vod&amp;l:stream:startup_time=0&amp;l:stream:fps=0&amp;l:stream:bitrate=0&amp;l:stream:dropped_frames=0&amp;s:meta:a.media.asset=6318425658112&amp;s:meta:streamType=vod&amp;s:meta:length=200&amp;s:meta:app_id=Fox+News+amazon+tv+4.57.0+%282022121901%29&amp;s:meta:a.media.pass.mvpd=&amp;s:meta:s%3Aasset%3Aname=Biden+accused+of+mishandling+classified+documents&amp;s:meta:video_id=6318425658112&amp;s:meta:a.media.network=Fox+News.</t>
         </is>
       </c>
     </row>
@@ -759,7 +759,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>'l</t>
+          <t>parameter found.</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -769,7 +769,7 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>Pass: 'l:event:playhead' parameter found.</t>
+          <t>Pass: 'l:event:duration' parameter found.</t>
         </is>
       </c>
     </row>
@@ -781,7 +781,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>'l</t>
+          <t>parameter found.</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
@@ -803,7 +803,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>'l</t>
+          <t>parameter found.</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
@@ -825,7 +825,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>'s</t>
+          <t>parameter found.</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
@@ -847,7 +847,7 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>'l</t>
+          <t>parameter found.</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
@@ -869,7 +869,7 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>'s</t>
+          <t>parameter found.</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
@@ -891,7 +891,7 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>'s</t>
+          <t>parameter found.</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
@@ -913,7 +913,7 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>'s</t>
+          <t>parameter found with value foxnewsglobalproduction. URL: http://foxnews.hb.omtrdc.net/?s:sc:rsid=foxnewsglobalproduction&amp;s:sc:tracking_server=smetrics.foxnews.com&amp;h:sc:ssl=1&amp;&amp;&amp;&amp;s:sp:ovp=Akamai&amp;s:sp:channel=Fox+News&amp;s:sp:player_name=Fox+News+Android+Player&amp;s:sp:hb_version=android-2.1.0.154-42fb90&amp;l:sp:hb_api_lvl=4&amp;s:event:sid=1673312989776217636246&amp;l:event:duration=0&amp;l:event:playhead=0&amp;l:event:prev_ts=-1&amp;s:event:type=start&amp;l:event:ts=1673312989797&amp;s:asset:name=Biden+accused+of+mishandling+classified+documents&amp;l:asset:length=200&amp;s:asset:publisher=foxnews&amp;s:asset:type=main&amp;s:asset:video_id=6318425658112&amp;s:stream:type=vod&amp;l:stream:startup_time=0&amp;l:stream:fps=0&amp;l:stream:bitrate=0&amp;l:stream:dropped_frames=0&amp;s:meta:a.media.asset=6318425658112&amp;s:meta:streamType=vod&amp;s:meta:length=200&amp;s:meta:app_id=Fox+News+amazon+tv+4.57.0+%282022121901%29&amp;s:meta:a.media.pass.mvpd=&amp;s:meta:s%3Aasset%3Aname=Biden+accused+of+mishandling+classified+documents&amp;s:meta:video_id=6318425658112&amp;s:meta:a.media.network=Fox+News.</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
@@ -935,7 +935,7 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>'s</t>
+          <t>parameter found with value start. URL: http://foxnews.hb.omtrdc.net/?s:sc:rsid=foxnewsglobalproduction&amp;s:sc:tracking_server=smetrics.foxnews.com&amp;h:sc:ssl=1&amp;&amp;&amp;&amp;s:sp:ovp=Akamai&amp;s:sp:channel=Fox+News&amp;s:sp:player_name=Fox+News+Android+Player&amp;s:sp:hb_version=android-2.1.0.154-42fb90&amp;l:sp:hb_api_lvl=4&amp;s:event:sid=1673312989776217636246&amp;l:event:duration=45&amp;l:event:playhead=0&amp;l:event:prev_ts=1673312989797&amp;s:event:type=start&amp;l:event:ts=1673312989842&amp;s:asset:name=Biden+accused+of+mishandling+classified+documents&amp;l:asset:length=200&amp;s:asset:publisher=foxnews&amp;s:asset:type=main&amp;s:asset:video_id=6318425658112&amp;s:stream:type=vod&amp;l:stream:startup_time=0&amp;l:stream:fps=0&amp;l:stream:bitrate=0&amp;l:stream:dropped_frames=0&amp;s:meta:a.media.asset=6318425658112&amp;s:meta:streamType=vod&amp;s:meta:length=200&amp;s:meta:app_id=Fox+News+amazon+tv+4.57.0+%282022121901%29&amp;s:meta:a.media.pass.mvpd=&amp;s:meta:s%3Aasset%3Aname=Biden+accused+of+mishandling+classified+documents&amp;s:meta:video_id=6318425658112&amp;s:meta:a.media.network=Fox+News.</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
@@ -957,7 +957,7 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>'s</t>
+          <t>parameter found with value start. URL: http://foxnews.hb.omtrdc.net/?s:sc:rsid=foxnewsglobalproduction&amp;s:sc:tracking_server=smetrics.foxnews.com&amp;h:sc:ssl=1&amp;&amp;&amp;&amp;s:sp:ovp=Akamai&amp;s:sp:channel=Fox+News&amp;s:sp:player_name=Fox+News+Android+Player&amp;s:sp:hb_version=android-2.1.0.154-42fb90&amp;l:sp:hb_api_lvl=4&amp;s:event:sid=1673312989776217636246&amp;l:event:duration=45&amp;l:event:playhead=0&amp;l:event:prev_ts=1673312989797&amp;s:event:type=start&amp;l:event:ts=1673312989842&amp;s:asset:name=Biden+accused+of+mishandling+classified+documents&amp;l:asset:length=200&amp;s:asset:publisher=foxnews&amp;s:asset:type=main&amp;s:asset:video_id=6318425658112&amp;s:stream:type=vod&amp;l:stream:startup_time=0&amp;l:stream:fps=0&amp;l:stream:bitrate=0&amp;l:stream:dropped_frames=0&amp;s:meta:a.media.asset=6318425658112&amp;s:meta:streamType=vod&amp;s:meta:length=200&amp;s:meta:app_id=Fox+News+amazon+tv+4.57.0+%282022121901%29&amp;s:meta:a.media.pass.mvpd=&amp;s:meta:s%3Aasset%3Aname=Biden+accused+of+mishandling+classified+documents&amp;s:meta:video_id=6318425658112&amp;s:meta:a.media.network=Fox+News.</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
@@ -967,7 +967,7 @@
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>Pass: 's:event:sid' parameter found. URL: http://foxnews.hb.omtrdc.net/?s:sc:rsid=foxnewsglobalproduction&amp;s:sc:tracking_server=smetrics.foxnews.com&amp;h:sc:ssl=1&amp;&amp;&amp;&amp;s:sp:ovp=Akamai&amp;s:sp:channel=Fox+News&amp;s:sp:player_name=Fox+News+Android+Player&amp;s:sp:hb_version=android-2.1.0.154-42fb90&amp;l:sp:hb_api_lvl=4&amp;s:event:sid=1673312989776217636246&amp;l:event:duration=45&amp;l:event:playhead=0&amp;l:event:prev_ts=1673312989797&amp;s:event:type=start&amp;l:event:ts=1673312989842&amp;s:asset:name=Biden+accused+of+mishandling+classified+documents&amp;l:asset:length=200&amp;s:asset:publisher=foxnews&amp;s:asset:type=main&amp;s:asset:video_id=6318425658112&amp;s:stream:type=vod&amp;l:stream:startup_time=0&amp;l:stream:fps=0&amp;l:stream:bitrate=0&amp;l:stream:dropped_frames=0&amp;s:meta:a.media.asset=6318425658112&amp;s:meta:streamType=vod&amp;s:meta:length=200&amp;s:meta:app_id=Fox+News+amazon+tv+4.57.0+%282022121901%29&amp;s:meta:a.media.pass.mvpd=&amp;s:meta:s%3Aasset%3Aname=Biden+accused+of+mishandling+classified+documents&amp;s:meta:video_id=6318425658112&amp;s:meta:a.media.network=Fox+News.</t>
+          <t>Pass: 's:event:type' parameter found with value start. URL: http://foxnews.hb.omtrdc.net/?s:sc:rsid=foxnewsglobalproduction&amp;s:sc:tracking_server=smetrics.foxnews.com&amp;h:sc:ssl=1&amp;&amp;&amp;&amp;s:sp:ovp=Akamai&amp;s:sp:channel=Fox+News&amp;s:sp:player_name=Fox+News+Android+Player&amp;s:sp:hb_version=android-2.1.0.154-42fb90&amp;l:sp:hb_api_lvl=4&amp;s:event:sid=1673312989776217636246&amp;l:event:duration=45&amp;l:event:playhead=0&amp;l:event:prev_ts=1673312989797&amp;s:event:type=start&amp;l:event:ts=1673312989842&amp;s:asset:name=Biden+accused+of+mishandling+classified+documents&amp;l:asset:length=200&amp;s:asset:publisher=foxnews&amp;s:asset:type=main&amp;s:asset:video_id=6318425658112&amp;s:stream:type=vod&amp;l:stream:startup_time=0&amp;l:stream:fps=0&amp;l:stream:bitrate=0&amp;l:stream:dropped_frames=0&amp;s:meta:a.media.asset=6318425658112&amp;s:meta:streamType=vod&amp;s:meta:length=200&amp;s:meta:app_id=Fox+News+amazon+tv+4.57.0+%282022121901%29&amp;s:meta:a.media.pass.mvpd=&amp;s:meta:s%3Aasset%3Aname=Biden+accused+of+mishandling+classified+documents&amp;s:meta:video_id=6318425658112&amp;s:meta:a.media.network=Fox+News.</t>
         </is>
       </c>
     </row>
@@ -979,7 +979,7 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>'l</t>
+          <t>parameter found. URL: http://foxnews.hb.omtrdc.net/?s:sc:rsid=foxnewsglobalproduction&amp;s:sc:tracking_server=smetrics.foxnews.com&amp;h:sc:ssl=1&amp;&amp;&amp;&amp;s:sp:ovp=Akamai&amp;s:sp:channel=Fox+News&amp;s:sp:player_name=Fox+News+Android+Player&amp;s:sp:hb_version=android-2.1.0.154-42fb90&amp;l:sp:hb_api_lvl=4&amp;s:event:sid=1673312989776217636246&amp;l:event:duration=45&amp;l:event:playhead=0&amp;l:event:prev_ts=1673312989797&amp;s:event:type=start&amp;l:event:ts=1673312989842&amp;s:asset:name=Biden+accused+of+mishandling+classified+documents&amp;l:asset:length=200&amp;s:asset:publisher=foxnews&amp;s:asset:type=main&amp;s:asset:video_id=6318425658112&amp;s:stream:type=vod&amp;l:stream:startup_time=0&amp;l:stream:fps=0&amp;l:stream:bitrate=0&amp;l:stream:dropped_frames=0&amp;s:meta:a.media.asset=6318425658112&amp;s:meta:streamType=vod&amp;s:meta:length=200&amp;s:meta:app_id=Fox+News+amazon+tv+4.57.0+%282022121901%29&amp;s:meta:a.media.pass.mvpd=&amp;s:meta:s%3Aasset%3Aname=Biden+accused+of+mishandling+classified+documents&amp;s:meta:video_id=6318425658112&amp;s:meta:a.media.network=Fox+News.</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
@@ -989,7 +989,7 @@
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>Pass: 'l:event:duration' parameter found.</t>
+          <t>Pass: 's:event:sid' parameter found. URL: http://foxnews.hb.omtrdc.net/?s:sc:rsid=foxnewsglobalproduction&amp;s:sc:tracking_server=smetrics.foxnews.com&amp;h:sc:ssl=1&amp;&amp;&amp;&amp;s:sp:ovp=Akamai&amp;s:sp:channel=Fox+News&amp;s:sp:player_name=Fox+News+Android+Player&amp;s:sp:hb_version=android-2.1.0.154-42fb90&amp;l:sp:hb_api_lvl=4&amp;s:event:sid=1673312989776217636246&amp;l:event:duration=45&amp;l:event:playhead=0&amp;l:event:prev_ts=1673312989797&amp;s:event:type=start&amp;l:event:ts=1673312989842&amp;s:asset:name=Biden+accused+of+mishandling+classified+documents&amp;l:asset:length=200&amp;s:asset:publisher=foxnews&amp;s:asset:type=main&amp;s:asset:video_id=6318425658112&amp;s:stream:type=vod&amp;l:stream:startup_time=0&amp;l:stream:fps=0&amp;l:stream:bitrate=0&amp;l:stream:dropped_frames=0&amp;s:meta:a.media.asset=6318425658112&amp;s:meta:streamType=vod&amp;s:meta:length=200&amp;s:meta:app_id=Fox+News+amazon+tv+4.57.0+%282022121901%29&amp;s:meta:a.media.pass.mvpd=&amp;s:meta:s%3Aasset%3Aname=Biden+accused+of+mishandling+classified+documents&amp;s:meta:video_id=6318425658112&amp;s:meta:a.media.network=Fox+News.</t>
         </is>
       </c>
     </row>
@@ -1001,7 +1001,7 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>'l</t>
+          <t>parameter found.</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
@@ -1011,7 +1011,7 @@
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>Pass: 'l:event:playhead' parameter found.</t>
+          <t>Pass: 'l:event:duration' parameter found.</t>
         </is>
       </c>
     </row>
@@ -1023,7 +1023,7 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>'l</t>
+          <t>parameter found.</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
@@ -1045,7 +1045,7 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>'l</t>
+          <t>parameter found.</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
@@ -1067,7 +1067,7 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>'s</t>
+          <t>parameter found.</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
@@ -1089,7 +1089,7 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>'l</t>
+          <t>parameter found.</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
@@ -1111,7 +1111,7 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>'s</t>
+          <t>parameter found.</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
@@ -1133,7 +1133,7 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>'s</t>
+          <t>parameter found.</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
@@ -1155,7 +1155,7 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>'s</t>
+          <t>parameter found with value foxnewsglobalproduction. URL: http://foxnews.hb.omtrdc.net/?s:sc:rsid=foxnewsglobalproduction&amp;s:sc:tracking_server=smetrics.foxnews.com&amp;h:sc:ssl=1&amp;&amp;&amp;&amp;s:sp:ovp=Akamai&amp;s:sp:channel=Fox+News&amp;s:sp:player_name=Fox+News+Android+Player&amp;s:sp:hb_version=android-2.1.0.154-42fb90&amp;l:sp:hb_api_lvl=4&amp;s:event:sid=1673312989776217636246&amp;l:event:duration=45&amp;l:event:playhead=0&amp;l:event:prev_ts=1673312989797&amp;s:event:type=start&amp;l:event:ts=1673312989842&amp;s:asset:name=Biden+accused+of+mishandling+classified+documents&amp;l:asset:length=200&amp;s:asset:publisher=foxnews&amp;s:asset:type=main&amp;s:asset:video_id=6318425658112&amp;s:stream:type=vod&amp;l:stream:startup_time=0&amp;l:stream:fps=0&amp;l:stream:bitrate=0&amp;l:stream:dropped_frames=0&amp;s:meta:a.media.asset=6318425658112&amp;s:meta:streamType=vod&amp;s:meta:length=200&amp;s:meta:app_id=Fox+News+amazon+tv+4.57.0+%282022121901%29&amp;s:meta:a.media.pass.mvpd=&amp;s:meta:s%3Aasset%3Aname=Biden+accused+of+mishandling+classified+documents&amp;s:meta:video_id=6318425658112&amp;s:meta:a.media.network=Fox+News.</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
@@ -1177,7 +1177,7 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>'s</t>
+          <t>parameter found with value buffer. URL: http://foxnews.hb.omtrdc.net/?s:sc:rsid=foxnewsglobalproduction&amp;s:sc:tracking_server=smetrics.foxnews.com&amp;h:sc:ssl=1&amp;&amp;&amp;&amp;s:sp:ovp=Akamai&amp;s:sp:channel=Fox+News&amp;s:sp:player_name=Fox+News+Android+Player&amp;s:sp:hb_version=android-2.1.0.154-42fb90&amp;l:sp:hb_api_lvl=4&amp;s:event:sid=1673312989776217636246&amp;l:event:duration=0&amp;l:event:playhead=0&amp;l:event:prev_ts=-1&amp;s:event:type=buffer&amp;l:event:ts=1673312989842&amp;s:asset:name=Biden+accused+of+mishandling+classified+documents&amp;l:asset:length=200&amp;s:asset:publisher=foxnews&amp;s:asset:type=main&amp;s:asset:video_id=6318425658112&amp;s:stream:type=vod&amp;l:stream:startup_time=0&amp;l:stream:fps=0&amp;l:stream:bitrate=0&amp;l:stream:dropped_frames=0.</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
@@ -1199,7 +1199,7 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>'s</t>
+          <t>parameter found with value buffer. URL: http://foxnews.hb.omtrdc.net/?s:sc:rsid=foxnewsglobalproduction&amp;s:sc:tracking_server=smetrics.foxnews.com&amp;h:sc:ssl=1&amp;&amp;&amp;&amp;s:sp:ovp=Akamai&amp;s:sp:channel=Fox+News&amp;s:sp:player_name=Fox+News+Android+Player&amp;s:sp:hb_version=android-2.1.0.154-42fb90&amp;l:sp:hb_api_lvl=4&amp;s:event:sid=1673312989776217636246&amp;l:event:duration=0&amp;l:event:playhead=0&amp;l:event:prev_ts=-1&amp;s:event:type=buffer&amp;l:event:ts=1673312989842&amp;s:asset:name=Biden+accused+of+mishandling+classified+documents&amp;l:asset:length=200&amp;s:asset:publisher=foxnews&amp;s:asset:type=main&amp;s:asset:video_id=6318425658112&amp;s:stream:type=vod&amp;l:stream:startup_time=0&amp;l:stream:fps=0&amp;l:stream:bitrate=0&amp;l:stream:dropped_frames=0.</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
@@ -1209,7 +1209,7 @@
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>Pass: 's:event:sid' parameter found. URL: http://foxnews.hb.omtrdc.net/?s:sc:rsid=foxnewsglobalproduction&amp;s:sc:tracking_server=smetrics.foxnews.com&amp;h:sc:ssl=1&amp;&amp;&amp;&amp;s:sp:ovp=Akamai&amp;s:sp:channel=Fox+News&amp;s:sp:player_name=Fox+News+Android+Player&amp;s:sp:hb_version=android-2.1.0.154-42fb90&amp;l:sp:hb_api_lvl=4&amp;s:event:sid=1673312989776217636246&amp;l:event:duration=0&amp;l:event:playhead=0&amp;l:event:prev_ts=-1&amp;s:event:type=buffer&amp;l:event:ts=1673312989842&amp;s:asset:name=Biden+accused+of+mishandling+classified+documents&amp;l:asset:length=200&amp;s:asset:publisher=foxnews&amp;s:asset:type=main&amp;s:asset:video_id=6318425658112&amp;s:stream:type=vod&amp;l:stream:startup_time=0&amp;l:stream:fps=0&amp;l:stream:bitrate=0&amp;l:stream:dropped_frames=0.</t>
+          <t>Pass: 's:event:type' parameter found with value buffer. URL: http://foxnews.hb.omtrdc.net/?s:sc:rsid=foxnewsglobalproduction&amp;s:sc:tracking_server=smetrics.foxnews.com&amp;h:sc:ssl=1&amp;&amp;&amp;&amp;s:sp:ovp=Akamai&amp;s:sp:channel=Fox+News&amp;s:sp:player_name=Fox+News+Android+Player&amp;s:sp:hb_version=android-2.1.0.154-42fb90&amp;l:sp:hb_api_lvl=4&amp;s:event:sid=1673312989776217636246&amp;l:event:duration=0&amp;l:event:playhead=0&amp;l:event:prev_ts=-1&amp;s:event:type=buffer&amp;l:event:ts=1673312989842&amp;s:asset:name=Biden+accused+of+mishandling+classified+documents&amp;l:asset:length=200&amp;s:asset:publisher=foxnews&amp;s:asset:type=main&amp;s:asset:video_id=6318425658112&amp;s:stream:type=vod&amp;l:stream:startup_time=0&amp;l:stream:fps=0&amp;l:stream:bitrate=0&amp;l:stream:dropped_frames=0.</t>
         </is>
       </c>
     </row>
@@ -1221,7 +1221,7 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>'l</t>
+          <t>parameter found. URL: http://foxnews.hb.omtrdc.net/?s:sc:rsid=foxnewsglobalproduction&amp;s:sc:tracking_server=smetrics.foxnews.com&amp;h:sc:ssl=1&amp;&amp;&amp;&amp;s:sp:ovp=Akamai&amp;s:sp:channel=Fox+News&amp;s:sp:player_name=Fox+News+Android+Player&amp;s:sp:hb_version=android-2.1.0.154-42fb90&amp;l:sp:hb_api_lvl=4&amp;s:event:sid=1673312989776217636246&amp;l:event:duration=0&amp;l:event:playhead=0&amp;l:event:prev_ts=-1&amp;s:event:type=buffer&amp;l:event:ts=1673312989842&amp;s:asset:name=Biden+accused+of+mishandling+classified+documents&amp;l:asset:length=200&amp;s:asset:publisher=foxnews&amp;s:asset:type=main&amp;s:asset:video_id=6318425658112&amp;s:stream:type=vod&amp;l:stream:startup_time=0&amp;l:stream:fps=0&amp;l:stream:bitrate=0&amp;l:stream:dropped_frames=0.</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
@@ -1231,7 +1231,7 @@
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>Pass: 'l:event:duration' parameter found.</t>
+          <t>Pass: 's:event:sid' parameter found. URL: http://foxnews.hb.omtrdc.net/?s:sc:rsid=foxnewsglobalproduction&amp;s:sc:tracking_server=smetrics.foxnews.com&amp;h:sc:ssl=1&amp;&amp;&amp;&amp;s:sp:ovp=Akamai&amp;s:sp:channel=Fox+News&amp;s:sp:player_name=Fox+News+Android+Player&amp;s:sp:hb_version=android-2.1.0.154-42fb90&amp;l:sp:hb_api_lvl=4&amp;s:event:sid=1673312989776217636246&amp;l:event:duration=0&amp;l:event:playhead=0&amp;l:event:prev_ts=-1&amp;s:event:type=buffer&amp;l:event:ts=1673312989842&amp;s:asset:name=Biden+accused+of+mishandling+classified+documents&amp;l:asset:length=200&amp;s:asset:publisher=foxnews&amp;s:asset:type=main&amp;s:asset:video_id=6318425658112&amp;s:stream:type=vod&amp;l:stream:startup_time=0&amp;l:stream:fps=0&amp;l:stream:bitrate=0&amp;l:stream:dropped_frames=0.</t>
         </is>
       </c>
     </row>
@@ -1243,7 +1243,7 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>'l</t>
+          <t>parameter found.</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
@@ -1253,7 +1253,7 @@
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>Pass: 'l:event:playhead' parameter found.</t>
+          <t>Pass: 'l:event:duration' parameter found.</t>
         </is>
       </c>
     </row>
@@ -1265,7 +1265,7 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>'l</t>
+          <t>parameter found.</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
@@ -1287,7 +1287,7 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>'l</t>
+          <t>parameter found.</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
@@ -1309,7 +1309,7 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>'s</t>
+          <t>parameter found.</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
@@ -1331,7 +1331,7 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>'l</t>
+          <t>parameter found.</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
@@ -1353,7 +1353,7 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>'s</t>
+          <t>parameter found.</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
@@ -1375,7 +1375,7 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>'s</t>
+          <t>parameter found.</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
@@ -1397,7 +1397,7 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>'s</t>
+          <t>parameter found with value foxnewsglobalproduction. URL: http://foxnews.hb.omtrdc.net/?s:sc:rsid=foxnewsglobalproduction&amp;s:sc:tracking_server=smetrics.foxnews.com&amp;h:sc:ssl=1&amp;&amp;&amp;&amp;s:sp:ovp=Akamai&amp;s:sp:channel=Fox+News&amp;s:sp:player_name=Fox+News+Android+Player&amp;s:sp:hb_version=android-2.1.0.154-42fb90&amp;l:sp:hb_api_lvl=4&amp;s:event:sid=1673312989776217636246&amp;l:event:duration=0&amp;l:event:playhead=0&amp;l:event:prev_ts=-1&amp;s:event:type=buffer&amp;l:event:ts=1673312989842&amp;s:asset:name=Biden+accused+of+mishandling+classified+documents&amp;l:asset:length=200&amp;s:asset:publisher=foxnews&amp;s:asset:type=main&amp;s:asset:video_id=6318425658112&amp;s:stream:type=vod&amp;l:stream:startup_time=0&amp;l:stream:fps=0&amp;l:stream:bitrate=0&amp;l:stream:dropped_frames=0.</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
@@ -1419,7 +1419,7 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>'app_build' parameter missing. URL</t>
+          <t>parameter missing. URL: https://smetrics.foxnews.com/id?mid=69099319612994832056547930341105758682&amp;mcorgid=foxnews. Please add the</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
@@ -1441,7 +1441,7 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>'app_name' parameter missing. URL</t>
+          <t>parameter missing. URL: https://smetrics.foxnews.com/id?mid=69099319612994832056547930341105758682&amp;mcorgid=foxnews. Please add the</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
@@ -1463,7 +1463,7 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>'app_version' parameter missing. URL</t>
+          <t>parameter missing. URL: https://smetrics.foxnews.com/id?mid=69099319612994832056547930341105758682&amp;mcorgid=foxnews. Please add the</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
@@ -1485,7 +1485,7 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>'s</t>
+          <t>parameter missing. URL: https://smetrics.foxnews.com/id?mid=69099319612994832056547930341105758682&amp;mcorgid=foxnews. Please add the</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
@@ -1507,7 +1507,7 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>'s</t>
+          <t>parameter missing. URL: https://smetrics.foxnews.com/id?mid=69099319612994832056547930341105758682&amp;mcorgid=foxnews. Please add the</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
@@ -1517,7 +1517,7 @@
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>Fail: 's:event:sid' parameter missing. URL: https://smetrics.foxnews.com/id?mid=69099319612994832056547930341105758682&amp;mcorgid=foxnews. Please add this parameter.</t>
+          <t>Fail: 's:event:type' parameter missing. URL: https://smetrics.foxnews.com/id?mid=69099319612994832056547930341105758682&amp;mcorgid=foxnews. Please add the 's:event:type' parameter.</t>
         </is>
       </c>
     </row>
@@ -1529,7 +1529,7 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>'l</t>
+          <t>parameter missing. URL: https://smetrics.foxnews.com/id?mid=69099319612994832056547930341105758682&amp;mcorgid=foxnews. Please add this parameter.</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
@@ -1539,7 +1539,7 @@
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>Fail: 'l:event:duration' parameter missing. Please add this parameter.</t>
+          <t>Fail: 's:event:sid' parameter missing. URL: https://smetrics.foxnews.com/id?mid=69099319612994832056547930341105758682&amp;mcorgid=foxnews. Please add this parameter.</t>
         </is>
       </c>
     </row>
@@ -1551,7 +1551,7 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>'l</t>
+          <t>parameter missing. Please add this parameter.</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
@@ -1561,7 +1561,7 @@
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>Fail: 'l:event:playhead' parameter missing. Please add this parameter.</t>
+          <t>Fail: 'l:event:duration' parameter missing. Please add this parameter.</t>
         </is>
       </c>
     </row>
@@ -1573,7 +1573,7 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>'l</t>
+          <t>parameter missing. Please add this parameter.</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
@@ -1583,7 +1583,7 @@
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>Fail: 'l:event:prev_ts' parameter missing. Please add this parameter.</t>
+          <t>Fail: 'l:event:playhead' parameter missing. Please add this parameter.</t>
         </is>
       </c>
     </row>
@@ -1595,7 +1595,7 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>'l</t>
+          <t>parameter missing. Please add this parameter.</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
@@ -1605,7 +1605,7 @@
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>Fail: 'l:event:ts' parameter missing. Please add this parameter.</t>
+          <t>Fail: 'l:event:prev_ts' parameter missing. Please add this parameter.</t>
         </is>
       </c>
     </row>
@@ -1617,7 +1617,7 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>'s</t>
+          <t>parameter missing. Please add this parameter.</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
@@ -1627,7 +1627,7 @@
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>Fail: 's:asset:name' parameter missing. Please add this parameter.</t>
+          <t>Fail: 'l:event:ts' parameter missing. Please add this parameter.</t>
         </is>
       </c>
     </row>
@@ -1639,7 +1639,7 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>'l</t>
+          <t>parameter missing. Please add this parameter.</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
@@ -1649,7 +1649,7 @@
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>Fail: 'l:asset:length' parameter missing. Please add this parameter.</t>
+          <t>Fail: 's:asset:name' parameter missing. Please add this parameter.</t>
         </is>
       </c>
     </row>
@@ -1661,7 +1661,7 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>'s</t>
+          <t>parameter missing. Please add this parameter.</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
@@ -1671,7 +1671,7 @@
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>Fail: 's:asset:publisher' parameter missing. Please add this parameter.</t>
+          <t>Fail: 'l:asset:length' parameter missing. Please add this parameter.</t>
         </is>
       </c>
     </row>
@@ -1683,7 +1683,7 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>'s</t>
+          <t>parameter missing. Please add this parameter.</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
@@ -1693,7 +1693,7 @@
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>Fail: 's:asset:type' parameter missing. Please add this parameter.</t>
+          <t>Fail: 's:asset:publisher' parameter missing. Please add this parameter.</t>
         </is>
       </c>
     </row>
@@ -1705,17 +1705,17 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>One of 'mid' variations found with value 69099319612994832056547930341105758682. URL</t>
+          <t>parameter missing. Please add this parameter.</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>Pass</t>
+          <t>Fail</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>Pass: One of 'mid' variations found with value 69099319612994832056547930341105758682. URL: https://smetrics.foxnews.com/id?mid=69099319612994832056547930341105758682&amp;mcorgid=foxnews.</t>
+          <t>Fail: 's:asset:type' parameter missing. Please add this parameter.</t>
         </is>
       </c>
     </row>
@@ -1727,17 +1727,17 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>'page_type' parameter missing. URL</t>
+          <t>variations found with value 69099319612994832056547930341105758682. URL: https://smetrics.foxnews.com/id?mid=69099319612994832056547930341105758682&amp;mcorgid=foxnews.</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>Fail</t>
+          <t>Pass</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>Fail: 'page_type' parameter missing. URL: https://smetrics.foxnews.com/id?mid=69099319612994832056547930341105758682&amp;mcorgid=foxnews. Please add the 'page_type' parameter.</t>
+          <t>Pass: One of 'mid' variations found with value 69099319612994832056547930341105758682. URL: https://smetrics.foxnews.com/id?mid=69099319612994832056547930341105758682&amp;mcorgid=foxnews.</t>
         </is>
       </c>
     </row>
@@ -1749,7 +1749,7 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>'primary_business_unit' parameter missing. URL</t>
+          <t>parameter missing. URL: https://smetrics.foxnews.com/id?mid=69099319612994832056547930341105758682&amp;mcorgid=foxnews. Please add the</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
@@ -1759,7 +1759,7 @@
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>Fail: 'primary_business_unit' parameter missing. URL: https://smetrics.foxnews.com/id?mid=69099319612994832056547930341105758682&amp;mcorgid=foxnews. Please add the 'primary_business_unit' parameter.</t>
+          <t>Fail: 'page_type' parameter missing. URL: https://smetrics.foxnews.com/id?mid=69099319612994832056547930341105758682&amp;mcorgid=foxnews. Please add the 'page_type' parameter.</t>
         </is>
       </c>
     </row>
@@ -1771,7 +1771,7 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>'user_fox_anonymous_profile_id' parameter missing. Please add the 'user_fox_anonymous_profile_id' parameter.</t>
+          <t>parameter missing. URL: https://smetrics.foxnews.com/id?mid=69099319612994832056547930341105758682&amp;mcorgid=foxnews. Please add the</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
@@ -1781,19 +1781,19 @@
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>Fail: 'user_fox_anonymous_profile_id' parameter missing. Please add the 'user_fox_anonymous_profile_id' parameter.</t>
+          <t>Fail: 'primary_business_unit' parameter missing. URL: https://smetrics.foxnews.com/id?mid=69099319612994832056547930341105758682&amp;mcorgid=foxnews. Please add the 'primary_business_unit' parameter.</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>https://smetrics.foxnews.com/b/ss/foxnewsglobalproduction/0/JAVA-4.17.9-AN/s40450848</t>
+          <t>https://smetrics.foxnews.com/id?mid=69099319612994832056547930341105758682&amp;mcorgid=foxnews</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>'app_build' parameter missing. URL</t>
+          <t>parameter missing. Please add the</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
@@ -1803,7 +1803,7 @@
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>Fail: 'app_build' parameter missing. URL: https://smetrics.foxnews.com/b/ss/foxnewsglobalproduction/0/JAVA-4.17.9-AN/s40450848. Please add the 'app_build' parameter.</t>
+          <t>Fail: 'user_fox_anonymous_profile_id' parameter missing. Please add the 'user_fox_anonymous_profile_id' parameter.</t>
         </is>
       </c>
     </row>
@@ -1815,7 +1815,7 @@
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>'app_name' parameter missing. URL</t>
+          <t>parameter missing. URL: https://smetrics.foxnews.com/b/ss/foxnewsglobalproduction/0/JAVA-4.17.9-AN/s40450848. Please add the</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
@@ -1825,7 +1825,7 @@
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>Fail: 'app_name' parameter missing. URL: https://smetrics.foxnews.com/b/ss/foxnewsglobalproduction/0/JAVA-4.17.9-AN/s40450848. Please add the 'app_name' parameter.</t>
+          <t>Fail: 'app_build' parameter missing. URL: https://smetrics.foxnews.com/b/ss/foxnewsglobalproduction/0/JAVA-4.17.9-AN/s40450848. Please add the 'app_build' parameter.</t>
         </is>
       </c>
     </row>
@@ -1837,7 +1837,7 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>'app_version' parameter missing. URL</t>
+          <t>parameter missing. URL: https://smetrics.foxnews.com/b/ss/foxnewsglobalproduction/0/JAVA-4.17.9-AN/s40450848. Please add the</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
@@ -1847,7 +1847,7 @@
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>Fail: 'app_version' parameter missing. URL: https://smetrics.foxnews.com/b/ss/foxnewsglobalproduction/0/JAVA-4.17.9-AN/s40450848. Please add the 'app_version' parameter.</t>
+          <t>Fail: 'app_name' parameter missing. URL: https://smetrics.foxnews.com/b/ss/foxnewsglobalproduction/0/JAVA-4.17.9-AN/s40450848. Please add the 'app_name' parameter.</t>
         </is>
       </c>
     </row>
@@ -1859,7 +1859,7 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>'s</t>
+          <t>parameter missing. URL: https://smetrics.foxnews.com/b/ss/foxnewsglobalproduction/0/JAVA-4.17.9-AN/s40450848. Please add the</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
@@ -1869,7 +1869,7 @@
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>Fail: 's:event:type' parameter missing. URL: https://smetrics.foxnews.com/b/ss/foxnewsglobalproduction/0/JAVA-4.17.9-AN/s40450848. Please add the 's:event:type' parameter.</t>
+          <t>Fail: 'app_version' parameter missing. URL: https://smetrics.foxnews.com/b/ss/foxnewsglobalproduction/0/JAVA-4.17.9-AN/s40450848. Please add the 'app_version' parameter.</t>
         </is>
       </c>
     </row>
@@ -1881,7 +1881,7 @@
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>'s</t>
+          <t>parameter missing. URL: https://smetrics.foxnews.com/b/ss/foxnewsglobalproduction/0/JAVA-4.17.9-AN/s40450848. Please add the</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
@@ -1891,7 +1891,7 @@
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>Fail: 's:event:sid' parameter missing. URL: https://smetrics.foxnews.com/b/ss/foxnewsglobalproduction/0/JAVA-4.17.9-AN/s40450848. Please add this parameter.</t>
+          <t>Fail: 's:event:type' parameter missing. URL: https://smetrics.foxnews.com/b/ss/foxnewsglobalproduction/0/JAVA-4.17.9-AN/s40450848. Please add the 's:event:type' parameter.</t>
         </is>
       </c>
     </row>
@@ -1903,7 +1903,7 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>'l</t>
+          <t>parameter missing. URL: https://smetrics.foxnews.com/b/ss/foxnewsglobalproduction/0/JAVA-4.17.9-AN/s40450848. Please add the</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
@@ -1913,7 +1913,7 @@
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>Fail: 'l:event:duration' parameter missing. Please add this parameter.</t>
+          <t>Fail: 's:event:type' parameter missing. URL: https://smetrics.foxnews.com/b/ss/foxnewsglobalproduction/0/JAVA-4.17.9-AN/s40450848. Please add the 's:event:type' parameter.</t>
         </is>
       </c>
     </row>
@@ -1925,7 +1925,7 @@
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>'l</t>
+          <t>parameter missing. URL: https://smetrics.foxnews.com/b/ss/foxnewsglobalproduction/0/JAVA-4.17.9-AN/s40450848. Please add this parameter.</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
@@ -1935,7 +1935,7 @@
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>Fail: 'l:event:playhead' parameter missing. Please add this parameter.</t>
+          <t>Fail: 's:event:sid' parameter missing. URL: https://smetrics.foxnews.com/b/ss/foxnewsglobalproduction/0/JAVA-4.17.9-AN/s40450848. Please add this parameter.</t>
         </is>
       </c>
     </row>
@@ -1947,7 +1947,7 @@
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>'l</t>
+          <t>parameter missing. Please add this parameter.</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
@@ -1957,7 +1957,7 @@
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>Fail: 'l:event:prev_ts' parameter missing. Please add this parameter.</t>
+          <t>Fail: 'l:event:duration' parameter missing. Please add this parameter.</t>
         </is>
       </c>
     </row>
@@ -1969,7 +1969,7 @@
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>'l</t>
+          <t>parameter missing. Please add this parameter.</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
@@ -1979,7 +1979,7 @@
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>Fail: 'l:event:ts' parameter missing. Please add this parameter.</t>
+          <t>Fail: 'l:event:playhead' parameter missing. Please add this parameter.</t>
         </is>
       </c>
     </row>
@@ -1991,7 +1991,7 @@
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>'s</t>
+          <t>parameter missing. Please add this parameter.</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
@@ -2001,7 +2001,7 @@
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>Fail: 's:asset:name' parameter missing. Please add this parameter.</t>
+          <t>Fail: 'l:event:prev_ts' parameter missing. Please add this parameter.</t>
         </is>
       </c>
     </row>
@@ -2013,7 +2013,7 @@
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>'l</t>
+          <t>parameter missing. Please add this parameter.</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
@@ -2023,7 +2023,7 @@
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>Fail: 'l:asset:length' parameter missing. Please add this parameter.</t>
+          <t>Fail: 'l:event:ts' parameter missing. Please add this parameter.</t>
         </is>
       </c>
     </row>
@@ -2035,7 +2035,7 @@
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>'s</t>
+          <t>parameter missing. Please add this parameter.</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
@@ -2045,7 +2045,7 @@
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>Fail: 's:asset:publisher' parameter missing. Please add this parameter.</t>
+          <t>Fail: 's:asset:name' parameter missing. Please add this parameter.</t>
         </is>
       </c>
     </row>
@@ -2057,7 +2057,7 @@
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>'s</t>
+          <t>parameter missing. Please add this parameter.</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
@@ -2067,7 +2067,7 @@
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>Fail: 's:asset:type' parameter missing. Please add this parameter.</t>
+          <t>Fail: 'l:asset:length' parameter missing. Please add this parameter.</t>
         </is>
       </c>
     </row>
@@ -2079,17 +2079,17 @@
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>One of 'mid' variations found with value 69099319612994832056547930341105758682. URL</t>
+          <t>parameter missing. Please add this parameter.</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>Pass</t>
+          <t>Fail</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>Pass: One of 'mid' variations found with value 69099319612994832056547930341105758682. URL: https://smetrics.foxnews.com/b/ss/foxnewsglobalproduction/0/JAVA-4.17.9-AN/s40450848.</t>
+          <t>Fail: 's:asset:publisher' parameter missing. Please add this parameter.</t>
         </is>
       </c>
     </row>
@@ -2101,7 +2101,7 @@
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>'page_type' parameter missing. URL</t>
+          <t>parameter missing. Please add this parameter.</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
@@ -2111,7 +2111,7 @@
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>Fail: 'page_type' parameter missing. URL: https://smetrics.foxnews.com/b/ss/foxnewsglobalproduction/0/JAVA-4.17.9-AN/s40450848. Please add the 'page_type' parameter.</t>
+          <t>Fail: 's:asset:type' parameter missing. Please add this parameter.</t>
         </is>
       </c>
     </row>
@@ -2123,17 +2123,17 @@
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>'primary_business_unit' parameter missing. URL</t>
+          <t>variations found with value 69099319612994832056547930341105758682. URL: https://smetrics.foxnews.com/b/ss/foxnewsglobalproduction/0/JAVA-4.17.9-AN/s40450848.</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>Fail</t>
+          <t>Pass</t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>Fail: 'primary_business_unit' parameter missing. URL: https://smetrics.foxnews.com/b/ss/foxnewsglobalproduction/0/JAVA-4.17.9-AN/s40450848. Please add the 'primary_business_unit' parameter.</t>
+          <t>Pass: One of 'mid' variations found with value 69099319612994832056547930341105758682. URL: https://smetrics.foxnews.com/b/ss/foxnewsglobalproduction/0/JAVA-4.17.9-AN/s40450848.</t>
         </is>
       </c>
     </row>
@@ -2145,7 +2145,7 @@
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>'user_fox_anonymous_profile_id' parameter missing. Please add the 'user_fox_anonymous_profile_id' parameter.</t>
+          <t>parameter missing. URL: https://smetrics.foxnews.com/b/ss/foxnewsglobalproduction/0/JAVA-4.17.9-AN/s40450848. Please add the</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
@@ -2155,51 +2155,51 @@
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>Fail: 'user_fox_anonymous_profile_id' parameter missing. Please add the 'user_fox_anonymous_profile_id' parameter.</t>
+          <t>Fail: 'page_type' parameter missing. URL: https://smetrics.foxnews.com/b/ss/foxnewsglobalproduction/0/JAVA-4.17.9-AN/s40450848. Please add the 'page_type' parameter.</t>
         </is>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>http://foxnews.hb.omtrdc.net/?s:sc:rsid=foxnewsglobalproduction&amp;s:sc:tracking_server=smetrics.foxnews.com&amp;h:sc:ssl=1&amp;s:user:mid=69099319612994832056547930341105758682&amp;&amp;&amp;s:sp:ovp=Akamai&amp;s:sp:channel=Fox+News&amp;s:sp:player_name=Fox+News+Android+Player&amp;s:sp:hb_version=android-2.1.0.154-42fb90&amp;l:sp:hb_api_lvl=4&amp;s:event:sid=1673312989776217636246&amp;l:event:duration=0&amp;l:event:playhead=0&amp;l:event:prev_ts=-1&amp;s:event:type=aa_start&amp;l:event:ts=1673312991238&amp;s:asset:name=Biden+accused+of+mishandling+classified+documents&amp;l:asset:length=200&amp;s:asset:publisher=foxnews&amp;s:asset:type=main&amp;s:asset:video_id=6318425658112&amp;s:stream:type=vod&amp;l:stream:startup_time=0&amp;l:stream:fps=0&amp;l:stream:bitrate=0&amp;l:stream:dropped_frames=0</t>
+          <t>https://smetrics.foxnews.com/b/ss/foxnewsglobalproduction/0/JAVA-4.17.9-AN/s40450848</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>'s</t>
+          <t>parameter missing. URL: https://smetrics.foxnews.com/b/ss/foxnewsglobalproduction/0/JAVA-4.17.9-AN/s40450848. Please add the</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>Pass</t>
+          <t>Fail</t>
         </is>
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>Pass: 's:event:type' parameter found with value aa_start. URL: http://foxnews.hb.omtrdc.net/?s:sc:rsid=foxnewsglobalproduction&amp;s:sc:tracking_server=smetrics.foxnews.com&amp;h:sc:ssl=1&amp;s:user:mid=69099319612994832056547930341105758682&amp;&amp;&amp;s:sp:ovp=Akamai&amp;s:sp:channel=Fox+News&amp;s:sp:player_name=Fox+News+Android+Player&amp;s:sp:hb_version=android-2.1.0.154-42fb90&amp;l:sp:hb_api_lvl=4&amp;s:event:sid=1673312989776217636246&amp;l:event:duration=0&amp;l:event:playhead=0&amp;l:event:prev_ts=-1&amp;s:event:type=aa_start&amp;l:event:ts=1673312991238&amp;s:asset:name=Biden+accused+of+mishandling+classified+documents&amp;l:asset:length=200&amp;s:asset:publisher=foxnews&amp;s:asset:type=main&amp;s:asset:video_id=6318425658112&amp;s:stream:type=vod&amp;l:stream:startup_time=0&amp;l:stream:fps=0&amp;l:stream:bitrate=0&amp;l:stream:dropped_frames=0.</t>
+          <t>Fail: 'primary_business_unit' parameter missing. URL: https://smetrics.foxnews.com/b/ss/foxnewsglobalproduction/0/JAVA-4.17.9-AN/s40450848. Please add the 'primary_business_unit' parameter.</t>
         </is>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>http://foxnews.hb.omtrdc.net/?s:sc:rsid=foxnewsglobalproduction&amp;s:sc:tracking_server=smetrics.foxnews.com&amp;h:sc:ssl=1&amp;s:user:mid=69099319612994832056547930341105758682&amp;&amp;&amp;s:sp:ovp=Akamai&amp;s:sp:channel=Fox+News&amp;s:sp:player_name=Fox+News+Android+Player&amp;s:sp:hb_version=android-2.1.0.154-42fb90&amp;l:sp:hb_api_lvl=4&amp;s:event:sid=1673312989776217636246&amp;l:event:duration=0&amp;l:event:playhead=0&amp;l:event:prev_ts=-1&amp;s:event:type=aa_start&amp;l:event:ts=1673312991238&amp;s:asset:name=Biden+accused+of+mishandling+classified+documents&amp;l:asset:length=200&amp;s:asset:publisher=foxnews&amp;s:asset:type=main&amp;s:asset:video_id=6318425658112&amp;s:stream:type=vod&amp;l:stream:startup_time=0&amp;l:stream:fps=0&amp;l:stream:bitrate=0&amp;l:stream:dropped_frames=0</t>
+          <t>https://smetrics.foxnews.com/b/ss/foxnewsglobalproduction/0/JAVA-4.17.9-AN/s40450848</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>'s</t>
+          <t>parameter missing. Please add the</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>Pass</t>
+          <t>Fail</t>
         </is>
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>Pass: 's:event:sid' parameter found. URL: http://foxnews.hb.omtrdc.net/?s:sc:rsid=foxnewsglobalproduction&amp;s:sc:tracking_server=smetrics.foxnews.com&amp;h:sc:ssl=1&amp;s:user:mid=69099319612994832056547930341105758682&amp;&amp;&amp;s:sp:ovp=Akamai&amp;s:sp:channel=Fox+News&amp;s:sp:player_name=Fox+News+Android+Player&amp;s:sp:hb_version=android-2.1.0.154-42fb90&amp;l:sp:hb_api_lvl=4&amp;s:event:sid=1673312989776217636246&amp;l:event:duration=0&amp;l:event:playhead=0&amp;l:event:prev_ts=-1&amp;s:event:type=aa_start&amp;l:event:ts=1673312991238&amp;s:asset:name=Biden+accused+of+mishandling+classified+documents&amp;l:asset:length=200&amp;s:asset:publisher=foxnews&amp;s:asset:type=main&amp;s:asset:video_id=6318425658112&amp;s:stream:type=vod&amp;l:stream:startup_time=0&amp;l:stream:fps=0&amp;l:stream:bitrate=0&amp;l:stream:dropped_frames=0.</t>
+          <t>Fail: 'user_fox_anonymous_profile_id' parameter missing. Please add the 'user_fox_anonymous_profile_id' parameter.</t>
         </is>
       </c>
     </row>
@@ -2211,7 +2211,7 @@
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>'l</t>
+          <t>parameter found with value aa_start. URL: http://foxnews.hb.omtrdc.net/?s:sc:rsid=foxnewsglobalproduction&amp;s:sc:tracking_server=smetrics.foxnews.com&amp;h:sc:ssl=1&amp;s:user:mid=69099319612994832056547930341105758682&amp;&amp;&amp;s:sp:ovp=Akamai&amp;s:sp:channel=Fox+News&amp;s:sp:player_name=Fox+News+Android+Player&amp;s:sp:hb_version=android-2.1.0.154-42fb90&amp;l:sp:hb_api_lvl=4&amp;s:event:sid=1673312989776217636246&amp;l:event:duration=0&amp;l:event:playhead=0&amp;l:event:prev_ts=-1&amp;s:event:type=aa_start&amp;l:event:ts=1673312991238&amp;s:asset:name=Biden+accused+of+mishandling+classified+documents&amp;l:asset:length=200&amp;s:asset:publisher=foxnews&amp;s:asset:type=main&amp;s:asset:video_id=6318425658112&amp;s:stream:type=vod&amp;l:stream:startup_time=0&amp;l:stream:fps=0&amp;l:stream:bitrate=0&amp;l:stream:dropped_frames=0.</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
@@ -2221,7 +2221,7 @@
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>Pass: 'l:event:duration' parameter found.</t>
+          <t>Pass: 's:event:type' parameter found with value aa_start. URL: http://foxnews.hb.omtrdc.net/?s:sc:rsid=foxnewsglobalproduction&amp;s:sc:tracking_server=smetrics.foxnews.com&amp;h:sc:ssl=1&amp;s:user:mid=69099319612994832056547930341105758682&amp;&amp;&amp;s:sp:ovp=Akamai&amp;s:sp:channel=Fox+News&amp;s:sp:player_name=Fox+News+Android+Player&amp;s:sp:hb_version=android-2.1.0.154-42fb90&amp;l:sp:hb_api_lvl=4&amp;s:event:sid=1673312989776217636246&amp;l:event:duration=0&amp;l:event:playhead=0&amp;l:event:prev_ts=-1&amp;s:event:type=aa_start&amp;l:event:ts=1673312991238&amp;s:asset:name=Biden+accused+of+mishandling+classified+documents&amp;l:asset:length=200&amp;s:asset:publisher=foxnews&amp;s:asset:type=main&amp;s:asset:video_id=6318425658112&amp;s:stream:type=vod&amp;l:stream:startup_time=0&amp;l:stream:fps=0&amp;l:stream:bitrate=0&amp;l:stream:dropped_frames=0.</t>
         </is>
       </c>
     </row>
@@ -2233,7 +2233,7 @@
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>'l</t>
+          <t>parameter found with value aa_start. URL: http://foxnews.hb.omtrdc.net/?s:sc:rsid=foxnewsglobalproduction&amp;s:sc:tracking_server=smetrics.foxnews.com&amp;h:sc:ssl=1&amp;s:user:mid=69099319612994832056547930341105758682&amp;&amp;&amp;s:sp:ovp=Akamai&amp;s:sp:channel=Fox+News&amp;s:sp:player_name=Fox+News+Android+Player&amp;s:sp:hb_version=android-2.1.0.154-42fb90&amp;l:sp:hb_api_lvl=4&amp;s:event:sid=1673312989776217636246&amp;l:event:duration=0&amp;l:event:playhead=0&amp;l:event:prev_ts=-1&amp;s:event:type=aa_start&amp;l:event:ts=1673312991238&amp;s:asset:name=Biden+accused+of+mishandling+classified+documents&amp;l:asset:length=200&amp;s:asset:publisher=foxnews&amp;s:asset:type=main&amp;s:asset:video_id=6318425658112&amp;s:stream:type=vod&amp;l:stream:startup_time=0&amp;l:stream:fps=0&amp;l:stream:bitrate=0&amp;l:stream:dropped_frames=0.</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
@@ -2243,7 +2243,7 @@
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>Pass: 'l:event:playhead' parameter found.</t>
+          <t>Pass: 's:event:type' parameter found with value aa_start. URL: http://foxnews.hb.omtrdc.net/?s:sc:rsid=foxnewsglobalproduction&amp;s:sc:tracking_server=smetrics.foxnews.com&amp;h:sc:ssl=1&amp;s:user:mid=69099319612994832056547930341105758682&amp;&amp;&amp;s:sp:ovp=Akamai&amp;s:sp:channel=Fox+News&amp;s:sp:player_name=Fox+News+Android+Player&amp;s:sp:hb_version=android-2.1.0.154-42fb90&amp;l:sp:hb_api_lvl=4&amp;s:event:sid=1673312989776217636246&amp;l:event:duration=0&amp;l:event:playhead=0&amp;l:event:prev_ts=-1&amp;s:event:type=aa_start&amp;l:event:ts=1673312991238&amp;s:asset:name=Biden+accused+of+mishandling+classified+documents&amp;l:asset:length=200&amp;s:asset:publisher=foxnews&amp;s:asset:type=main&amp;s:asset:video_id=6318425658112&amp;s:stream:type=vod&amp;l:stream:startup_time=0&amp;l:stream:fps=0&amp;l:stream:bitrate=0&amp;l:stream:dropped_frames=0.</t>
         </is>
       </c>
     </row>
@@ -2255,7 +2255,7 @@
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>'l</t>
+          <t>parameter found. URL: http://foxnews.hb.omtrdc.net/?s:sc:rsid=foxnewsglobalproduction&amp;s:sc:tracking_server=smetrics.foxnews.com&amp;h:sc:ssl=1&amp;s:user:mid=69099319612994832056547930341105758682&amp;&amp;&amp;s:sp:ovp=Akamai&amp;s:sp:channel=Fox+News&amp;s:sp:player_name=Fox+News+Android+Player&amp;s:sp:hb_version=android-2.1.0.154-42fb90&amp;l:sp:hb_api_lvl=4&amp;s:event:sid=1673312989776217636246&amp;l:event:duration=0&amp;l:event:playhead=0&amp;l:event:prev_ts=-1&amp;s:event:type=aa_start&amp;l:event:ts=1673312991238&amp;s:asset:name=Biden+accused+of+mishandling+classified+documents&amp;l:asset:length=200&amp;s:asset:publisher=foxnews&amp;s:asset:type=main&amp;s:asset:video_id=6318425658112&amp;s:stream:type=vod&amp;l:stream:startup_time=0&amp;l:stream:fps=0&amp;l:stream:bitrate=0&amp;l:stream:dropped_frames=0.</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
@@ -2265,7 +2265,7 @@
       </c>
       <c r="D84" t="inlineStr">
         <is>
-          <t>Pass: 'l:event:prev_ts' parameter found.</t>
+          <t>Pass: 's:event:sid' parameter found. URL: http://foxnews.hb.omtrdc.net/?s:sc:rsid=foxnewsglobalproduction&amp;s:sc:tracking_server=smetrics.foxnews.com&amp;h:sc:ssl=1&amp;s:user:mid=69099319612994832056547930341105758682&amp;&amp;&amp;s:sp:ovp=Akamai&amp;s:sp:channel=Fox+News&amp;s:sp:player_name=Fox+News+Android+Player&amp;s:sp:hb_version=android-2.1.0.154-42fb90&amp;l:sp:hb_api_lvl=4&amp;s:event:sid=1673312989776217636246&amp;l:event:duration=0&amp;l:event:playhead=0&amp;l:event:prev_ts=-1&amp;s:event:type=aa_start&amp;l:event:ts=1673312991238&amp;s:asset:name=Biden+accused+of+mishandling+classified+documents&amp;l:asset:length=200&amp;s:asset:publisher=foxnews&amp;s:asset:type=main&amp;s:asset:video_id=6318425658112&amp;s:stream:type=vod&amp;l:stream:startup_time=0&amp;l:stream:fps=0&amp;l:stream:bitrate=0&amp;l:stream:dropped_frames=0.</t>
         </is>
       </c>
     </row>
@@ -2277,7 +2277,7 @@
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>'l</t>
+          <t>parameter found.</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
@@ -2287,7 +2287,7 @@
       </c>
       <c r="D85" t="inlineStr">
         <is>
-          <t>Pass: 'l:event:ts' parameter found.</t>
+          <t>Pass: 'l:event:duration' parameter found.</t>
         </is>
       </c>
     </row>
@@ -2299,7 +2299,7 @@
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>'s</t>
+          <t>parameter found.</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
@@ -2309,7 +2309,7 @@
       </c>
       <c r="D86" t="inlineStr">
         <is>
-          <t>Pass: 's:asset:name' parameter found.</t>
+          <t>Pass: 'l:event:prev_ts' parameter found.</t>
         </is>
       </c>
     </row>
@@ -2321,7 +2321,7 @@
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>'l</t>
+          <t>parameter found.</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
@@ -2331,7 +2331,7 @@
       </c>
       <c r="D87" t="inlineStr">
         <is>
-          <t>Pass: 'l:asset:length' parameter found.</t>
+          <t>Pass: 'l:event:ts' parameter found.</t>
         </is>
       </c>
     </row>
@@ -2343,7 +2343,7 @@
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>'s</t>
+          <t>parameter found.</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
@@ -2353,7 +2353,7 @@
       </c>
       <c r="D88" t="inlineStr">
         <is>
-          <t>Pass: 's:asset:publisher' parameter found.</t>
+          <t>Pass: 's:asset:name' parameter found.</t>
         </is>
       </c>
     </row>
@@ -2365,7 +2365,7 @@
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>'s</t>
+          <t>parameter found.</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
@@ -2375,7 +2375,7 @@
       </c>
       <c r="D89" t="inlineStr">
         <is>
-          <t>Pass: 's:asset:type' parameter found.</t>
+          <t>Pass: 'l:asset:length' parameter found.</t>
         </is>
       </c>
     </row>
@@ -2387,7 +2387,7 @@
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>'s</t>
+          <t>parameter found.</t>
         </is>
       </c>
       <c r="C90" t="inlineStr">
@@ -2397,19 +2397,19 @@
       </c>
       <c r="D90" t="inlineStr">
         <is>
-          <t>Pass: 's:sc:rsid' parameter found with value foxnewsglobalproduction. URL: http://foxnews.hb.omtrdc.net/?s:sc:rsid=foxnewsglobalproduction&amp;s:sc:tracking_server=smetrics.foxnews.com&amp;h:sc:ssl=1&amp;s:user:mid=69099319612994832056547930341105758682&amp;&amp;&amp;s:sp:ovp=Akamai&amp;s:sp:channel=Fox+News&amp;s:sp:player_name=Fox+News+Android+Player&amp;s:sp:hb_version=android-2.1.0.154-42fb90&amp;l:sp:hb_api_lvl=4&amp;s:event:sid=1673312989776217636246&amp;l:event:duration=0&amp;l:event:playhead=0&amp;l:event:prev_ts=-1&amp;s:event:type=aa_start&amp;l:event:ts=1673312991238&amp;s:asset:name=Biden+accused+of+mishandling+classified+documents&amp;l:asset:length=200&amp;s:asset:publisher=foxnews&amp;s:asset:type=main&amp;s:asset:video_id=6318425658112&amp;s:stream:type=vod&amp;l:stream:startup_time=0&amp;l:stream:fps=0&amp;l:stream:bitrate=0&amp;l:stream:dropped_frames=0.</t>
+          <t>Pass: 's:asset:publisher' parameter found.</t>
         </is>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>http://foxnews.hb.omtrdc.net/?s:sc:rsid=foxnewsglobalproduction&amp;s:sc:tracking_server=smetrics.foxnews.com&amp;h:sc:ssl=1&amp;s:user:mid=69099319612994832056547930341105758682&amp;&amp;&amp;s:sp:ovp=Akamai&amp;s:sp:channel=Fox+News&amp;s:sp:player_name=Fox+News+Android+Player&amp;s:sp:hb_version=android-2.1.0.154-42fb90&amp;l:sp:hb_api_lvl=4&amp;s:event:sid=1673312989776217636246&amp;l:event:duration=3908&amp;l:event:playhead=0&amp;l:event:prev_ts=1673312989842&amp;s:event:type=buffer&amp;l:event:ts=1673312993750&amp;s:asset:name=Biden+accused+of+mishandling+classified+documents&amp;l:asset:length=200&amp;s:asset:publisher=foxnews&amp;s:asset:type=main&amp;s:asset:video_id=6318425658112&amp;s:stream:type=vod&amp;l:stream:startup_time=0&amp;l:stream:fps=0&amp;l:stream:bitrate=0&amp;l:stream:dropped_frames=0</t>
+          <t>http://foxnews.hb.omtrdc.net/?s:sc:rsid=foxnewsglobalproduction&amp;s:sc:tracking_server=smetrics.foxnews.com&amp;h:sc:ssl=1&amp;s:user:mid=69099319612994832056547930341105758682&amp;&amp;&amp;s:sp:ovp=Akamai&amp;s:sp:channel=Fox+News&amp;s:sp:player_name=Fox+News+Android+Player&amp;s:sp:hb_version=android-2.1.0.154-42fb90&amp;l:sp:hb_api_lvl=4&amp;s:event:sid=1673312989776217636246&amp;l:event:duration=0&amp;l:event:playhead=0&amp;l:event:prev_ts=-1&amp;s:event:type=aa_start&amp;l:event:ts=1673312991238&amp;s:asset:name=Biden+accused+of+mishandling+classified+documents&amp;l:asset:length=200&amp;s:asset:publisher=foxnews&amp;s:asset:type=main&amp;s:asset:video_id=6318425658112&amp;s:stream:type=vod&amp;l:stream:startup_time=0&amp;l:stream:fps=0&amp;l:stream:bitrate=0&amp;l:stream:dropped_frames=0</t>
         </is>
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>'s</t>
+          <t>parameter found.</t>
         </is>
       </c>
       <c r="C91" t="inlineStr">
@@ -2419,19 +2419,19 @@
       </c>
       <c r="D91" t="inlineStr">
         <is>
-          <t>Pass: 's:event:type' parameter found with value buffer. URL: http://foxnews.hb.omtrdc.net/?s:sc:rsid=foxnewsglobalproduction&amp;s:sc:tracking_server=smetrics.foxnews.com&amp;h:sc:ssl=1&amp;s:user:mid=69099319612994832056547930341105758682&amp;&amp;&amp;s:sp:ovp=Akamai&amp;s:sp:channel=Fox+News&amp;s:sp:player_name=Fox+News+Android+Player&amp;s:sp:hb_version=android-2.1.0.154-42fb90&amp;l:sp:hb_api_lvl=4&amp;s:event:sid=1673312989776217636246&amp;l:event:duration=3908&amp;l:event:playhead=0&amp;l:event:prev_ts=1673312989842&amp;s:event:type=buffer&amp;l:event:ts=1673312993750&amp;s:asset:name=Biden+accused+of+mishandling+classified+documents&amp;l:asset:length=200&amp;s:asset:publisher=foxnews&amp;s:asset:type=main&amp;s:asset:video_id=6318425658112&amp;s:stream:type=vod&amp;l:stream:startup_time=0&amp;l:stream:fps=0&amp;l:stream:bitrate=0&amp;l:stream:dropped_frames=0.</t>
+          <t>Pass: 's:asset:type' parameter found.</t>
         </is>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>http://foxnews.hb.omtrdc.net/?s:sc:rsid=foxnewsglobalproduction&amp;s:sc:tracking_server=smetrics.foxnews.com&amp;h:sc:ssl=1&amp;s:user:mid=69099319612994832056547930341105758682&amp;&amp;&amp;s:sp:ovp=Akamai&amp;s:sp:channel=Fox+News&amp;s:sp:player_name=Fox+News+Android+Player&amp;s:sp:hb_version=android-2.1.0.154-42fb90&amp;l:sp:hb_api_lvl=4&amp;s:event:sid=1673312989776217636246&amp;l:event:duration=3908&amp;l:event:playhead=0&amp;l:event:prev_ts=1673312989842&amp;s:event:type=buffer&amp;l:event:ts=1673312993750&amp;s:asset:name=Biden+accused+of+mishandling+classified+documents&amp;l:asset:length=200&amp;s:asset:publisher=foxnews&amp;s:asset:type=main&amp;s:asset:video_id=6318425658112&amp;s:stream:type=vod&amp;l:stream:startup_time=0&amp;l:stream:fps=0&amp;l:stream:bitrate=0&amp;l:stream:dropped_frames=0</t>
+          <t>http://foxnews.hb.omtrdc.net/?s:sc:rsid=foxnewsglobalproduction&amp;s:sc:tracking_server=smetrics.foxnews.com&amp;h:sc:ssl=1&amp;s:user:mid=69099319612994832056547930341105758682&amp;&amp;&amp;s:sp:ovp=Akamai&amp;s:sp:channel=Fox+News&amp;s:sp:player_name=Fox+News+Android+Player&amp;s:sp:hb_version=android-2.1.0.154-42fb90&amp;l:sp:hb_api_lvl=4&amp;s:event:sid=1673312989776217636246&amp;l:event:duration=0&amp;l:event:playhead=0&amp;l:event:prev_ts=-1&amp;s:event:type=aa_start&amp;l:event:ts=1673312991238&amp;s:asset:name=Biden+accused+of+mishandling+classified+documents&amp;l:asset:length=200&amp;s:asset:publisher=foxnews&amp;s:asset:type=main&amp;s:asset:video_id=6318425658112&amp;s:stream:type=vod&amp;l:stream:startup_time=0&amp;l:stream:fps=0&amp;l:stream:bitrate=0&amp;l:stream:dropped_frames=0</t>
         </is>
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>'s</t>
+          <t>parameter found with value foxnewsglobalproduction. URL: http://foxnews.hb.omtrdc.net/?s:sc:rsid=foxnewsglobalproduction&amp;s:sc:tracking_server=smetrics.foxnews.com&amp;h:sc:ssl=1&amp;s:user:mid=69099319612994832056547930341105758682&amp;&amp;&amp;s:sp:ovp=Akamai&amp;s:sp:channel=Fox+News&amp;s:sp:player_name=Fox+News+Android+Player&amp;s:sp:hb_version=android-2.1.0.154-42fb90&amp;l:sp:hb_api_lvl=4&amp;s:event:sid=1673312989776217636246&amp;l:event:duration=0&amp;l:event:playhead=0&amp;l:event:prev_ts=-1&amp;s:event:type=aa_start&amp;l:event:ts=1673312991238&amp;s:asset:name=Biden+accused+of+mishandling+classified+documents&amp;l:asset:length=200&amp;s:asset:publisher=foxnews&amp;s:asset:type=main&amp;s:asset:video_id=6318425658112&amp;s:stream:type=vod&amp;l:stream:startup_time=0&amp;l:stream:fps=0&amp;l:stream:bitrate=0&amp;l:stream:dropped_frames=0.</t>
         </is>
       </c>
       <c r="C92" t="inlineStr">
@@ -2441,7 +2441,7 @@
       </c>
       <c r="D92" t="inlineStr">
         <is>
-          <t>Pass: 's:event:sid' parameter found. URL: http://foxnews.hb.omtrdc.net/?s:sc:rsid=foxnewsglobalproduction&amp;s:sc:tracking_server=smetrics.foxnews.com&amp;h:sc:ssl=1&amp;s:user:mid=69099319612994832056547930341105758682&amp;&amp;&amp;s:sp:ovp=Akamai&amp;s:sp:channel=Fox+News&amp;s:sp:player_name=Fox+News+Android+Player&amp;s:sp:hb_version=android-2.1.0.154-42fb90&amp;l:sp:hb_api_lvl=4&amp;s:event:sid=1673312989776217636246&amp;l:event:duration=3908&amp;l:event:playhead=0&amp;l:event:prev_ts=1673312989842&amp;s:event:type=buffer&amp;l:event:ts=1673312993750&amp;s:asset:name=Biden+accused+of+mishandling+classified+documents&amp;l:asset:length=200&amp;s:asset:publisher=foxnews&amp;s:asset:type=main&amp;s:asset:video_id=6318425658112&amp;s:stream:type=vod&amp;l:stream:startup_time=0&amp;l:stream:fps=0&amp;l:stream:bitrate=0&amp;l:stream:dropped_frames=0.</t>
+          <t>Pass: 's:sc:rsid' parameter found with value foxnewsglobalproduction. URL: http://foxnews.hb.omtrdc.net/?s:sc:rsid=foxnewsglobalproduction&amp;s:sc:tracking_server=smetrics.foxnews.com&amp;h:sc:ssl=1&amp;s:user:mid=69099319612994832056547930341105758682&amp;&amp;&amp;s:sp:ovp=Akamai&amp;s:sp:channel=Fox+News&amp;s:sp:player_name=Fox+News+Android+Player&amp;s:sp:hb_version=android-2.1.0.154-42fb90&amp;l:sp:hb_api_lvl=4&amp;s:event:sid=1673312989776217636246&amp;l:event:duration=0&amp;l:event:playhead=0&amp;l:event:prev_ts=-1&amp;s:event:type=aa_start&amp;l:event:ts=1673312991238&amp;s:asset:name=Biden+accused+of+mishandling+classified+documents&amp;l:asset:length=200&amp;s:asset:publisher=foxnews&amp;s:asset:type=main&amp;s:asset:video_id=6318425658112&amp;s:stream:type=vod&amp;l:stream:startup_time=0&amp;l:stream:fps=0&amp;l:stream:bitrate=0&amp;l:stream:dropped_frames=0.</t>
         </is>
       </c>
     </row>
@@ -2453,7 +2453,7 @@
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>'l</t>
+          <t>parameter found with value buffer. URL: http://foxnews.hb.omtrdc.net/?s:sc:rsid=foxnewsglobalproduction&amp;s:sc:tracking_server=smetrics.foxnews.com&amp;h:sc:ssl=1&amp;s:user:mid=69099319612994832056547930341105758682&amp;&amp;&amp;s:sp:ovp=Akamai&amp;s:sp:channel=Fox+News&amp;s:sp:player_name=Fox+News+Android+Player&amp;s:sp:hb_version=android-2.1.0.154-42fb90&amp;l:sp:hb_api_lvl=4&amp;s:event:sid=1673312989776217636246&amp;l:event:duration=3908&amp;l:event:playhead=0&amp;l:event:prev_ts=1673312989842&amp;s:event:type=buffer&amp;l:event:ts=1673312993750&amp;s:asset:name=Biden+accused+of+mishandling+classified+documents&amp;l:asset:length=200&amp;s:asset:publisher=foxnews&amp;s:asset:type=main&amp;s:asset:video_id=6318425658112&amp;s:stream:type=vod&amp;l:stream:startup_time=0&amp;l:stream:fps=0&amp;l:stream:bitrate=0&amp;l:stream:dropped_frames=0.</t>
         </is>
       </c>
       <c r="C93" t="inlineStr">
@@ -2463,7 +2463,7 @@
       </c>
       <c r="D93" t="inlineStr">
         <is>
-          <t>Pass: 'l:event:duration' parameter found.</t>
+          <t>Pass: 's:event:type' parameter found with value buffer. URL: http://foxnews.hb.omtrdc.net/?s:sc:rsid=foxnewsglobalproduction&amp;s:sc:tracking_server=smetrics.foxnews.com&amp;h:sc:ssl=1&amp;s:user:mid=69099319612994832056547930341105758682&amp;&amp;&amp;s:sp:ovp=Akamai&amp;s:sp:channel=Fox+News&amp;s:sp:player_name=Fox+News+Android+Player&amp;s:sp:hb_version=android-2.1.0.154-42fb90&amp;l:sp:hb_api_lvl=4&amp;s:event:sid=1673312989776217636246&amp;l:event:duration=3908&amp;l:event:playhead=0&amp;l:event:prev_ts=1673312989842&amp;s:event:type=buffer&amp;l:event:ts=1673312993750&amp;s:asset:name=Biden+accused+of+mishandling+classified+documents&amp;l:asset:length=200&amp;s:asset:publisher=foxnews&amp;s:asset:type=main&amp;s:asset:video_id=6318425658112&amp;s:stream:type=vod&amp;l:stream:startup_time=0&amp;l:stream:fps=0&amp;l:stream:bitrate=0&amp;l:stream:dropped_frames=0.</t>
         </is>
       </c>
     </row>
@@ -2475,7 +2475,7 @@
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>'l</t>
+          <t>parameter found with value buffer. URL: http://foxnews.hb.omtrdc.net/?s:sc:rsid=foxnewsglobalproduction&amp;s:sc:tracking_server=smetrics.foxnews.com&amp;h:sc:ssl=1&amp;s:user:mid=69099319612994832056547930341105758682&amp;&amp;&amp;s:sp:ovp=Akamai&amp;s:sp:channel=Fox+News&amp;s:sp:player_name=Fox+News+Android+Player&amp;s:sp:hb_version=android-2.1.0.154-42fb90&amp;l:sp:hb_api_lvl=4&amp;s:event:sid=1673312989776217636246&amp;l:event:duration=3908&amp;l:event:playhead=0&amp;l:event:prev_ts=1673312989842&amp;s:event:type=buffer&amp;l:event:ts=1673312993750&amp;s:asset:name=Biden+accused+of+mishandling+classified+documents&amp;l:asset:length=200&amp;s:asset:publisher=foxnews&amp;s:asset:type=main&amp;s:asset:video_id=6318425658112&amp;s:stream:type=vod&amp;l:stream:startup_time=0&amp;l:stream:fps=0&amp;l:stream:bitrate=0&amp;l:stream:dropped_frames=0.</t>
         </is>
       </c>
       <c r="C94" t="inlineStr">
@@ -2485,7 +2485,7 @@
       </c>
       <c r="D94" t="inlineStr">
         <is>
-          <t>Pass: 'l:event:playhead' parameter found.</t>
+          <t>Pass: 's:event:type' parameter found with value buffer. URL: http://foxnews.hb.omtrdc.net/?s:sc:rsid=foxnewsglobalproduction&amp;s:sc:tracking_server=smetrics.foxnews.com&amp;h:sc:ssl=1&amp;s:user:mid=69099319612994832056547930341105758682&amp;&amp;&amp;s:sp:ovp=Akamai&amp;s:sp:channel=Fox+News&amp;s:sp:player_name=Fox+News+Android+Player&amp;s:sp:hb_version=android-2.1.0.154-42fb90&amp;l:sp:hb_api_lvl=4&amp;s:event:sid=1673312989776217636246&amp;l:event:duration=3908&amp;l:event:playhead=0&amp;l:event:prev_ts=1673312989842&amp;s:event:type=buffer&amp;l:event:ts=1673312993750&amp;s:asset:name=Biden+accused+of+mishandling+classified+documents&amp;l:asset:length=200&amp;s:asset:publisher=foxnews&amp;s:asset:type=main&amp;s:asset:video_id=6318425658112&amp;s:stream:type=vod&amp;l:stream:startup_time=0&amp;l:stream:fps=0&amp;l:stream:bitrate=0&amp;l:stream:dropped_frames=0.</t>
         </is>
       </c>
     </row>
@@ -2497,7 +2497,7 @@
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>'l</t>
+          <t>parameter found. URL: http://foxnews.hb.omtrdc.net/?s:sc:rsid=foxnewsglobalproduction&amp;s:sc:tracking_server=smetrics.foxnews.com&amp;h:sc:ssl=1&amp;s:user:mid=69099319612994832056547930341105758682&amp;&amp;&amp;s:sp:ovp=Akamai&amp;s:sp:channel=Fox+News&amp;s:sp:player_name=Fox+News+Android+Player&amp;s:sp:hb_version=android-2.1.0.154-42fb90&amp;l:sp:hb_api_lvl=4&amp;s:event:sid=1673312989776217636246&amp;l:event:duration=3908&amp;l:event:playhead=0&amp;l:event:prev_ts=1673312989842&amp;s:event:type=buffer&amp;l:event:ts=1673312993750&amp;s:asset:name=Biden+accused+of+mishandling+classified+documents&amp;l:asset:length=200&amp;s:asset:publisher=foxnews&amp;s:asset:type=main&amp;s:asset:video_id=6318425658112&amp;s:stream:type=vod&amp;l:stream:startup_time=0&amp;l:stream:fps=0&amp;l:stream:bitrate=0&amp;l:stream:dropped_frames=0.</t>
         </is>
       </c>
       <c r="C95" t="inlineStr">
@@ -2507,7 +2507,7 @@
       </c>
       <c r="D95" t="inlineStr">
         <is>
-          <t>Pass: 'l:event:prev_ts' parameter found.</t>
+          <t>Pass: 's:event:sid' parameter found. URL: http://foxnews.hb.omtrdc.net/?s:sc:rsid=foxnewsglobalproduction&amp;s:sc:tracking_server=smetrics.foxnews.com&amp;h:sc:ssl=1&amp;s:user:mid=69099319612994832056547930341105758682&amp;&amp;&amp;s:sp:ovp=Akamai&amp;s:sp:channel=Fox+News&amp;s:sp:player_name=Fox+News+Android+Player&amp;s:sp:hb_version=android-2.1.0.154-42fb90&amp;l:sp:hb_api_lvl=4&amp;s:event:sid=1673312989776217636246&amp;l:event:duration=3908&amp;l:event:playhead=0&amp;l:event:prev_ts=1673312989842&amp;s:event:type=buffer&amp;l:event:ts=1673312993750&amp;s:asset:name=Biden+accused+of+mishandling+classified+documents&amp;l:asset:length=200&amp;s:asset:publisher=foxnews&amp;s:asset:type=main&amp;s:asset:video_id=6318425658112&amp;s:stream:type=vod&amp;l:stream:startup_time=0&amp;l:stream:fps=0&amp;l:stream:bitrate=0&amp;l:stream:dropped_frames=0.</t>
         </is>
       </c>
     </row>
@@ -2519,7 +2519,7 @@
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>'l</t>
+          <t>parameter found.</t>
         </is>
       </c>
       <c r="C96" t="inlineStr">
@@ -2529,7 +2529,7 @@
       </c>
       <c r="D96" t="inlineStr">
         <is>
-          <t>Pass: 'l:event:ts' parameter found.</t>
+          <t>Pass: 'l:event:duration' parameter found.</t>
         </is>
       </c>
     </row>
@@ -2541,7 +2541,7 @@
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>'s</t>
+          <t>parameter found.</t>
         </is>
       </c>
       <c r="C97" t="inlineStr">
@@ -2551,7 +2551,7 @@
       </c>
       <c r="D97" t="inlineStr">
         <is>
-          <t>Pass: 's:asset:name' parameter found.</t>
+          <t>Pass: 'l:event:prev_ts' parameter found.</t>
         </is>
       </c>
     </row>
@@ -2563,7 +2563,7 @@
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>'l</t>
+          <t>parameter found.</t>
         </is>
       </c>
       <c r="C98" t="inlineStr">
@@ -2573,7 +2573,7 @@
       </c>
       <c r="D98" t="inlineStr">
         <is>
-          <t>Pass: 'l:asset:length' parameter found.</t>
+          <t>Pass: 'l:event:ts' parameter found.</t>
         </is>
       </c>
     </row>
@@ -2585,7 +2585,7 @@
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>'s</t>
+          <t>parameter found.</t>
         </is>
       </c>
       <c r="C99" t="inlineStr">
@@ -2595,7 +2595,7 @@
       </c>
       <c r="D99" t="inlineStr">
         <is>
-          <t>Pass: 's:asset:publisher' parameter found.</t>
+          <t>Pass: 's:asset:name' parameter found.</t>
         </is>
       </c>
     </row>
@@ -2607,7 +2607,7 @@
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>'s</t>
+          <t>parameter found.</t>
         </is>
       </c>
       <c r="C100" t="inlineStr">
@@ -2617,7 +2617,7 @@
       </c>
       <c r="D100" t="inlineStr">
         <is>
-          <t>Pass: 's:asset:type' parameter found.</t>
+          <t>Pass: 'l:asset:length' parameter found.</t>
         </is>
       </c>
     </row>
@@ -2629,7 +2629,7 @@
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>'s</t>
+          <t>parameter found.</t>
         </is>
       </c>
       <c r="C101" t="inlineStr">
@@ -2639,19 +2639,19 @@
       </c>
       <c r="D101" t="inlineStr">
         <is>
-          <t>Pass: 's:sc:rsid' parameter found with value foxnewsglobalproduction. URL: http://foxnews.hb.omtrdc.net/?s:sc:rsid=foxnewsglobalproduction&amp;s:sc:tracking_server=smetrics.foxnews.com&amp;h:sc:ssl=1&amp;s:user:mid=69099319612994832056547930341105758682&amp;&amp;&amp;s:sp:ovp=Akamai&amp;s:sp:channel=Fox+News&amp;s:sp:player_name=Fox+News+Android+Player&amp;s:sp:hb_version=android-2.1.0.154-42fb90&amp;l:sp:hb_api_lvl=4&amp;s:event:sid=1673312989776217636246&amp;l:event:duration=3908&amp;l:event:playhead=0&amp;l:event:prev_ts=1673312989842&amp;s:event:type=buffer&amp;l:event:ts=1673312993750&amp;s:asset:name=Biden+accused+of+mishandling+classified+documents&amp;l:asset:length=200&amp;s:asset:publisher=foxnews&amp;s:asset:type=main&amp;s:asset:video_id=6318425658112&amp;s:stream:type=vod&amp;l:stream:startup_time=0&amp;l:stream:fps=0&amp;l:stream:bitrate=0&amp;l:stream:dropped_frames=0.</t>
+          <t>Pass: 's:asset:publisher' parameter found.</t>
         </is>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>http://foxnews.hb.omtrdc.net/?s:sc:rsid=foxnewsglobalproduction&amp;s:sc:tracking_server=smetrics.foxnews.com&amp;h:sc:ssl=1&amp;s:user:mid=69099319612994832056547930341105758682&amp;&amp;&amp;s:sp:ovp=Akamai&amp;s:sp:channel=Fox+News&amp;s:sp:player_name=Fox+News+Android+Player&amp;s:sp:hb_version=android-2.1.0.154-42fb90&amp;l:sp:hb_api_lvl=4&amp;s:event:sid=1673312989776217636246&amp;l:event:duration=338&amp;l:event:playhead=227&amp;l:event:prev_ts=-1&amp;s:event:type=pause&amp;l:event:ts=1673312994087&amp;s:asset:name=Biden+accused+of+mishandling+classified+documents&amp;l:asset:length=200&amp;s:asset:publisher=foxnews&amp;s:asset:type=main&amp;s:asset:video_id=6318425658112&amp;s:stream:type=vod&amp;l:stream:startup_time=0&amp;l:stream:fps=0&amp;l:stream:bitrate=0&amp;l:stream:dropped_frames=0</t>
+          <t>http://foxnews.hb.omtrdc.net/?s:sc:rsid=foxnewsglobalproduction&amp;s:sc:tracking_server=smetrics.foxnews.com&amp;h:sc:ssl=1&amp;s:user:mid=69099319612994832056547930341105758682&amp;&amp;&amp;s:sp:ovp=Akamai&amp;s:sp:channel=Fox+News&amp;s:sp:player_name=Fox+News+Android+Player&amp;s:sp:hb_version=android-2.1.0.154-42fb90&amp;l:sp:hb_api_lvl=4&amp;s:event:sid=1673312989776217636246&amp;l:event:duration=3908&amp;l:event:playhead=0&amp;l:event:prev_ts=1673312989842&amp;s:event:type=buffer&amp;l:event:ts=1673312993750&amp;s:asset:name=Biden+accused+of+mishandling+classified+documents&amp;l:asset:length=200&amp;s:asset:publisher=foxnews&amp;s:asset:type=main&amp;s:asset:video_id=6318425658112&amp;s:stream:type=vod&amp;l:stream:startup_time=0&amp;l:stream:fps=0&amp;l:stream:bitrate=0&amp;l:stream:dropped_frames=0</t>
         </is>
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>'s</t>
+          <t>parameter found.</t>
         </is>
       </c>
       <c r="C102" t="inlineStr">
@@ -2661,19 +2661,19 @@
       </c>
       <c r="D102" t="inlineStr">
         <is>
-          <t>Pass: 's:event:type' parameter found with value pause. URL: http://foxnews.hb.omtrdc.net/?s:sc:rsid=foxnewsglobalproduction&amp;s:sc:tracking_server=smetrics.foxnews.com&amp;h:sc:ssl=1&amp;s:user:mid=69099319612994832056547930341105758682&amp;&amp;&amp;s:sp:ovp=Akamai&amp;s:sp:channel=Fox+News&amp;s:sp:player_name=Fox+News+Android+Player&amp;s:sp:hb_version=android-2.1.0.154-42fb90&amp;l:sp:hb_api_lvl=4&amp;s:event:sid=1673312989776217636246&amp;l:event:duration=338&amp;l:event:playhead=227&amp;l:event:prev_ts=-1&amp;s:event:type=pause&amp;l:event:ts=1673312994087&amp;s:asset:name=Biden+accused+of+mishandling+classified+documents&amp;l:asset:length=200&amp;s:asset:publisher=foxnews&amp;s:asset:type=main&amp;s:asset:video_id=6318425658112&amp;s:stream:type=vod&amp;l:stream:startup_time=0&amp;l:stream:fps=0&amp;l:stream:bitrate=0&amp;l:stream:dropped_frames=0.</t>
+          <t>Pass: 's:asset:type' parameter found.</t>
         </is>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>http://foxnews.hb.omtrdc.net/?s:sc:rsid=foxnewsglobalproduction&amp;s:sc:tracking_server=smetrics.foxnews.com&amp;h:sc:ssl=1&amp;s:user:mid=69099319612994832056547930341105758682&amp;&amp;&amp;s:sp:ovp=Akamai&amp;s:sp:channel=Fox+News&amp;s:sp:player_name=Fox+News+Android+Player&amp;s:sp:hb_version=android-2.1.0.154-42fb90&amp;l:sp:hb_api_lvl=4&amp;s:event:sid=1673312989776217636246&amp;l:event:duration=338&amp;l:event:playhead=227&amp;l:event:prev_ts=-1&amp;s:event:type=pause&amp;l:event:ts=1673312994087&amp;s:asset:name=Biden+accused+of+mishandling+classified+documents&amp;l:asset:length=200&amp;s:asset:publisher=foxnews&amp;s:asset:type=main&amp;s:asset:video_id=6318425658112&amp;s:stream:type=vod&amp;l:stream:startup_time=0&amp;l:stream:fps=0&amp;l:stream:bitrate=0&amp;l:stream:dropped_frames=0</t>
+          <t>http://foxnews.hb.omtrdc.net/?s:sc:rsid=foxnewsglobalproduction&amp;s:sc:tracking_server=smetrics.foxnews.com&amp;h:sc:ssl=1&amp;s:user:mid=69099319612994832056547930341105758682&amp;&amp;&amp;s:sp:ovp=Akamai&amp;s:sp:channel=Fox+News&amp;s:sp:player_name=Fox+News+Android+Player&amp;s:sp:hb_version=android-2.1.0.154-42fb90&amp;l:sp:hb_api_lvl=4&amp;s:event:sid=1673312989776217636246&amp;l:event:duration=3908&amp;l:event:playhead=0&amp;l:event:prev_ts=1673312989842&amp;s:event:type=buffer&amp;l:event:ts=1673312993750&amp;s:asset:name=Biden+accused+of+mishandling+classified+documents&amp;l:asset:length=200&amp;s:asset:publisher=foxnews&amp;s:asset:type=main&amp;s:asset:video_id=6318425658112&amp;s:stream:type=vod&amp;l:stream:startup_time=0&amp;l:stream:fps=0&amp;l:stream:bitrate=0&amp;l:stream:dropped_frames=0</t>
         </is>
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>'s</t>
+          <t>parameter found with value foxnewsglobalproduction. URL: http://foxnews.hb.omtrdc.net/?s:sc:rsid=foxnewsglobalproduction&amp;s:sc:tracking_server=smetrics.foxnews.com&amp;h:sc:ssl=1&amp;s:user:mid=69099319612994832056547930341105758682&amp;&amp;&amp;s:sp:ovp=Akamai&amp;s:sp:channel=Fox+News&amp;s:sp:player_name=Fox+News+Android+Player&amp;s:sp:hb_version=android-2.1.0.154-42fb90&amp;l:sp:hb_api_lvl=4&amp;s:event:sid=1673312989776217636246&amp;l:event:duration=3908&amp;l:event:playhead=0&amp;l:event:prev_ts=1673312989842&amp;s:event:type=buffer&amp;l:event:ts=1673312993750&amp;s:asset:name=Biden+accused+of+mishandling+classified+documents&amp;l:asset:length=200&amp;s:asset:publisher=foxnews&amp;s:asset:type=main&amp;s:asset:video_id=6318425658112&amp;s:stream:type=vod&amp;l:stream:startup_time=0&amp;l:stream:fps=0&amp;l:stream:bitrate=0&amp;l:stream:dropped_frames=0.</t>
         </is>
       </c>
       <c r="C103" t="inlineStr">
@@ -2683,7 +2683,7 @@
       </c>
       <c r="D103" t="inlineStr">
         <is>
-          <t>Pass: 's:event:sid' parameter found. URL: http://foxnews.hb.omtrdc.net/?s:sc:rsid=foxnewsglobalproduction&amp;s:sc:tracking_server=smetrics.foxnews.com&amp;h:sc:ssl=1&amp;s:user:mid=69099319612994832056547930341105758682&amp;&amp;&amp;s:sp:ovp=Akamai&amp;s:sp:channel=Fox+News&amp;s:sp:player_name=Fox+News+Android+Player&amp;s:sp:hb_version=android-2.1.0.154-42fb90&amp;l:sp:hb_api_lvl=4&amp;s:event:sid=1673312989776217636246&amp;l:event:duration=338&amp;l:event:playhead=227&amp;l:event:prev_ts=-1&amp;s:event:type=pause&amp;l:event:ts=1673312994087&amp;s:asset:name=Biden+accused+of+mishandling+classified+documents&amp;l:asset:length=200&amp;s:asset:publisher=foxnews&amp;s:asset:type=main&amp;s:asset:video_id=6318425658112&amp;s:stream:type=vod&amp;l:stream:startup_time=0&amp;l:stream:fps=0&amp;l:stream:bitrate=0&amp;l:stream:dropped_frames=0.</t>
+          <t>Pass: 's:sc:rsid' parameter found with value foxnewsglobalproduction. URL: http://foxnews.hb.omtrdc.net/?s:sc:rsid=foxnewsglobalproduction&amp;s:sc:tracking_server=smetrics.foxnews.com&amp;h:sc:ssl=1&amp;s:user:mid=69099319612994832056547930341105758682&amp;&amp;&amp;s:sp:ovp=Akamai&amp;s:sp:channel=Fox+News&amp;s:sp:player_name=Fox+News+Android+Player&amp;s:sp:hb_version=android-2.1.0.154-42fb90&amp;l:sp:hb_api_lvl=4&amp;s:event:sid=1673312989776217636246&amp;l:event:duration=3908&amp;l:event:playhead=0&amp;l:event:prev_ts=1673312989842&amp;s:event:type=buffer&amp;l:event:ts=1673312993750&amp;s:asset:name=Biden+accused+of+mishandling+classified+documents&amp;l:asset:length=200&amp;s:asset:publisher=foxnews&amp;s:asset:type=main&amp;s:asset:video_id=6318425658112&amp;s:stream:type=vod&amp;l:stream:startup_time=0&amp;l:stream:fps=0&amp;l:stream:bitrate=0&amp;l:stream:dropped_frames=0.</t>
         </is>
       </c>
     </row>
@@ -2695,7 +2695,7 @@
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>'l</t>
+          <t>parameter found with value pause. URL: http://foxnews.hb.omtrdc.net/?s:sc:rsid=foxnewsglobalproduction&amp;s:sc:tracking_server=smetrics.foxnews.com&amp;h:sc:ssl=1&amp;s:user:mid=69099319612994832056547930341105758682&amp;&amp;&amp;s:sp:ovp=Akamai&amp;s:sp:channel=Fox+News&amp;s:sp:player_name=Fox+News+Android+Player&amp;s:sp:hb_version=android-2.1.0.154-42fb90&amp;l:sp:hb_api_lvl=4&amp;s:event:sid=1673312989776217636246&amp;l:event:duration=338&amp;l:event:playhead=227&amp;l:event:prev_ts=-1&amp;s:event:type=pause&amp;l:event:ts=1673312994087&amp;s:asset:name=Biden+accused+of+mishandling+classified+documents&amp;l:asset:length=200&amp;s:asset:publisher=foxnews&amp;s:asset:type=main&amp;s:asset:video_id=6318425658112&amp;s:stream:type=vod&amp;l:stream:startup_time=0&amp;l:stream:fps=0&amp;l:stream:bitrate=0&amp;l:stream:dropped_frames=0.</t>
         </is>
       </c>
       <c r="C104" t="inlineStr">
@@ -2705,7 +2705,7 @@
       </c>
       <c r="D104" t="inlineStr">
         <is>
-          <t>Pass: 'l:event:duration' parameter found.</t>
+          <t>Pass: 's:event:type' parameter found with value pause. URL: http://foxnews.hb.omtrdc.net/?s:sc:rsid=foxnewsglobalproduction&amp;s:sc:tracking_server=smetrics.foxnews.com&amp;h:sc:ssl=1&amp;s:user:mid=69099319612994832056547930341105758682&amp;&amp;&amp;s:sp:ovp=Akamai&amp;s:sp:channel=Fox+News&amp;s:sp:player_name=Fox+News+Android+Player&amp;s:sp:hb_version=android-2.1.0.154-42fb90&amp;l:sp:hb_api_lvl=4&amp;s:event:sid=1673312989776217636246&amp;l:event:duration=338&amp;l:event:playhead=227&amp;l:event:prev_ts=-1&amp;s:event:type=pause&amp;l:event:ts=1673312994087&amp;s:asset:name=Biden+accused+of+mishandling+classified+documents&amp;l:asset:length=200&amp;s:asset:publisher=foxnews&amp;s:asset:type=main&amp;s:asset:video_id=6318425658112&amp;s:stream:type=vod&amp;l:stream:startup_time=0&amp;l:stream:fps=0&amp;l:stream:bitrate=0&amp;l:stream:dropped_frames=0.</t>
         </is>
       </c>
     </row>
@@ -2717,7 +2717,7 @@
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>'l</t>
+          <t>parameter found with value pause. URL: http://foxnews.hb.omtrdc.net/?s:sc:rsid=foxnewsglobalproduction&amp;s:sc:tracking_server=smetrics.foxnews.com&amp;h:sc:ssl=1&amp;s:user:mid=69099319612994832056547930341105758682&amp;&amp;&amp;s:sp:ovp=Akamai&amp;s:sp:channel=Fox+News&amp;s:sp:player_name=Fox+News+Android+Player&amp;s:sp:hb_version=android-2.1.0.154-42fb90&amp;l:sp:hb_api_lvl=4&amp;s:event:sid=1673312989776217636246&amp;l:event:duration=338&amp;l:event:playhead=227&amp;l:event:prev_ts=-1&amp;s:event:type=pause&amp;l:event:ts=1673312994087&amp;s:asset:name=Biden+accused+of+mishandling+classified+documents&amp;l:asset:length=200&amp;s:asset:publisher=foxnews&amp;s:asset:type=main&amp;s:asset:video_id=6318425658112&amp;s:stream:type=vod&amp;l:stream:startup_time=0&amp;l:stream:fps=0&amp;l:stream:bitrate=0&amp;l:stream:dropped_frames=0.</t>
         </is>
       </c>
       <c r="C105" t="inlineStr">
@@ -2727,7 +2727,7 @@
       </c>
       <c r="D105" t="inlineStr">
         <is>
-          <t>Pass: 'l:event:playhead' parameter found.</t>
+          <t>Pass: 's:event:type' parameter found with value pause. URL: http://foxnews.hb.omtrdc.net/?s:sc:rsid=foxnewsglobalproduction&amp;s:sc:tracking_server=smetrics.foxnews.com&amp;h:sc:ssl=1&amp;s:user:mid=69099319612994832056547930341105758682&amp;&amp;&amp;s:sp:ovp=Akamai&amp;s:sp:channel=Fox+News&amp;s:sp:player_name=Fox+News+Android+Player&amp;s:sp:hb_version=android-2.1.0.154-42fb90&amp;l:sp:hb_api_lvl=4&amp;s:event:sid=1673312989776217636246&amp;l:event:duration=338&amp;l:event:playhead=227&amp;l:event:prev_ts=-1&amp;s:event:type=pause&amp;l:event:ts=1673312994087&amp;s:asset:name=Biden+accused+of+mishandling+classified+documents&amp;l:asset:length=200&amp;s:asset:publisher=foxnews&amp;s:asset:type=main&amp;s:asset:video_id=6318425658112&amp;s:stream:type=vod&amp;l:stream:startup_time=0&amp;l:stream:fps=0&amp;l:stream:bitrate=0&amp;l:stream:dropped_frames=0.</t>
         </is>
       </c>
     </row>
@@ -2739,7 +2739,7 @@
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>'l</t>
+          <t>parameter found. URL: http://foxnews.hb.omtrdc.net/?s:sc:rsid=foxnewsglobalproduction&amp;s:sc:tracking_server=smetrics.foxnews.com&amp;h:sc:ssl=1&amp;s:user:mid=69099319612994832056547930341105758682&amp;&amp;&amp;s:sp:ovp=Akamai&amp;s:sp:channel=Fox+News&amp;s:sp:player_name=Fox+News+Android+Player&amp;s:sp:hb_version=android-2.1.0.154-42fb90&amp;l:sp:hb_api_lvl=4&amp;s:event:sid=1673312989776217636246&amp;l:event:duration=338&amp;l:event:playhead=227&amp;l:event:prev_ts=-1&amp;s:event:type=pause&amp;l:event:ts=1673312994087&amp;s:asset:name=Biden+accused+of+mishandling+classified+documents&amp;l:asset:length=200&amp;s:asset:publisher=foxnews&amp;s:asset:type=main&amp;s:asset:video_id=6318425658112&amp;s:stream:type=vod&amp;l:stream:startup_time=0&amp;l:stream:fps=0&amp;l:stream:bitrate=0&amp;l:stream:dropped_frames=0.</t>
         </is>
       </c>
       <c r="C106" t="inlineStr">
@@ -2749,7 +2749,7 @@
       </c>
       <c r="D106" t="inlineStr">
         <is>
-          <t>Pass: 'l:event:prev_ts' parameter found.</t>
+          <t>Pass: 's:event:sid' parameter found. URL: http://foxnews.hb.omtrdc.net/?s:sc:rsid=foxnewsglobalproduction&amp;s:sc:tracking_server=smetrics.foxnews.com&amp;h:sc:ssl=1&amp;s:user:mid=69099319612994832056547930341105758682&amp;&amp;&amp;s:sp:ovp=Akamai&amp;s:sp:channel=Fox+News&amp;s:sp:player_name=Fox+News+Android+Player&amp;s:sp:hb_version=android-2.1.0.154-42fb90&amp;l:sp:hb_api_lvl=4&amp;s:event:sid=1673312989776217636246&amp;l:event:duration=338&amp;l:event:playhead=227&amp;l:event:prev_ts=-1&amp;s:event:type=pause&amp;l:event:ts=1673312994087&amp;s:asset:name=Biden+accused+of+mishandling+classified+documents&amp;l:asset:length=200&amp;s:asset:publisher=foxnews&amp;s:asset:type=main&amp;s:asset:video_id=6318425658112&amp;s:stream:type=vod&amp;l:stream:startup_time=0&amp;l:stream:fps=0&amp;l:stream:bitrate=0&amp;l:stream:dropped_frames=0.</t>
         </is>
       </c>
     </row>
@@ -2761,7 +2761,7 @@
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>'l</t>
+          <t>parameter found.</t>
         </is>
       </c>
       <c r="C107" t="inlineStr">
@@ -2771,7 +2771,7 @@
       </c>
       <c r="D107" t="inlineStr">
         <is>
-          <t>Pass: 'l:event:ts' parameter found.</t>
+          <t>Pass: 'l:event:duration' parameter found.</t>
         </is>
       </c>
     </row>
@@ -2783,7 +2783,7 @@
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>'s</t>
+          <t>parameter found.</t>
         </is>
       </c>
       <c r="C108" t="inlineStr">
@@ -2793,7 +2793,7 @@
       </c>
       <c r="D108" t="inlineStr">
         <is>
-          <t>Pass: 's:asset:name' parameter found.</t>
+          <t>Pass: 'l:event:prev_ts' parameter found.</t>
         </is>
       </c>
     </row>
@@ -2805,7 +2805,7 @@
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>'l</t>
+          <t>parameter found.</t>
         </is>
       </c>
       <c r="C109" t="inlineStr">
@@ -2815,7 +2815,7 @@
       </c>
       <c r="D109" t="inlineStr">
         <is>
-          <t>Pass: 'l:asset:length' parameter found.</t>
+          <t>Pass: 'l:event:ts' parameter found.</t>
         </is>
       </c>
     </row>
@@ -2827,7 +2827,7 @@
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>'s</t>
+          <t>parameter found.</t>
         </is>
       </c>
       <c r="C110" t="inlineStr">
@@ -2837,7 +2837,7 @@
       </c>
       <c r="D110" t="inlineStr">
         <is>
-          <t>Pass: 's:asset:publisher' parameter found.</t>
+          <t>Pass: 's:asset:name' parameter found.</t>
         </is>
       </c>
     </row>
@@ -2849,7 +2849,7 @@
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>'s</t>
+          <t>parameter found.</t>
         </is>
       </c>
       <c r="C111" t="inlineStr">
@@ -2859,7 +2859,7 @@
       </c>
       <c r="D111" t="inlineStr">
         <is>
-          <t>Pass: 's:asset:type' parameter found.</t>
+          <t>Pass: 'l:asset:length' parameter found.</t>
         </is>
       </c>
     </row>
@@ -2871,7 +2871,7 @@
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>'s</t>
+          <t>parameter found.</t>
         </is>
       </c>
       <c r="C112" t="inlineStr">
@@ -2881,19 +2881,19 @@
       </c>
       <c r="D112" t="inlineStr">
         <is>
-          <t>Pass: 's:sc:rsid' parameter found with value foxnewsglobalproduction. URL: http://foxnews.hb.omtrdc.net/?s:sc:rsid=foxnewsglobalproduction&amp;s:sc:tracking_server=smetrics.foxnews.com&amp;h:sc:ssl=1&amp;s:user:mid=69099319612994832056547930341105758682&amp;&amp;&amp;s:sp:ovp=Akamai&amp;s:sp:channel=Fox+News&amp;s:sp:player_name=Fox+News+Android+Player&amp;s:sp:hb_version=android-2.1.0.154-42fb90&amp;l:sp:hb_api_lvl=4&amp;s:event:sid=1673312989776217636246&amp;l:event:duration=338&amp;l:event:playhead=227&amp;l:event:prev_ts=-1&amp;s:event:type=pause&amp;l:event:ts=1673312994087&amp;s:asset:name=Biden+accused+of+mishandling+classified+documents&amp;l:asset:length=200&amp;s:asset:publisher=foxnews&amp;s:asset:type=main&amp;s:asset:video_id=6318425658112&amp;s:stream:type=vod&amp;l:stream:startup_time=0&amp;l:stream:fps=0&amp;l:stream:bitrate=0&amp;l:stream:dropped_frames=0.</t>
+          <t>Pass: 's:asset:publisher' parameter found.</t>
         </is>
       </c>
     </row>
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>http://foxnews.hb.omtrdc.net/?s:sc:rsid=foxnewsglobalproduction&amp;s:sc:tracking_server=smetrics.foxnews.com&amp;h:sc:ssl=1&amp;s:user:mid=69099319612994832056547930341105758682&amp;&amp;&amp;s:sp:ovp=Akamai&amp;s:sp:channel=Fox+News&amp;s:sp:player_name=Fox+News+Android+Player&amp;s:sp:hb_version=android-2.1.0.154-42fb90&amp;l:sp:hb_api_lvl=4&amp;s:event:sid=1673312989776217636246&amp;l:event:duration=0&amp;l:event:playhead=227&amp;l:event:prev_ts=-1&amp;s:event:type=play&amp;l:event:ts=1673312994087&amp;s:asset:name=Biden+accused+of+mishandling+classified+documents&amp;l:asset:length=200&amp;s:asset:publisher=foxnews&amp;s:asset:type=main&amp;s:asset:video_id=6318425658112&amp;s:stream:type=vod&amp;l:stream:startup_time=0&amp;l:stream:fps=0&amp;l:stream:bitrate=0&amp;l:stream:dropped_frames=0</t>
+          <t>http://foxnews.hb.omtrdc.net/?s:sc:rsid=foxnewsglobalproduction&amp;s:sc:tracking_server=smetrics.foxnews.com&amp;h:sc:ssl=1&amp;s:user:mid=69099319612994832056547930341105758682&amp;&amp;&amp;s:sp:ovp=Akamai&amp;s:sp:channel=Fox+News&amp;s:sp:player_name=Fox+News+Android+Player&amp;s:sp:hb_version=android-2.1.0.154-42fb90&amp;l:sp:hb_api_lvl=4&amp;s:event:sid=1673312989776217636246&amp;l:event:duration=338&amp;l:event:playhead=227&amp;l:event:prev_ts=-1&amp;s:event:type=pause&amp;l:event:ts=1673312994087&amp;s:asset:name=Biden+accused+of+mishandling+classified+documents&amp;l:asset:length=200&amp;s:asset:publisher=foxnews&amp;s:asset:type=main&amp;s:asset:video_id=6318425658112&amp;s:stream:type=vod&amp;l:stream:startup_time=0&amp;l:stream:fps=0&amp;l:stream:bitrate=0&amp;l:stream:dropped_frames=0</t>
         </is>
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>'s</t>
+          <t>parameter found.</t>
         </is>
       </c>
       <c r="C113" t="inlineStr">
@@ -2903,19 +2903,19 @@
       </c>
       <c r="D113" t="inlineStr">
         <is>
-          <t>Pass: 's:event:type' parameter found with value play. URL: http://foxnews.hb.omtrdc.net/?s:sc:rsid=foxnewsglobalproduction&amp;s:sc:tracking_server=smetrics.foxnews.com&amp;h:sc:ssl=1&amp;s:user:mid=69099319612994832056547930341105758682&amp;&amp;&amp;s:sp:ovp=Akamai&amp;s:sp:channel=Fox+News&amp;s:sp:player_name=Fox+News+Android+Player&amp;s:sp:hb_version=android-2.1.0.154-42fb90&amp;l:sp:hb_api_lvl=4&amp;s:event:sid=1673312989776217636246&amp;l:event:duration=0&amp;l:event:playhead=227&amp;l:event:prev_ts=-1&amp;s:event:type=play&amp;l:event:ts=1673312994087&amp;s:asset:name=Biden+accused+of+mishandling+classified+documents&amp;l:asset:length=200&amp;s:asset:publisher=foxnews&amp;s:asset:type=main&amp;s:asset:video_id=6318425658112&amp;s:stream:type=vod&amp;l:stream:startup_time=0&amp;l:stream:fps=0&amp;l:stream:bitrate=0&amp;l:stream:dropped_frames=0.</t>
+          <t>Pass: 's:asset:type' parameter found.</t>
         </is>
       </c>
     </row>
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>http://foxnews.hb.omtrdc.net/?s:sc:rsid=foxnewsglobalproduction&amp;s:sc:tracking_server=smetrics.foxnews.com&amp;h:sc:ssl=1&amp;s:user:mid=69099319612994832056547930341105758682&amp;&amp;&amp;s:sp:ovp=Akamai&amp;s:sp:channel=Fox+News&amp;s:sp:player_name=Fox+News+Android+Player&amp;s:sp:hb_version=android-2.1.0.154-42fb90&amp;l:sp:hb_api_lvl=4&amp;s:event:sid=1673312989776217636246&amp;l:event:duration=0&amp;l:event:playhead=227&amp;l:event:prev_ts=-1&amp;s:event:type=play&amp;l:event:ts=1673312994087&amp;s:asset:name=Biden+accused+of+mishandling+classified+documents&amp;l:asset:length=200&amp;s:asset:publisher=foxnews&amp;s:asset:type=main&amp;s:asset:video_id=6318425658112&amp;s:stream:type=vod&amp;l:stream:startup_time=0&amp;l:stream:fps=0&amp;l:stream:bitrate=0&amp;l:stream:dropped_frames=0</t>
+          <t>http://foxnews.hb.omtrdc.net/?s:sc:rsid=foxnewsglobalproduction&amp;s:sc:tracking_server=smetrics.foxnews.com&amp;h:sc:ssl=1&amp;s:user:mid=69099319612994832056547930341105758682&amp;&amp;&amp;s:sp:ovp=Akamai&amp;s:sp:channel=Fox+News&amp;s:sp:player_name=Fox+News+Android+Player&amp;s:sp:hb_version=android-2.1.0.154-42fb90&amp;l:sp:hb_api_lvl=4&amp;s:event:sid=1673312989776217636246&amp;l:event:duration=338&amp;l:event:playhead=227&amp;l:event:prev_ts=-1&amp;s:event:type=pause&amp;l:event:ts=1673312994087&amp;s:asset:name=Biden+accused+of+mishandling+classified+documents&amp;l:asset:length=200&amp;s:asset:publisher=foxnews&amp;s:asset:type=main&amp;s:asset:video_id=6318425658112&amp;s:stream:type=vod&amp;l:stream:startup_time=0&amp;l:stream:fps=0&amp;l:stream:bitrate=0&amp;l:stream:dropped_frames=0</t>
         </is>
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>'s</t>
+          <t>parameter found with value foxnewsglobalproduction. URL: http://foxnews.hb.omtrdc.net/?s:sc:rsid=foxnewsglobalproduction&amp;s:sc:tracking_server=smetrics.foxnews.com&amp;h:sc:ssl=1&amp;s:user:mid=69099319612994832056547930341105758682&amp;&amp;&amp;s:sp:ovp=Akamai&amp;s:sp:channel=Fox+News&amp;s:sp:player_name=Fox+News+Android+Player&amp;s:sp:hb_version=android-2.1.0.154-42fb90&amp;l:sp:hb_api_lvl=4&amp;s:event:sid=1673312989776217636246&amp;l:event:duration=338&amp;l:event:playhead=227&amp;l:event:prev_ts=-1&amp;s:event:type=pause&amp;l:event:ts=1673312994087&amp;s:asset:name=Biden+accused+of+mishandling+classified+documents&amp;l:asset:length=200&amp;s:asset:publisher=foxnews&amp;s:asset:type=main&amp;s:asset:video_id=6318425658112&amp;s:stream:type=vod&amp;l:stream:startup_time=0&amp;l:stream:fps=0&amp;l:stream:bitrate=0&amp;l:stream:dropped_frames=0.</t>
         </is>
       </c>
       <c r="C114" t="inlineStr">
@@ -2925,7 +2925,7 @@
       </c>
       <c r="D114" t="inlineStr">
         <is>
-          <t>Pass: 's:event:sid' parameter found. URL: http://foxnews.hb.omtrdc.net/?s:sc:rsid=foxnewsglobalproduction&amp;s:sc:tracking_server=smetrics.foxnews.com&amp;h:sc:ssl=1&amp;s:user:mid=69099319612994832056547930341105758682&amp;&amp;&amp;s:sp:ovp=Akamai&amp;s:sp:channel=Fox+News&amp;s:sp:player_name=Fox+News+Android+Player&amp;s:sp:hb_version=android-2.1.0.154-42fb90&amp;l:sp:hb_api_lvl=4&amp;s:event:sid=1673312989776217636246&amp;l:event:duration=0&amp;l:event:playhead=227&amp;l:event:prev_ts=-1&amp;s:event:type=play&amp;l:event:ts=1673312994087&amp;s:asset:name=Biden+accused+of+mishandling+classified+documents&amp;l:asset:length=200&amp;s:asset:publisher=foxnews&amp;s:asset:type=main&amp;s:asset:video_id=6318425658112&amp;s:stream:type=vod&amp;l:stream:startup_time=0&amp;l:stream:fps=0&amp;l:stream:bitrate=0&amp;l:stream:dropped_frames=0.</t>
+          <t>Pass: 's:sc:rsid' parameter found with value foxnewsglobalproduction. URL: http://foxnews.hb.omtrdc.net/?s:sc:rsid=foxnewsglobalproduction&amp;s:sc:tracking_server=smetrics.foxnews.com&amp;h:sc:ssl=1&amp;s:user:mid=69099319612994832056547930341105758682&amp;&amp;&amp;s:sp:ovp=Akamai&amp;s:sp:channel=Fox+News&amp;s:sp:player_name=Fox+News+Android+Player&amp;s:sp:hb_version=android-2.1.0.154-42fb90&amp;l:sp:hb_api_lvl=4&amp;s:event:sid=1673312989776217636246&amp;l:event:duration=338&amp;l:event:playhead=227&amp;l:event:prev_ts=-1&amp;s:event:type=pause&amp;l:event:ts=1673312994087&amp;s:asset:name=Biden+accused+of+mishandling+classified+documents&amp;l:asset:length=200&amp;s:asset:publisher=foxnews&amp;s:asset:type=main&amp;s:asset:video_id=6318425658112&amp;s:stream:type=vod&amp;l:stream:startup_time=0&amp;l:stream:fps=0&amp;l:stream:bitrate=0&amp;l:stream:dropped_frames=0.</t>
         </is>
       </c>
     </row>
@@ -2937,7 +2937,7 @@
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>'l</t>
+          <t>parameter found with value play. URL: http://foxnews.hb.omtrdc.net/?s:sc:rsid=foxnewsglobalproduction&amp;s:sc:tracking_server=smetrics.foxnews.com&amp;h:sc:ssl=1&amp;s:user:mid=69099319612994832056547930341105758682&amp;&amp;&amp;s:sp:ovp=Akamai&amp;s:sp:channel=Fox+News&amp;s:sp:player_name=Fox+News+Android+Player&amp;s:sp:hb_version=android-2.1.0.154-42fb90&amp;l:sp:hb_api_lvl=4&amp;s:event:sid=1673312989776217636246&amp;l:event:duration=0&amp;l:event:playhead=227&amp;l:event:prev_ts=-1&amp;s:event:type=play&amp;l:event:ts=1673312994087&amp;s:asset:name=Biden+accused+of+mishandling+classified+documents&amp;l:asset:length=200&amp;s:asset:publisher=foxnews&amp;s:asset:type=main&amp;s:asset:video_id=6318425658112&amp;s:stream:type=vod&amp;l:stream:startup_time=0&amp;l:stream:fps=0&amp;l:stream:bitrate=0&amp;l:stream:dropped_frames=0.</t>
         </is>
       </c>
       <c r="C115" t="inlineStr">
@@ -2947,7 +2947,7 @@
       </c>
       <c r="D115" t="inlineStr">
         <is>
-          <t>Pass: 'l:event:duration' parameter found.</t>
+          <t>Pass: 's:event:type' parameter found with value play. URL: http://foxnews.hb.omtrdc.net/?s:sc:rsid=foxnewsglobalproduction&amp;s:sc:tracking_server=smetrics.foxnews.com&amp;h:sc:ssl=1&amp;s:user:mid=69099319612994832056547930341105758682&amp;&amp;&amp;s:sp:ovp=Akamai&amp;s:sp:channel=Fox+News&amp;s:sp:player_name=Fox+News+Android+Player&amp;s:sp:hb_version=android-2.1.0.154-42fb90&amp;l:sp:hb_api_lvl=4&amp;s:event:sid=1673312989776217636246&amp;l:event:duration=0&amp;l:event:playhead=227&amp;l:event:prev_ts=-1&amp;s:event:type=play&amp;l:event:ts=1673312994087&amp;s:asset:name=Biden+accused+of+mishandling+classified+documents&amp;l:asset:length=200&amp;s:asset:publisher=foxnews&amp;s:asset:type=main&amp;s:asset:video_id=6318425658112&amp;s:stream:type=vod&amp;l:stream:startup_time=0&amp;l:stream:fps=0&amp;l:stream:bitrate=0&amp;l:stream:dropped_frames=0.</t>
         </is>
       </c>
     </row>
@@ -2959,7 +2959,7 @@
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>'l</t>
+          <t>parameter found with value play. URL: http://foxnews.hb.omtrdc.net/?s:sc:rsid=foxnewsglobalproduction&amp;s:sc:tracking_server=smetrics.foxnews.com&amp;h:sc:ssl=1&amp;s:user:mid=69099319612994832056547930341105758682&amp;&amp;&amp;s:sp:ovp=Akamai&amp;s:sp:channel=Fox+News&amp;s:sp:player_name=Fox+News+Android+Player&amp;s:sp:hb_version=android-2.1.0.154-42fb90&amp;l:sp:hb_api_lvl=4&amp;s:event:sid=1673312989776217636246&amp;l:event:duration=0&amp;l:event:playhead=227&amp;l:event:prev_ts=-1&amp;s:event:type=play&amp;l:event:ts=1673312994087&amp;s:asset:name=Biden+accused+of+mishandling+classified+documents&amp;l:asset:length=200&amp;s:asset:publisher=foxnews&amp;s:asset:type=main&amp;s:asset:video_id=6318425658112&amp;s:stream:type=vod&amp;l:stream:startup_time=0&amp;l:stream:fps=0&amp;l:stream:bitrate=0&amp;l:stream:dropped_frames=0.</t>
         </is>
       </c>
       <c r="C116" t="inlineStr">
@@ -2969,7 +2969,7 @@
       </c>
       <c r="D116" t="inlineStr">
         <is>
-          <t>Pass: 'l:event:playhead' parameter found.</t>
+          <t>Pass: 's:event:type' parameter found with value play. URL: http://foxnews.hb.omtrdc.net/?s:sc:rsid=foxnewsglobalproduction&amp;s:sc:tracking_server=smetrics.foxnews.com&amp;h:sc:ssl=1&amp;s:user:mid=69099319612994832056547930341105758682&amp;&amp;&amp;s:sp:ovp=Akamai&amp;s:sp:channel=Fox+News&amp;s:sp:player_name=Fox+News+Android+Player&amp;s:sp:hb_version=android-2.1.0.154-42fb90&amp;l:sp:hb_api_lvl=4&amp;s:event:sid=1673312989776217636246&amp;l:event:duration=0&amp;l:event:playhead=227&amp;l:event:prev_ts=-1&amp;s:event:type=play&amp;l:event:ts=1673312994087&amp;s:asset:name=Biden+accused+of+mishandling+classified+documents&amp;l:asset:length=200&amp;s:asset:publisher=foxnews&amp;s:asset:type=main&amp;s:asset:video_id=6318425658112&amp;s:stream:type=vod&amp;l:stream:startup_time=0&amp;l:stream:fps=0&amp;l:stream:bitrate=0&amp;l:stream:dropped_frames=0.</t>
         </is>
       </c>
     </row>
@@ -2981,7 +2981,7 @@
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>'l</t>
+          <t>parameter found. URL: http://foxnews.hb.omtrdc.net/?s:sc:rsid=foxnewsglobalproduction&amp;s:sc:tracking_server=smetrics.foxnews.com&amp;h:sc:ssl=1&amp;s:user:mid=69099319612994832056547930341105758682&amp;&amp;&amp;s:sp:ovp=Akamai&amp;s:sp:channel=Fox+News&amp;s:sp:player_name=Fox+News+Android+Player&amp;s:sp:hb_version=android-2.1.0.154-42fb90&amp;l:sp:hb_api_lvl=4&amp;s:event:sid=1673312989776217636246&amp;l:event:duration=0&amp;l:event:playhead=227&amp;l:event:prev_ts=-1&amp;s:event:type=play&amp;l:event:ts=1673312994087&amp;s:asset:name=Biden+accused+of+mishandling+classified+documents&amp;l:asset:length=200&amp;s:asset:publisher=foxnews&amp;s:asset:type=main&amp;s:asset:video_id=6318425658112&amp;s:stream:type=vod&amp;l:stream:startup_time=0&amp;l:stream:fps=0&amp;l:stream:bitrate=0&amp;l:stream:dropped_frames=0.</t>
         </is>
       </c>
       <c r="C117" t="inlineStr">
@@ -2991,7 +2991,7 @@
       </c>
       <c r="D117" t="inlineStr">
         <is>
-          <t>Pass: 'l:event:prev_ts' parameter found.</t>
+          <t>Pass: 's:event:sid' parameter found. URL: http://foxnews.hb.omtrdc.net/?s:sc:rsid=foxnewsglobalproduction&amp;s:sc:tracking_server=smetrics.foxnews.com&amp;h:sc:ssl=1&amp;s:user:mid=69099319612994832056547930341105758682&amp;&amp;&amp;s:sp:ovp=Akamai&amp;s:sp:channel=Fox+News&amp;s:sp:player_name=Fox+News+Android+Player&amp;s:sp:hb_version=android-2.1.0.154-42fb90&amp;l:sp:hb_api_lvl=4&amp;s:event:sid=1673312989776217636246&amp;l:event:duration=0&amp;l:event:playhead=227&amp;l:event:prev_ts=-1&amp;s:event:type=play&amp;l:event:ts=1673312994087&amp;s:asset:name=Biden+accused+of+mishandling+classified+documents&amp;l:asset:length=200&amp;s:asset:publisher=foxnews&amp;s:asset:type=main&amp;s:asset:video_id=6318425658112&amp;s:stream:type=vod&amp;l:stream:startup_time=0&amp;l:stream:fps=0&amp;l:stream:bitrate=0&amp;l:stream:dropped_frames=0.</t>
         </is>
       </c>
     </row>
@@ -3003,7 +3003,7 @@
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>'l</t>
+          <t>parameter found.</t>
         </is>
       </c>
       <c r="C118" t="inlineStr">
@@ -3013,7 +3013,7 @@
       </c>
       <c r="D118" t="inlineStr">
         <is>
-          <t>Pass: 'l:event:ts' parameter found.</t>
+          <t>Pass: 'l:event:duration' parameter found.</t>
         </is>
       </c>
     </row>
@@ -3025,7 +3025,7 @@
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>'s</t>
+          <t>parameter found.</t>
         </is>
       </c>
       <c r="C119" t="inlineStr">
@@ -3035,7 +3035,7 @@
       </c>
       <c r="D119" t="inlineStr">
         <is>
-          <t>Pass: 's:asset:name' parameter found.</t>
+          <t>Pass: 'l:event:prev_ts' parameter found.</t>
         </is>
       </c>
     </row>
@@ -3047,7 +3047,7 @@
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>'l</t>
+          <t>parameter found.</t>
         </is>
       </c>
       <c r="C120" t="inlineStr">
@@ -3057,7 +3057,7 @@
       </c>
       <c r="D120" t="inlineStr">
         <is>
-          <t>Pass: 'l:asset:length' parameter found.</t>
+          <t>Pass: 'l:event:ts' parameter found.</t>
         </is>
       </c>
     </row>
@@ -3069,7 +3069,7 @@
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>'s</t>
+          <t>parameter found.</t>
         </is>
       </c>
       <c r="C121" t="inlineStr">
@@ -3079,7 +3079,7 @@
       </c>
       <c r="D121" t="inlineStr">
         <is>
-          <t>Pass: 's:asset:publisher' parameter found.</t>
+          <t>Pass: 's:asset:name' parameter found.</t>
         </is>
       </c>
     </row>
@@ -3091,7 +3091,7 @@
       </c>
       <c r="B122" t="inlineStr">
         <is>
-          <t>'s</t>
+          <t>parameter found.</t>
         </is>
       </c>
       <c r="C122" t="inlineStr">
@@ -3101,7 +3101,7 @@
       </c>
       <c r="D122" t="inlineStr">
         <is>
-          <t>Pass: 's:asset:type' parameter found.</t>
+          <t>Pass: 'l:asset:length' parameter found.</t>
         </is>
       </c>
     </row>
@@ -3113,7 +3113,7 @@
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t>'s</t>
+          <t>parameter found.</t>
         </is>
       </c>
       <c r="C123" t="inlineStr">
@@ -3123,19 +3123,19 @@
       </c>
       <c r="D123" t="inlineStr">
         <is>
-          <t>Pass: 's:sc:rsid' parameter found with value foxnewsglobalproduction. URL: http://foxnews.hb.omtrdc.net/?s:sc:rsid=foxnewsglobalproduction&amp;s:sc:tracking_server=smetrics.foxnews.com&amp;h:sc:ssl=1&amp;s:user:mid=69099319612994832056547930341105758682&amp;&amp;&amp;s:sp:ovp=Akamai&amp;s:sp:channel=Fox+News&amp;s:sp:player_name=Fox+News+Android+Player&amp;s:sp:hb_version=android-2.1.0.154-42fb90&amp;l:sp:hb_api_lvl=4&amp;s:event:sid=1673312989776217636246&amp;l:event:duration=0&amp;l:event:playhead=227&amp;l:event:prev_ts=-1&amp;s:event:type=play&amp;l:event:ts=1673312994087&amp;s:asset:name=Biden+accused+of+mishandling+classified+documents&amp;l:asset:length=200&amp;s:asset:publisher=foxnews&amp;s:asset:type=main&amp;s:asset:video_id=6318425658112&amp;s:stream:type=vod&amp;l:stream:startup_time=0&amp;l:stream:fps=0&amp;l:stream:bitrate=0&amp;l:stream:dropped_frames=0.</t>
+          <t>Pass: 's:asset:publisher' parameter found.</t>
         </is>
       </c>
     </row>
     <row r="124">
       <c r="A124" t="inlineStr">
         <is>
-          <t>http://foxnews.hb.omtrdc.net/?s:sc:rsid=foxnewsglobalproduction&amp;s:sc:tracking_server=smetrics.foxnews.com&amp;h:sc:ssl=1&amp;s:user:mid=69099319612994832056547930341105758682&amp;&amp;&amp;s:sp:ovp=Akamai&amp;s:sp:channel=Fox+News&amp;s:sp:player_name=Fox+News+Android+Player&amp;s:sp:hb_version=android-2.1.0.154-42fb90&amp;l:sp:hb_api_lvl=4&amp;s:event:sid=1673312989776217636246&amp;l:event:duration=1001&amp;l:event:playhead=1217&amp;l:event:prev_ts=1673312994087&amp;s:event:type=play&amp;l:event:ts=1673312995088&amp;s:asset:name=Biden+accused+of+mishandling+classified+documents&amp;l:asset:length=200&amp;s:asset:publisher=foxnews&amp;s:asset:type=main&amp;s:asset:video_id=6318425658112&amp;s:stream:type=vod&amp;l:stream:startup_time=0&amp;l:stream:fps=0&amp;l:stream:bitrate=0&amp;l:stream:dropped_frames=0</t>
+          <t>http://foxnews.hb.omtrdc.net/?s:sc:rsid=foxnewsglobalproduction&amp;s:sc:tracking_server=smetrics.foxnews.com&amp;h:sc:ssl=1&amp;s:user:mid=69099319612994832056547930341105758682&amp;&amp;&amp;s:sp:ovp=Akamai&amp;s:sp:channel=Fox+News&amp;s:sp:player_name=Fox+News+Android+Player&amp;s:sp:hb_version=android-2.1.0.154-42fb90&amp;l:sp:hb_api_lvl=4&amp;s:event:sid=1673312989776217636246&amp;l:event:duration=0&amp;l:event:playhead=227&amp;l:event:prev_ts=-1&amp;s:event:type=play&amp;l:event:ts=1673312994087&amp;s:asset:name=Biden+accused+of+mishandling+classified+documents&amp;l:asset:length=200&amp;s:asset:publisher=foxnews&amp;s:asset:type=main&amp;s:asset:video_id=6318425658112&amp;s:stream:type=vod&amp;l:stream:startup_time=0&amp;l:stream:fps=0&amp;l:stream:bitrate=0&amp;l:stream:dropped_frames=0</t>
         </is>
       </c>
       <c r="B124" t="inlineStr">
         <is>
-          <t>'s</t>
+          <t>parameter found.</t>
         </is>
       </c>
       <c r="C124" t="inlineStr">
@@ -3145,19 +3145,19 @@
       </c>
       <c r="D124" t="inlineStr">
         <is>
-          <t>Pass: 's:event:type' parameter found with value play. URL: http://foxnews.hb.omtrdc.net/?s:sc:rsid=foxnewsglobalproduction&amp;s:sc:tracking_server=smetrics.foxnews.com&amp;h:sc:ssl=1&amp;s:user:mid=69099319612994832056547930341105758682&amp;&amp;&amp;s:sp:ovp=Akamai&amp;s:sp:channel=Fox+News&amp;s:sp:player_name=Fox+News+Android+Player&amp;s:sp:hb_version=android-2.1.0.154-42fb90&amp;l:sp:hb_api_lvl=4&amp;s:event:sid=1673312989776217636246&amp;l:event:duration=1001&amp;l:event:playhead=1217&amp;l:event:prev_ts=1673312994087&amp;s:event:type=play&amp;l:event:ts=1673312995088&amp;s:asset:name=Biden+accused+of+mishandling+classified+documents&amp;l:asset:length=200&amp;s:asset:publisher=foxnews&amp;s:asset:type=main&amp;s:asset:video_id=6318425658112&amp;s:stream:type=vod&amp;l:stream:startup_time=0&amp;l:stream:fps=0&amp;l:stream:bitrate=0&amp;l:stream:dropped_frames=0.</t>
+          <t>Pass: 's:asset:type' parameter found.</t>
         </is>
       </c>
     </row>
     <row r="125">
       <c r="A125" t="inlineStr">
         <is>
-          <t>http://foxnews.hb.omtrdc.net/?s:sc:rsid=foxnewsglobalproduction&amp;s:sc:tracking_server=smetrics.foxnews.com&amp;h:sc:ssl=1&amp;s:user:mid=69099319612994832056547930341105758682&amp;&amp;&amp;s:sp:ovp=Akamai&amp;s:sp:channel=Fox+News&amp;s:sp:player_name=Fox+News+Android+Player&amp;s:sp:hb_version=android-2.1.0.154-42fb90&amp;l:sp:hb_api_lvl=4&amp;s:event:sid=1673312989776217636246&amp;l:event:duration=1001&amp;l:event:playhead=1217&amp;l:event:prev_ts=1673312994087&amp;s:event:type=play&amp;l:event:ts=1673312995088&amp;s:asset:name=Biden+accused+of+mishandling+classified+documents&amp;l:asset:length=200&amp;s:asset:publisher=foxnews&amp;s:asset:type=main&amp;s:asset:video_id=6318425658112&amp;s:stream:type=vod&amp;l:stream:startup_time=0&amp;l:stream:fps=0&amp;l:stream:bitrate=0&amp;l:stream:dropped_frames=0</t>
+          <t>http://foxnews.hb.omtrdc.net/?s:sc:rsid=foxnewsglobalproduction&amp;s:sc:tracking_server=smetrics.foxnews.com&amp;h:sc:ssl=1&amp;s:user:mid=69099319612994832056547930341105758682&amp;&amp;&amp;s:sp:ovp=Akamai&amp;s:sp:channel=Fox+News&amp;s:sp:player_name=Fox+News+Android+Player&amp;s:sp:hb_version=android-2.1.0.154-42fb90&amp;l:sp:hb_api_lvl=4&amp;s:event:sid=1673312989776217636246&amp;l:event:duration=0&amp;l:event:playhead=227&amp;l:event:prev_ts=-1&amp;s:event:type=play&amp;l:event:ts=1673312994087&amp;s:asset:name=Biden+accused+of+mishandling+classified+documents&amp;l:asset:length=200&amp;s:asset:publisher=foxnews&amp;s:asset:type=main&amp;s:asset:video_id=6318425658112&amp;s:stream:type=vod&amp;l:stream:startup_time=0&amp;l:stream:fps=0&amp;l:stream:bitrate=0&amp;l:stream:dropped_frames=0</t>
         </is>
       </c>
       <c r="B125" t="inlineStr">
         <is>
-          <t>'s</t>
+          <t>parameter found with value foxnewsglobalproduction. URL: http://foxnews.hb.omtrdc.net/?s:sc:rsid=foxnewsglobalproduction&amp;s:sc:tracking_server=smetrics.foxnews.com&amp;h:sc:ssl=1&amp;s:user:mid=69099319612994832056547930341105758682&amp;&amp;&amp;s:sp:ovp=Akamai&amp;s:sp:channel=Fox+News&amp;s:sp:player_name=Fox+News+Android+Player&amp;s:sp:hb_version=android-2.1.0.154-42fb90&amp;l:sp:hb_api_lvl=4&amp;s:event:sid=1673312989776217636246&amp;l:event:duration=0&amp;l:event:playhead=227&amp;l:event:prev_ts=-1&amp;s:event:type=play&amp;l:event:ts=1673312994087&amp;s:asset:name=Biden+accused+of+mishandling+classified+documents&amp;l:asset:length=200&amp;s:asset:publisher=foxnews&amp;s:asset:type=main&amp;s:asset:video_id=6318425658112&amp;s:stream:type=vod&amp;l:stream:startup_time=0&amp;l:stream:fps=0&amp;l:stream:bitrate=0&amp;l:stream:dropped_frames=0.</t>
         </is>
       </c>
       <c r="C125" t="inlineStr">
@@ -3167,7 +3167,7 @@
       </c>
       <c r="D125" t="inlineStr">
         <is>
-          <t>Pass: 's:event:sid' parameter found. URL: http://foxnews.hb.omtrdc.net/?s:sc:rsid=foxnewsglobalproduction&amp;s:sc:tracking_server=smetrics.foxnews.com&amp;h:sc:ssl=1&amp;s:user:mid=69099319612994832056547930341105758682&amp;&amp;&amp;s:sp:ovp=Akamai&amp;s:sp:channel=Fox+News&amp;s:sp:player_name=Fox+News+Android+Player&amp;s:sp:hb_version=android-2.1.0.154-42fb90&amp;l:sp:hb_api_lvl=4&amp;s:event:sid=1673312989776217636246&amp;l:event:duration=1001&amp;l:event:playhead=1217&amp;l:event:prev_ts=1673312994087&amp;s:event:type=play&amp;l:event:ts=1673312995088&amp;s:asset:name=Biden+accused+of+mishandling+classified+documents&amp;l:asset:length=200&amp;s:asset:publisher=foxnews&amp;s:asset:type=main&amp;s:asset:video_id=6318425658112&amp;s:stream:type=vod&amp;l:stream:startup_time=0&amp;l:stream:fps=0&amp;l:stream:bitrate=0&amp;l:stream:dropped_frames=0.</t>
+          <t>Pass: 's:sc:rsid' parameter found with value foxnewsglobalproduction. URL: http://foxnews.hb.omtrdc.net/?s:sc:rsid=foxnewsglobalproduction&amp;s:sc:tracking_server=smetrics.foxnews.com&amp;h:sc:ssl=1&amp;s:user:mid=69099319612994832056547930341105758682&amp;&amp;&amp;s:sp:ovp=Akamai&amp;s:sp:channel=Fox+News&amp;s:sp:player_name=Fox+News+Android+Player&amp;s:sp:hb_version=android-2.1.0.154-42fb90&amp;l:sp:hb_api_lvl=4&amp;s:event:sid=1673312989776217636246&amp;l:event:duration=0&amp;l:event:playhead=227&amp;l:event:prev_ts=-1&amp;s:event:type=play&amp;l:event:ts=1673312994087&amp;s:asset:name=Biden+accused+of+mishandling+classified+documents&amp;l:asset:length=200&amp;s:asset:publisher=foxnews&amp;s:asset:type=main&amp;s:asset:video_id=6318425658112&amp;s:stream:type=vod&amp;l:stream:startup_time=0&amp;l:stream:fps=0&amp;l:stream:bitrate=0&amp;l:stream:dropped_frames=0.</t>
         </is>
       </c>
     </row>
@@ -3179,7 +3179,7 @@
       </c>
       <c r="B126" t="inlineStr">
         <is>
-          <t>'l</t>
+          <t>parameter found with value play. URL: http://foxnews.hb.omtrdc.net/?s:sc:rsid=foxnewsglobalproduction&amp;s:sc:tracking_server=smetrics.foxnews.com&amp;h:sc:ssl=1&amp;s:user:mid=69099319612994832056547930341105758682&amp;&amp;&amp;s:sp:ovp=Akamai&amp;s:sp:channel=Fox+News&amp;s:sp:player_name=Fox+News+Android+Player&amp;s:sp:hb_version=android-2.1.0.154-42fb90&amp;l:sp:hb_api_lvl=4&amp;s:event:sid=1673312989776217636246&amp;l:event:duration=1001&amp;l:event:playhead=1217&amp;l:event:prev_ts=1673312994087&amp;s:event:type=play&amp;l:event:ts=1673312995088&amp;s:asset:name=Biden+accused+of+mishandling+classified+documents&amp;l:asset:length=200&amp;s:asset:publisher=foxnews&amp;s:asset:type=main&amp;s:asset:video_id=6318425658112&amp;s:stream:type=vod&amp;l:stream:startup_time=0&amp;l:stream:fps=0&amp;l:stream:bitrate=0&amp;l:stream:dropped_frames=0.</t>
         </is>
       </c>
       <c r="C126" t="inlineStr">
@@ -3189,7 +3189,7 @@
       </c>
       <c r="D126" t="inlineStr">
         <is>
-          <t>Pass: 'l:event:duration' parameter found.</t>
+          <t>Pass: 's:event:type' parameter found with value play. URL: http://foxnews.hb.omtrdc.net/?s:sc:rsid=foxnewsglobalproduction&amp;s:sc:tracking_server=smetrics.foxnews.com&amp;h:sc:ssl=1&amp;s:user:mid=69099319612994832056547930341105758682&amp;&amp;&amp;s:sp:ovp=Akamai&amp;s:sp:channel=Fox+News&amp;s:sp:player_name=Fox+News+Android+Player&amp;s:sp:hb_version=android-2.1.0.154-42fb90&amp;l:sp:hb_api_lvl=4&amp;s:event:sid=1673312989776217636246&amp;l:event:duration=1001&amp;l:event:playhead=1217&amp;l:event:prev_ts=1673312994087&amp;s:event:type=play&amp;l:event:ts=1673312995088&amp;s:asset:name=Biden+accused+of+mishandling+classified+documents&amp;l:asset:length=200&amp;s:asset:publisher=foxnews&amp;s:asset:type=main&amp;s:asset:video_id=6318425658112&amp;s:stream:type=vod&amp;l:stream:startup_time=0&amp;l:stream:fps=0&amp;l:stream:bitrate=0&amp;l:stream:dropped_frames=0.</t>
         </is>
       </c>
     </row>
@@ -3201,7 +3201,7 @@
       </c>
       <c r="B127" t="inlineStr">
         <is>
-          <t>'l</t>
+          <t>parameter found with value play. URL: http://foxnews.hb.omtrdc.net/?s:sc:rsid=foxnewsglobalproduction&amp;s:sc:tracking_server=smetrics.foxnews.com&amp;h:sc:ssl=1&amp;s:user:mid=69099319612994832056547930341105758682&amp;&amp;&amp;s:sp:ovp=Akamai&amp;s:sp:channel=Fox+News&amp;s:sp:player_name=Fox+News+Android+Player&amp;s:sp:hb_version=android-2.1.0.154-42fb90&amp;l:sp:hb_api_lvl=4&amp;s:event:sid=1673312989776217636246&amp;l:event:duration=1001&amp;l:event:playhead=1217&amp;l:event:prev_ts=1673312994087&amp;s:event:type=play&amp;l:event:ts=1673312995088&amp;s:asset:name=Biden+accused+of+mishandling+classified+documents&amp;l:asset:length=200&amp;s:asset:publisher=foxnews&amp;s:asset:type=main&amp;s:asset:video_id=6318425658112&amp;s:stream:type=vod&amp;l:stream:startup_time=0&amp;l:stream:fps=0&amp;l:stream:bitrate=0&amp;l:stream:dropped_frames=0.</t>
         </is>
       </c>
       <c r="C127" t="inlineStr">
@@ -3211,7 +3211,7 @@
       </c>
       <c r="D127" t="inlineStr">
         <is>
-          <t>Pass: 'l:event:playhead' parameter found.</t>
+          <t>Pass: 's:event:type' parameter found with value play. URL: http://foxnews.hb.omtrdc.net/?s:sc:rsid=foxnewsglobalproduction&amp;s:sc:tracking_server=smetrics.foxnews.com&amp;h:sc:ssl=1&amp;s:user:mid=69099319612994832056547930341105758682&amp;&amp;&amp;s:sp:ovp=Akamai&amp;s:sp:channel=Fox+News&amp;s:sp:player_name=Fox+News+Android+Player&amp;s:sp:hb_version=android-2.1.0.154-42fb90&amp;l:sp:hb_api_lvl=4&amp;s:event:sid=1673312989776217636246&amp;l:event:duration=1001&amp;l:event:playhead=1217&amp;l:event:prev_ts=1673312994087&amp;s:event:type=play&amp;l:event:ts=1673312995088&amp;s:asset:name=Biden+accused+of+mishandling+classified+documents&amp;l:asset:length=200&amp;s:asset:publisher=foxnews&amp;s:asset:type=main&amp;s:asset:video_id=6318425658112&amp;s:stream:type=vod&amp;l:stream:startup_time=0&amp;l:stream:fps=0&amp;l:stream:bitrate=0&amp;l:stream:dropped_frames=0.</t>
         </is>
       </c>
     </row>
@@ -3223,7 +3223,7 @@
       </c>
       <c r="B128" t="inlineStr">
         <is>
-          <t>'l</t>
+          <t>parameter found. URL: http://foxnews.hb.omtrdc.net/?s:sc:rsid=foxnewsglobalproduction&amp;s:sc:tracking_server=smetrics.foxnews.com&amp;h:sc:ssl=1&amp;s:user:mid=69099319612994832056547930341105758682&amp;&amp;&amp;s:sp:ovp=Akamai&amp;s:sp:channel=Fox+News&amp;s:sp:player_name=Fox+News+Android+Player&amp;s:sp:hb_version=android-2.1.0.154-42fb90&amp;l:sp:hb_api_lvl=4&amp;s:event:sid=1673312989776217636246&amp;l:event:duration=1001&amp;l:event:playhead=1217&amp;l:event:prev_ts=1673312994087&amp;s:event:type=play&amp;l:event:ts=1673312995088&amp;s:asset:name=Biden+accused+of+mishandling+classified+documents&amp;l:asset:length=200&amp;s:asset:publisher=foxnews&amp;s:asset:type=main&amp;s:asset:video_id=6318425658112&amp;s:stream:type=vod&amp;l:stream:startup_time=0&amp;l:stream:fps=0&amp;l:stream:bitrate=0&amp;l:stream:dropped_frames=0.</t>
         </is>
       </c>
       <c r="C128" t="inlineStr">
@@ -3233,7 +3233,7 @@
       </c>
       <c r="D128" t="inlineStr">
         <is>
-          <t>Pass: 'l:event:prev_ts' parameter found.</t>
+          <t>Pass: 's:event:sid' parameter found. URL: http://foxnews.hb.omtrdc.net/?s:sc:rsid=foxnewsglobalproduction&amp;s:sc:tracking_server=smetrics.foxnews.com&amp;h:sc:ssl=1&amp;s:user:mid=69099319612994832056547930341105758682&amp;&amp;&amp;s:sp:ovp=Akamai&amp;s:sp:channel=Fox+News&amp;s:sp:player_name=Fox+News+Android+Player&amp;s:sp:hb_version=android-2.1.0.154-42fb90&amp;l:sp:hb_api_lvl=4&amp;s:event:sid=1673312989776217636246&amp;l:event:duration=1001&amp;l:event:playhead=1217&amp;l:event:prev_ts=1673312994087&amp;s:event:type=play&amp;l:event:ts=1673312995088&amp;s:asset:name=Biden+accused+of+mishandling+classified+documents&amp;l:asset:length=200&amp;s:asset:publisher=foxnews&amp;s:asset:type=main&amp;s:asset:video_id=6318425658112&amp;s:stream:type=vod&amp;l:stream:startup_time=0&amp;l:stream:fps=0&amp;l:stream:bitrate=0&amp;l:stream:dropped_frames=0.</t>
         </is>
       </c>
     </row>
@@ -3245,7 +3245,7 @@
       </c>
       <c r="B129" t="inlineStr">
         <is>
-          <t>'l</t>
+          <t>parameter found.</t>
         </is>
       </c>
       <c r="C129" t="inlineStr">
@@ -3255,7 +3255,7 @@
       </c>
       <c r="D129" t="inlineStr">
         <is>
-          <t>Pass: 'l:event:ts' parameter found.</t>
+          <t>Pass: 'l:event:duration' parameter found.</t>
         </is>
       </c>
     </row>
@@ -3267,7 +3267,7 @@
       </c>
       <c r="B130" t="inlineStr">
         <is>
-          <t>'s</t>
+          <t>parameter found.</t>
         </is>
       </c>
       <c r="C130" t="inlineStr">
@@ -3277,7 +3277,7 @@
       </c>
       <c r="D130" t="inlineStr">
         <is>
-          <t>Pass: 's:asset:name' parameter found.</t>
+          <t>Pass: 'l:event:prev_ts' parameter found.</t>
         </is>
       </c>
     </row>
@@ -3289,7 +3289,7 @@
       </c>
       <c r="B131" t="inlineStr">
         <is>
-          <t>'l</t>
+          <t>parameter found.</t>
         </is>
       </c>
       <c r="C131" t="inlineStr">
@@ -3299,7 +3299,7 @@
       </c>
       <c r="D131" t="inlineStr">
         <is>
-          <t>Pass: 'l:asset:length' parameter found.</t>
+          <t>Pass: 'l:event:ts' parameter found.</t>
         </is>
       </c>
     </row>
@@ -3311,7 +3311,7 @@
       </c>
       <c r="B132" t="inlineStr">
         <is>
-          <t>'s</t>
+          <t>parameter found.</t>
         </is>
       </c>
       <c r="C132" t="inlineStr">
@@ -3321,7 +3321,7 @@
       </c>
       <c r="D132" t="inlineStr">
         <is>
-          <t>Pass: 's:asset:publisher' parameter found.</t>
+          <t>Pass: 's:asset:name' parameter found.</t>
         </is>
       </c>
     </row>
@@ -3333,7 +3333,7 @@
       </c>
       <c r="B133" t="inlineStr">
         <is>
-          <t>'s</t>
+          <t>parameter found.</t>
         </is>
       </c>
       <c r="C133" t="inlineStr">
@@ -3343,7 +3343,7 @@
       </c>
       <c r="D133" t="inlineStr">
         <is>
-          <t>Pass: 's:asset:type' parameter found.</t>
+          <t>Pass: 'l:asset:length' parameter found.</t>
         </is>
       </c>
     </row>
@@ -3355,7 +3355,7 @@
       </c>
       <c r="B134" t="inlineStr">
         <is>
-          <t>'s</t>
+          <t>parameter found.</t>
         </is>
       </c>
       <c r="C134" t="inlineStr">
@@ -3365,19 +3365,19 @@
       </c>
       <c r="D134" t="inlineStr">
         <is>
-          <t>Pass: 's:sc:rsid' parameter found with value foxnewsglobalproduction. URL: http://foxnews.hb.omtrdc.net/?s:sc:rsid=foxnewsglobalproduction&amp;s:sc:tracking_server=smetrics.foxnews.com&amp;h:sc:ssl=1&amp;s:user:mid=69099319612994832056547930341105758682&amp;&amp;&amp;s:sp:ovp=Akamai&amp;s:sp:channel=Fox+News&amp;s:sp:player_name=Fox+News+Android+Player&amp;s:sp:hb_version=android-2.1.0.154-42fb90&amp;l:sp:hb_api_lvl=4&amp;s:event:sid=1673312989776217636246&amp;l:event:duration=1001&amp;l:event:playhead=1217&amp;l:event:prev_ts=1673312994087&amp;s:event:type=play&amp;l:event:ts=1673312995088&amp;s:asset:name=Biden+accused+of+mishandling+classified+documents&amp;l:asset:length=200&amp;s:asset:publisher=foxnews&amp;s:asset:type=main&amp;s:asset:video_id=6318425658112&amp;s:stream:type=vod&amp;l:stream:startup_time=0&amp;l:stream:fps=0&amp;l:stream:bitrate=0&amp;l:stream:dropped_frames=0.</t>
+          <t>Pass: 's:asset:publisher' parameter found.</t>
         </is>
       </c>
     </row>
     <row r="135">
       <c r="A135" t="inlineStr">
         <is>
-          <t>http://foxnews.hb.omtrdc.net/?s:sc:rsid=foxnewsglobalproduction&amp;s:sc:tracking_server=smetrics.foxnews.com&amp;h:sc:ssl=1&amp;s:user:mid=69099319612994832056547930341105758682&amp;&amp;&amp;s:sp:ovp=Akamai&amp;s:sp:channel=Fox+News&amp;s:sp:player_name=Fox+News+Android+Player&amp;s:sp:hb_version=android-2.1.0.154-42fb90&amp;l:sp:hb_api_lvl=4&amp;s:event:sid=1673312989776217636246&amp;l:event:duration=9892&amp;l:event:playhead=11124&amp;l:event:prev_ts=1673312995088&amp;s:event:type=play&amp;l:event:ts=1673313004980&amp;s:asset:name=Biden+accused+of+mishandling+classified+documents&amp;l:asset:length=200&amp;s:asset:publisher=foxnews&amp;s:asset:type=main&amp;s:asset:video_id=6318425658112&amp;s:stream:type=vod&amp;l:stream:startup_time=0&amp;l:stream:fps=0&amp;l:stream:bitrate=0&amp;l:stream:dropped_frames=0</t>
+          <t>http://foxnews.hb.omtrdc.net/?s:sc:rsid=foxnewsglobalproduction&amp;s:sc:tracking_server=smetrics.foxnews.com&amp;h:sc:ssl=1&amp;s:user:mid=69099319612994832056547930341105758682&amp;&amp;&amp;s:sp:ovp=Akamai&amp;s:sp:channel=Fox+News&amp;s:sp:player_name=Fox+News+Android+Player&amp;s:sp:hb_version=android-2.1.0.154-42fb90&amp;l:sp:hb_api_lvl=4&amp;s:event:sid=1673312989776217636246&amp;l:event:duration=1001&amp;l:event:playhead=1217&amp;l:event:prev_ts=1673312994087&amp;s:event:type=play&amp;l:event:ts=1673312995088&amp;s:asset:name=Biden+accused+of+mishandling+classified+documents&amp;l:asset:length=200&amp;s:asset:publisher=foxnews&amp;s:asset:type=main&amp;s:asset:video_id=6318425658112&amp;s:stream:type=vod&amp;l:stream:startup_time=0&amp;l:stream:fps=0&amp;l:stream:bitrate=0&amp;l:stream:dropped_frames=0</t>
         </is>
       </c>
       <c r="B135" t="inlineStr">
         <is>
-          <t>'s</t>
+          <t>parameter found.</t>
         </is>
       </c>
       <c r="C135" t="inlineStr">
@@ -3387,19 +3387,19 @@
       </c>
       <c r="D135" t="inlineStr">
         <is>
-          <t>Pass: 's:event:type' parameter found with value play. URL: http://foxnews.hb.omtrdc.net/?s:sc:rsid=foxnewsglobalproduction&amp;s:sc:tracking_server=smetrics.foxnews.com&amp;h:sc:ssl=1&amp;s:user:mid=69099319612994832056547930341105758682&amp;&amp;&amp;s:sp:ovp=Akamai&amp;s:sp:channel=Fox+News&amp;s:sp:player_name=Fox+News+Android+Player&amp;s:sp:hb_version=android-2.1.0.154-42fb90&amp;l:sp:hb_api_lvl=4&amp;s:event:sid=1673312989776217636246&amp;l:event:duration=9892&amp;l:event:playhead=11124&amp;l:event:prev_ts=1673312995088&amp;s:event:type=play&amp;l:event:ts=1673313004980&amp;s:asset:name=Biden+accused+of+mishandling+classified+documents&amp;l:asset:length=200&amp;s:asset:publisher=foxnews&amp;s:asset:type=main&amp;s:asset:video_id=6318425658112&amp;s:stream:type=vod&amp;l:stream:startup_time=0&amp;l:stream:fps=0&amp;l:stream:bitrate=0&amp;l:stream:dropped_frames=0.</t>
+          <t>Pass: 's:asset:type' parameter found.</t>
         </is>
       </c>
     </row>
     <row r="136">
       <c r="A136" t="inlineStr">
         <is>
-          <t>http://foxnews.hb.omtrdc.net/?s:sc:rsid=foxnewsglobalproduction&amp;s:sc:tracking_server=smetrics.foxnews.com&amp;h:sc:ssl=1&amp;s:user:mid=69099319612994832056547930341105758682&amp;&amp;&amp;s:sp:ovp=Akamai&amp;s:sp:channel=Fox+News&amp;s:sp:player_name=Fox+News+Android+Player&amp;s:sp:hb_version=android-2.1.0.154-42fb90&amp;l:sp:hb_api_lvl=4&amp;s:event:sid=1673312989776217636246&amp;l:event:duration=9892&amp;l:event:playhead=11124&amp;l:event:prev_ts=1673312995088&amp;s:event:type=play&amp;l:event:ts=1673313004980&amp;s:asset:name=Biden+accused+of+mishandling+classified+documents&amp;l:asset:length=200&amp;s:asset:publisher=foxnews&amp;s:asset:type=main&amp;s:asset:video_id=6318425658112&amp;s:stream:type=vod&amp;l:stream:startup_time=0&amp;l:stream:fps=0&amp;l:stream:bitrate=0&amp;l:stream:dropped_frames=0</t>
+          <t>http://foxnews.hb.omtrdc.net/?s:sc:rsid=foxnewsglobalproduction&amp;s:sc:tracking_server=smetrics.foxnews.com&amp;h:sc:ssl=1&amp;s:user:mid=69099319612994832056547930341105758682&amp;&amp;&amp;s:sp:ovp=Akamai&amp;s:sp:channel=Fox+News&amp;s:sp:player_name=Fox+News+Android+Player&amp;s:sp:hb_version=android-2.1.0.154-42fb90&amp;l:sp:hb_api_lvl=4&amp;s:event:sid=1673312989776217636246&amp;l:event:duration=1001&amp;l:event:playhead=1217&amp;l:event:prev_ts=1673312994087&amp;s:event:type=play&amp;l:event:ts=1673312995088&amp;s:asset:name=Biden+accused+of+mishandling+classified+documents&amp;l:asset:length=200&amp;s:asset:publisher=foxnews&amp;s:asset:type=main&amp;s:asset:video_id=6318425658112&amp;s:stream:type=vod&amp;l:stream:startup_time=0&amp;l:stream:fps=0&amp;l:stream:bitrate=0&amp;l:stream:dropped_frames=0</t>
         </is>
       </c>
       <c r="B136" t="inlineStr">
         <is>
-          <t>'s</t>
+          <t>parameter found with value foxnewsglobalproduction. URL: http://foxnews.hb.omtrdc.net/?s:sc:rsid=foxnewsglobalproduction&amp;s:sc:tracking_server=smetrics.foxnews.com&amp;h:sc:ssl=1&amp;s:user:mid=69099319612994832056547930341105758682&amp;&amp;&amp;s:sp:ovp=Akamai&amp;s:sp:channel=Fox+News&amp;s:sp:player_name=Fox+News+Android+Player&amp;s:sp:hb_version=android-2.1.0.154-42fb90&amp;l:sp:hb_api_lvl=4&amp;s:event:sid=1673312989776217636246&amp;l:event:duration=1001&amp;l:event:playhead=1217&amp;l:event:prev_ts=1673312994087&amp;s:event:type=play&amp;l:event:ts=1673312995088&amp;s:asset:name=Biden+accused+of+mishandling+classified+documents&amp;l:asset:length=200&amp;s:asset:publisher=foxnews&amp;s:asset:type=main&amp;s:asset:video_id=6318425658112&amp;s:stream:type=vod&amp;l:stream:startup_time=0&amp;l:stream:fps=0&amp;l:stream:bitrate=0&amp;l:stream:dropped_frames=0.</t>
         </is>
       </c>
       <c r="C136" t="inlineStr">
@@ -3409,7 +3409,7 @@
       </c>
       <c r="D136" t="inlineStr">
         <is>
-          <t>Pass: 's:event:sid' parameter found. URL: http://foxnews.hb.omtrdc.net/?s:sc:rsid=foxnewsglobalproduction&amp;s:sc:tracking_server=smetrics.foxnews.com&amp;h:sc:ssl=1&amp;s:user:mid=69099319612994832056547930341105758682&amp;&amp;&amp;s:sp:ovp=Akamai&amp;s:sp:channel=Fox+News&amp;s:sp:player_name=Fox+News+Android+Player&amp;s:sp:hb_version=android-2.1.0.154-42fb90&amp;l:sp:hb_api_lvl=4&amp;s:event:sid=1673312989776217636246&amp;l:event:duration=9892&amp;l:event:playhead=11124&amp;l:event:prev_ts=1673312995088&amp;s:event:type=play&amp;l:event:ts=1673313004980&amp;s:asset:name=Biden+accused+of+mishandling+classified+documents&amp;l:asset:length=200&amp;s:asset:publisher=foxnews&amp;s:asset:type=main&amp;s:asset:video_id=6318425658112&amp;s:stream:type=vod&amp;l:stream:startup_time=0&amp;l:stream:fps=0&amp;l:stream:bitrate=0&amp;l:stream:dropped_frames=0.</t>
+          <t>Pass: 's:sc:rsid' parameter found with value foxnewsglobalproduction. URL: http://foxnews.hb.omtrdc.net/?s:sc:rsid=foxnewsglobalproduction&amp;s:sc:tracking_server=smetrics.foxnews.com&amp;h:sc:ssl=1&amp;s:user:mid=69099319612994832056547930341105758682&amp;&amp;&amp;s:sp:ovp=Akamai&amp;s:sp:channel=Fox+News&amp;s:sp:player_name=Fox+News+Android+Player&amp;s:sp:hb_version=android-2.1.0.154-42fb90&amp;l:sp:hb_api_lvl=4&amp;s:event:sid=1673312989776217636246&amp;l:event:duration=1001&amp;l:event:playhead=1217&amp;l:event:prev_ts=1673312994087&amp;s:event:type=play&amp;l:event:ts=1673312995088&amp;s:asset:name=Biden+accused+of+mishandling+classified+documents&amp;l:asset:length=200&amp;s:asset:publisher=foxnews&amp;s:asset:type=main&amp;s:asset:video_id=6318425658112&amp;s:stream:type=vod&amp;l:stream:startup_time=0&amp;l:stream:fps=0&amp;l:stream:bitrate=0&amp;l:stream:dropped_frames=0.</t>
         </is>
       </c>
     </row>
@@ -3421,7 +3421,7 @@
       </c>
       <c r="B137" t="inlineStr">
         <is>
-          <t>'l</t>
+          <t>parameter found with value play. URL: http://foxnews.hb.omtrdc.net/?s:sc:rsid=foxnewsglobalproduction&amp;s:sc:tracking_server=smetrics.foxnews.com&amp;h:sc:ssl=1&amp;s:user:mid=69099319612994832056547930341105758682&amp;&amp;&amp;s:sp:ovp=Akamai&amp;s:sp:channel=Fox+News&amp;s:sp:player_name=Fox+News+Android+Player&amp;s:sp:hb_version=android-2.1.0.154-42fb90&amp;l:sp:hb_api_lvl=4&amp;s:event:sid=1673312989776217636246&amp;l:event:duration=9892&amp;l:event:playhead=11124&amp;l:event:prev_ts=1673312995088&amp;s:event:type=play&amp;l:event:ts=1673313004980&amp;s:asset:name=Biden+accused+of+mishandling+classified+documents&amp;l:asset:length=200&amp;s:asset:publisher=foxnews&amp;s:asset:type=main&amp;s:asset:video_id=6318425658112&amp;s:stream:type=vod&amp;l:stream:startup_time=0&amp;l:stream:fps=0&amp;l:stream:bitrate=0&amp;l:stream:dropped_frames=0.</t>
         </is>
       </c>
       <c r="C137" t="inlineStr">
@@ -3431,7 +3431,7 @@
       </c>
       <c r="D137" t="inlineStr">
         <is>
-          <t>Pass: 'l:event:duration' parameter found.</t>
+          <t>Pass: 's:event:type' parameter found with value play. URL: http://foxnews.hb.omtrdc.net/?s:sc:rsid=foxnewsglobalproduction&amp;s:sc:tracking_server=smetrics.foxnews.com&amp;h:sc:ssl=1&amp;s:user:mid=69099319612994832056547930341105758682&amp;&amp;&amp;s:sp:ovp=Akamai&amp;s:sp:channel=Fox+News&amp;s:sp:player_name=Fox+News+Android+Player&amp;s:sp:hb_version=android-2.1.0.154-42fb90&amp;l:sp:hb_api_lvl=4&amp;s:event:sid=1673312989776217636246&amp;l:event:duration=9892&amp;l:event:playhead=11124&amp;l:event:prev_ts=1673312995088&amp;s:event:type=play&amp;l:event:ts=1673313004980&amp;s:asset:name=Biden+accused+of+mishandling+classified+documents&amp;l:asset:length=200&amp;s:asset:publisher=foxnews&amp;s:asset:type=main&amp;s:asset:video_id=6318425658112&amp;s:stream:type=vod&amp;l:stream:startup_time=0&amp;l:stream:fps=0&amp;l:stream:bitrate=0&amp;l:stream:dropped_frames=0.</t>
         </is>
       </c>
     </row>
@@ -3443,7 +3443,7 @@
       </c>
       <c r="B138" t="inlineStr">
         <is>
-          <t>'l</t>
+          <t>parameter found with value play. URL: http://foxnews.hb.omtrdc.net/?s:sc:rsid=foxnewsglobalproduction&amp;s:sc:tracking_server=smetrics.foxnews.com&amp;h:sc:ssl=1&amp;s:user:mid=69099319612994832056547930341105758682&amp;&amp;&amp;s:sp:ovp=Akamai&amp;s:sp:channel=Fox+News&amp;s:sp:player_name=Fox+News+Android+Player&amp;s:sp:hb_version=android-2.1.0.154-42fb90&amp;l:sp:hb_api_lvl=4&amp;s:event:sid=1673312989776217636246&amp;l:event:duration=9892&amp;l:event:playhead=11124&amp;l:event:prev_ts=1673312995088&amp;s:event:type=play&amp;l:event:ts=1673313004980&amp;s:asset:name=Biden+accused+of+mishandling+classified+documents&amp;l:asset:length=200&amp;s:asset:publisher=foxnews&amp;s:asset:type=main&amp;s:asset:video_id=6318425658112&amp;s:stream:type=vod&amp;l:stream:startup_time=0&amp;l:stream:fps=0&amp;l:stream:bitrate=0&amp;l:stream:dropped_frames=0.</t>
         </is>
       </c>
       <c r="C138" t="inlineStr">
@@ -3453,7 +3453,7 @@
       </c>
       <c r="D138" t="inlineStr">
         <is>
-          <t>Pass: 'l:event:playhead' parameter found.</t>
+          <t>Pass: 's:event:type' parameter found with value play. URL: http://foxnews.hb.omtrdc.net/?s:sc:rsid=foxnewsglobalproduction&amp;s:sc:tracking_server=smetrics.foxnews.com&amp;h:sc:ssl=1&amp;s:user:mid=69099319612994832056547930341105758682&amp;&amp;&amp;s:sp:ovp=Akamai&amp;s:sp:channel=Fox+News&amp;s:sp:player_name=Fox+News+Android+Player&amp;s:sp:hb_version=android-2.1.0.154-42fb90&amp;l:sp:hb_api_lvl=4&amp;s:event:sid=1673312989776217636246&amp;l:event:duration=9892&amp;l:event:playhead=11124&amp;l:event:prev_ts=1673312995088&amp;s:event:type=play&amp;l:event:ts=1673313004980&amp;s:asset:name=Biden+accused+of+mishandling+classified+documents&amp;l:asset:length=200&amp;s:asset:publisher=foxnews&amp;s:asset:type=main&amp;s:asset:video_id=6318425658112&amp;s:stream:type=vod&amp;l:stream:startup_time=0&amp;l:stream:fps=0&amp;l:stream:bitrate=0&amp;l:stream:dropped_frames=0.</t>
         </is>
       </c>
     </row>
@@ -3465,7 +3465,7 @@
       </c>
       <c r="B139" t="inlineStr">
         <is>
-          <t>'l</t>
+          <t>parameter found. URL: http://foxnews.hb.omtrdc.net/?s:sc:rsid=foxnewsglobalproduction&amp;s:sc:tracking_server=smetrics.foxnews.com&amp;h:sc:ssl=1&amp;s:user:mid=69099319612994832056547930341105758682&amp;&amp;&amp;s:sp:ovp=Akamai&amp;s:sp:channel=Fox+News&amp;s:sp:player_name=Fox+News+Android+Player&amp;s:sp:hb_version=android-2.1.0.154-42fb90&amp;l:sp:hb_api_lvl=4&amp;s:event:sid=1673312989776217636246&amp;l:event:duration=9892&amp;l:event:playhead=11124&amp;l:event:prev_ts=1673312995088&amp;s:event:type=play&amp;l:event:ts=1673313004980&amp;s:asset:name=Biden+accused+of+mishandling+classified+documents&amp;l:asset:length=200&amp;s:asset:publisher=foxnews&amp;s:asset:type=main&amp;s:asset:video_id=6318425658112&amp;s:stream:type=vod&amp;l:stream:startup_time=0&amp;l:stream:fps=0&amp;l:stream:bitrate=0&amp;l:stream:dropped_frames=0.</t>
         </is>
       </c>
       <c r="C139" t="inlineStr">
@@ -3475,7 +3475,7 @@
       </c>
       <c r="D139" t="inlineStr">
         <is>
-          <t>Pass: 'l:event:prev_ts' parameter found.</t>
+          <t>Pass: 's:event:sid' parameter found. URL: http://foxnews.hb.omtrdc.net/?s:sc:rsid=foxnewsglobalproduction&amp;s:sc:tracking_server=smetrics.foxnews.com&amp;h:sc:ssl=1&amp;s:user:mid=69099319612994832056547930341105758682&amp;&amp;&amp;s:sp:ovp=Akamai&amp;s:sp:channel=Fox+News&amp;s:sp:player_name=Fox+News+Android+Player&amp;s:sp:hb_version=android-2.1.0.154-42fb90&amp;l:sp:hb_api_lvl=4&amp;s:event:sid=1673312989776217636246&amp;l:event:duration=9892&amp;l:event:playhead=11124&amp;l:event:prev_ts=1673312995088&amp;s:event:type=play&amp;l:event:ts=1673313004980&amp;s:asset:name=Biden+accused+of+mishandling+classified+documents&amp;l:asset:length=200&amp;s:asset:publisher=foxnews&amp;s:asset:type=main&amp;s:asset:video_id=6318425658112&amp;s:stream:type=vod&amp;l:stream:startup_time=0&amp;l:stream:fps=0&amp;l:stream:bitrate=0&amp;l:stream:dropped_frames=0.</t>
         </is>
       </c>
     </row>
@@ -3487,7 +3487,7 @@
       </c>
       <c r="B140" t="inlineStr">
         <is>
-          <t>'l</t>
+          <t>parameter found.</t>
         </is>
       </c>
       <c r="C140" t="inlineStr">
@@ -3497,7 +3497,7 @@
       </c>
       <c r="D140" t="inlineStr">
         <is>
-          <t>Pass: 'l:event:ts' parameter found.</t>
+          <t>Pass: 'l:event:duration' parameter found.</t>
         </is>
       </c>
     </row>
@@ -3509,7 +3509,7 @@
       </c>
       <c r="B141" t="inlineStr">
         <is>
-          <t>'s</t>
+          <t>parameter found.</t>
         </is>
       </c>
       <c r="C141" t="inlineStr">
@@ -3519,7 +3519,7 @@
       </c>
       <c r="D141" t="inlineStr">
         <is>
-          <t>Pass: 's:asset:name' parameter found.</t>
+          <t>Pass: 'l:event:prev_ts' parameter found.</t>
         </is>
       </c>
     </row>
@@ -3531,7 +3531,7 @@
       </c>
       <c r="B142" t="inlineStr">
         <is>
-          <t>'l</t>
+          <t>parameter found.</t>
         </is>
       </c>
       <c r="C142" t="inlineStr">
@@ -3541,7 +3541,7 @@
       </c>
       <c r="D142" t="inlineStr">
         <is>
-          <t>Pass: 'l:asset:length' parameter found.</t>
+          <t>Pass: 'l:event:ts' parameter found.</t>
         </is>
       </c>
     </row>
@@ -3553,7 +3553,7 @@
       </c>
       <c r="B143" t="inlineStr">
         <is>
-          <t>'s</t>
+          <t>parameter found.</t>
         </is>
       </c>
       <c r="C143" t="inlineStr">
@@ -3563,7 +3563,7 @@
       </c>
       <c r="D143" t="inlineStr">
         <is>
-          <t>Pass: 's:asset:publisher' parameter found.</t>
+          <t>Pass: 's:asset:name' parameter found.</t>
         </is>
       </c>
     </row>
@@ -3575,7 +3575,7 @@
       </c>
       <c r="B144" t="inlineStr">
         <is>
-          <t>'s</t>
+          <t>parameter found.</t>
         </is>
       </c>
       <c r="C144" t="inlineStr">
@@ -3585,7 +3585,7 @@
       </c>
       <c r="D144" t="inlineStr">
         <is>
-          <t>Pass: 's:asset:type' parameter found.</t>
+          <t>Pass: 'l:asset:length' parameter found.</t>
         </is>
       </c>
     </row>
@@ -3597,7 +3597,7 @@
       </c>
       <c r="B145" t="inlineStr">
         <is>
-          <t>'s</t>
+          <t>parameter found.</t>
         </is>
       </c>
       <c r="C145" t="inlineStr">
@@ -3607,19 +3607,19 @@
       </c>
       <c r="D145" t="inlineStr">
         <is>
-          <t>Pass: 's:sc:rsid' parameter found with value foxnewsglobalproduction. URL: http://foxnews.hb.omtrdc.net/?s:sc:rsid=foxnewsglobalproduction&amp;s:sc:tracking_server=smetrics.foxnews.com&amp;h:sc:ssl=1&amp;s:user:mid=69099319612994832056547930341105758682&amp;&amp;&amp;s:sp:ovp=Akamai&amp;s:sp:channel=Fox+News&amp;s:sp:player_name=Fox+News+Android+Player&amp;s:sp:hb_version=android-2.1.0.154-42fb90&amp;l:sp:hb_api_lvl=4&amp;s:event:sid=1673312989776217636246&amp;l:event:duration=9892&amp;l:event:playhead=11124&amp;l:event:prev_ts=1673312995088&amp;s:event:type=play&amp;l:event:ts=1673313004980&amp;s:asset:name=Biden+accused+of+mishandling+classified+documents&amp;l:asset:length=200&amp;s:asset:publisher=foxnews&amp;s:asset:type=main&amp;s:asset:video_id=6318425658112&amp;s:stream:type=vod&amp;l:stream:startup_time=0&amp;l:stream:fps=0&amp;l:stream:bitrate=0&amp;l:stream:dropped_frames=0.</t>
+          <t>Pass: 's:asset:publisher' parameter found.</t>
         </is>
       </c>
     </row>
     <row r="146">
       <c r="A146" t="inlineStr">
         <is>
-          <t>http://foxnews.hb.omtrdc.net/?s:sc:rsid=foxnewsglobalproduction&amp;s:sc:tracking_server=smetrics.foxnews.com&amp;h:sc:ssl=1&amp;s:user:mid=69099319612994832056547930341105758682&amp;&amp;&amp;s:sp:ovp=Akamai&amp;s:sp:channel=Fox+News&amp;s:sp:player_name=Fox+News+Android+Player&amp;s:sp:hb_version=android-2.1.0.154-42fb90&amp;l:sp:hb_api_lvl=4&amp;s:event:sid=1673312989776217636246&amp;l:event:duration=9945&amp;l:event:playhead=21071&amp;l:event:prev_ts=1673313004980&amp;s:event:type=play&amp;l:event:ts=1673313014925&amp;s:asset:name=Biden+accused+of+mishandling+classified+documents&amp;l:asset:length=200&amp;s:asset:publisher=foxnews&amp;s:asset:type=main&amp;s:asset:video_id=6318425658112&amp;s:stream:type=vod&amp;l:stream:startup_time=0&amp;l:stream:fps=0&amp;l:stream:bitrate=0&amp;l:stream:dropped_frames=0</t>
+          <t>http://foxnews.hb.omtrdc.net/?s:sc:rsid=foxnewsglobalproduction&amp;s:sc:tracking_server=smetrics.foxnews.com&amp;h:sc:ssl=1&amp;s:user:mid=69099319612994832056547930341105758682&amp;&amp;&amp;s:sp:ovp=Akamai&amp;s:sp:channel=Fox+News&amp;s:sp:player_name=Fox+News+Android+Player&amp;s:sp:hb_version=android-2.1.0.154-42fb90&amp;l:sp:hb_api_lvl=4&amp;s:event:sid=1673312989776217636246&amp;l:event:duration=9892&amp;l:event:playhead=11124&amp;l:event:prev_ts=1673312995088&amp;s:event:type=play&amp;l:event:ts=1673313004980&amp;s:asset:name=Biden+accused+of+mishandling+classified+documents&amp;l:asset:length=200&amp;s:asset:publisher=foxnews&amp;s:asset:type=main&amp;s:asset:video_id=6318425658112&amp;s:stream:type=vod&amp;l:stream:startup_time=0&amp;l:stream:fps=0&amp;l:stream:bitrate=0&amp;l:stream:dropped_frames=0</t>
         </is>
       </c>
       <c r="B146" t="inlineStr">
         <is>
-          <t>'s</t>
+          <t>parameter found.</t>
         </is>
       </c>
       <c r="C146" t="inlineStr">
@@ -3629,19 +3629,19 @@
       </c>
       <c r="D146" t="inlineStr">
         <is>
-          <t>Pass: 's:event:type' parameter found with value play. URL: http://foxnews.hb.omtrdc.net/?s:sc:rsid=foxnewsglobalproduction&amp;s:sc:tracking_server=smetrics.foxnews.com&amp;h:sc:ssl=1&amp;s:user:mid=69099319612994832056547930341105758682&amp;&amp;&amp;s:sp:ovp=Akamai&amp;s:sp:channel=Fox+News&amp;s:sp:player_name=Fox+News+Android+Player&amp;s:sp:hb_version=android-2.1.0.154-42fb90&amp;l:sp:hb_api_lvl=4&amp;s:event:sid=1673312989776217636246&amp;l:event:duration=9945&amp;l:event:playhead=21071&amp;l:event:prev_ts=1673313004980&amp;s:event:type=play&amp;l:event:ts=1673313014925&amp;s:asset:name=Biden+accused+of+mishandling+classified+documents&amp;l:asset:length=200&amp;s:asset:publisher=foxnews&amp;s:asset:type=main&amp;s:asset:video_id=6318425658112&amp;s:stream:type=vod&amp;l:stream:startup_time=0&amp;l:stream:fps=0&amp;l:stream:bitrate=0&amp;l:stream:dropped_frames=0.</t>
+          <t>Pass: 's:asset:type' parameter found.</t>
         </is>
       </c>
     </row>
     <row r="147">
       <c r="A147" t="inlineStr">
         <is>
-          <t>http://foxnews.hb.omtrdc.net/?s:sc:rsid=foxnewsglobalproduction&amp;s:sc:tracking_server=smetrics.foxnews.com&amp;h:sc:ssl=1&amp;s:user:mid=69099319612994832056547930341105758682&amp;&amp;&amp;s:sp:ovp=Akamai&amp;s:sp:channel=Fox+News&amp;s:sp:player_name=Fox+News+Android+Player&amp;s:sp:hb_version=android-2.1.0.154-42fb90&amp;l:sp:hb_api_lvl=4&amp;s:event:sid=1673312989776217636246&amp;l:event:duration=9945&amp;l:event:playhead=21071&amp;l:event:prev_ts=1673313004980&amp;s:event:type=play&amp;l:event:ts=1673313014925&amp;s:asset:name=Biden+accused+of+mishandling+classified+documents&amp;l:asset:length=200&amp;s:asset:publisher=foxnews&amp;s:asset:type=main&amp;s:asset:video_id=6318425658112&amp;s:stream:type=vod&amp;l:stream:startup_time=0&amp;l:stream:fps=0&amp;l:stream:bitrate=0&amp;l:stream:dropped_frames=0</t>
+          <t>http://foxnews.hb.omtrdc.net/?s:sc:rsid=foxnewsglobalproduction&amp;s:sc:tracking_server=smetrics.foxnews.com&amp;h:sc:ssl=1&amp;s:user:mid=69099319612994832056547930341105758682&amp;&amp;&amp;s:sp:ovp=Akamai&amp;s:sp:channel=Fox+News&amp;s:sp:player_name=Fox+News+Android+Player&amp;s:sp:hb_version=android-2.1.0.154-42fb90&amp;l:sp:hb_api_lvl=4&amp;s:event:sid=1673312989776217636246&amp;l:event:duration=9892&amp;l:event:playhead=11124&amp;l:event:prev_ts=1673312995088&amp;s:event:type=play&amp;l:event:ts=1673313004980&amp;s:asset:name=Biden+accused+of+mishandling+classified+documents&amp;l:asset:length=200&amp;s:asset:publisher=foxnews&amp;s:asset:type=main&amp;s:asset:video_id=6318425658112&amp;s:stream:type=vod&amp;l:stream:startup_time=0&amp;l:stream:fps=0&amp;l:stream:bitrate=0&amp;l:stream:dropped_frames=0</t>
         </is>
       </c>
       <c r="B147" t="inlineStr">
         <is>
-          <t>'s</t>
+          <t>parameter found with value foxnewsglobalproduction. URL: http://foxnews.hb.omtrdc.net/?s:sc:rsid=foxnewsglobalproduction&amp;s:sc:tracking_server=smetrics.foxnews.com&amp;h:sc:ssl=1&amp;s:user:mid=69099319612994832056547930341105758682&amp;&amp;&amp;s:sp:ovp=Akamai&amp;s:sp:channel=Fox+News&amp;s:sp:player_name=Fox+News+Android+Player&amp;s:sp:hb_version=android-2.1.0.154-42fb90&amp;l:sp:hb_api_lvl=4&amp;s:event:sid=1673312989776217636246&amp;l:event:duration=9892&amp;l:event:playhead=11124&amp;l:event:prev_ts=1673312995088&amp;s:event:type=play&amp;l:event:ts=1673313004980&amp;s:asset:name=Biden+accused+of+mishandling+classified+documents&amp;l:asset:length=200&amp;s:asset:publisher=foxnews&amp;s:asset:type=main&amp;s:asset:video_id=6318425658112&amp;s:stream:type=vod&amp;l:stream:startup_time=0&amp;l:stream:fps=0&amp;l:stream:bitrate=0&amp;l:stream:dropped_frames=0.</t>
         </is>
       </c>
       <c r="C147" t="inlineStr">
@@ -3651,7 +3651,7 @@
       </c>
       <c r="D147" t="inlineStr">
         <is>
-          <t>Pass: 's:event:sid' parameter found. URL: http://foxnews.hb.omtrdc.net/?s:sc:rsid=foxnewsglobalproduction&amp;s:sc:tracking_server=smetrics.foxnews.com&amp;h:sc:ssl=1&amp;s:user:mid=69099319612994832056547930341105758682&amp;&amp;&amp;s:sp:ovp=Akamai&amp;s:sp:channel=Fox+News&amp;s:sp:player_name=Fox+News+Android+Player&amp;s:sp:hb_version=android-2.1.0.154-42fb90&amp;l:sp:hb_api_lvl=4&amp;s:event:sid=1673312989776217636246&amp;l:event:duration=9945&amp;l:event:playhead=21071&amp;l:event:prev_ts=1673313004980&amp;s:event:type=play&amp;l:event:ts=1673313014925&amp;s:asset:name=Biden+accused+of+mishandling+classified+documents&amp;l:asset:length=200&amp;s:asset:publisher=foxnews&amp;s:asset:type=main&amp;s:asset:video_id=6318425658112&amp;s:stream:type=vod&amp;l:stream:startup_time=0&amp;l:stream:fps=0&amp;l:stream:bitrate=0&amp;l:stream:dropped_frames=0.</t>
+          <t>Pass: 's:sc:rsid' parameter found with value foxnewsglobalproduction. URL: http://foxnews.hb.omtrdc.net/?s:sc:rsid=foxnewsglobalproduction&amp;s:sc:tracking_server=smetrics.foxnews.com&amp;h:sc:ssl=1&amp;s:user:mid=69099319612994832056547930341105758682&amp;&amp;&amp;s:sp:ovp=Akamai&amp;s:sp:channel=Fox+News&amp;s:sp:player_name=Fox+News+Android+Player&amp;s:sp:hb_version=android-2.1.0.154-42fb90&amp;l:sp:hb_api_lvl=4&amp;s:event:sid=1673312989776217636246&amp;l:event:duration=9892&amp;l:event:playhead=11124&amp;l:event:prev_ts=1673312995088&amp;s:event:type=play&amp;l:event:ts=1673313004980&amp;s:asset:name=Biden+accused+of+mishandling+classified+documents&amp;l:asset:length=200&amp;s:asset:publisher=foxnews&amp;s:asset:type=main&amp;s:asset:video_id=6318425658112&amp;s:stream:type=vod&amp;l:stream:startup_time=0&amp;l:stream:fps=0&amp;l:stream:bitrate=0&amp;l:stream:dropped_frames=0.</t>
         </is>
       </c>
     </row>
@@ -3663,7 +3663,7 @@
       </c>
       <c r="B148" t="inlineStr">
         <is>
-          <t>'l</t>
+          <t>parameter found with value play. URL: http://foxnews.hb.omtrdc.net/?s:sc:rsid=foxnewsglobalproduction&amp;s:sc:tracking_server=smetrics.foxnews.com&amp;h:sc:ssl=1&amp;s:user:mid=69099319612994832056547930341105758682&amp;&amp;&amp;s:sp:ovp=Akamai&amp;s:sp:channel=Fox+News&amp;s:sp:player_name=Fox+News+Android+Player&amp;s:sp:hb_version=android-2.1.0.154-42fb90&amp;l:sp:hb_api_lvl=4&amp;s:event:sid=1673312989776217636246&amp;l:event:duration=9945&amp;l:event:playhead=21071&amp;l:event:prev_ts=1673313004980&amp;s:event:type=play&amp;l:event:ts=1673313014925&amp;s:asset:name=Biden+accused+of+mishandling+classified+documents&amp;l:asset:length=200&amp;s:asset:publisher=foxnews&amp;s:asset:type=main&amp;s:asset:video_id=6318425658112&amp;s:stream:type=vod&amp;l:stream:startup_time=0&amp;l:stream:fps=0&amp;l:stream:bitrate=0&amp;l:stream:dropped_frames=0.</t>
         </is>
       </c>
       <c r="C148" t="inlineStr">
@@ -3673,7 +3673,7 @@
       </c>
       <c r="D148" t="inlineStr">
         <is>
-          <t>Pass: 'l:event:duration' parameter found.</t>
+          <t>Pass: 's:event:type' parameter found with value play. URL: http://foxnews.hb.omtrdc.net/?s:sc:rsid=foxnewsglobalproduction&amp;s:sc:tracking_server=smetrics.foxnews.com&amp;h:sc:ssl=1&amp;s:user:mid=69099319612994832056547930341105758682&amp;&amp;&amp;s:sp:ovp=Akamai&amp;s:sp:channel=Fox+News&amp;s:sp:player_name=Fox+News+Android+Player&amp;s:sp:hb_version=android-2.1.0.154-42fb90&amp;l:sp:hb_api_lvl=4&amp;s:event:sid=1673312989776217636246&amp;l:event:duration=9945&amp;l:event:playhead=21071&amp;l:event:prev_ts=1673313004980&amp;s:event:type=play&amp;l:event:ts=1673313014925&amp;s:asset:name=Biden+accused+of+mishandling+classified+documents&amp;l:asset:length=200&amp;s:asset:publisher=foxnews&amp;s:asset:type=main&amp;s:asset:video_id=6318425658112&amp;s:stream:type=vod&amp;l:stream:startup_time=0&amp;l:stream:fps=0&amp;l:stream:bitrate=0&amp;l:stream:dropped_frames=0.</t>
         </is>
       </c>
     </row>
@@ -3685,7 +3685,7 @@
       </c>
       <c r="B149" t="inlineStr">
         <is>
-          <t>'l</t>
+          <t>parameter found with value play. URL: http://foxnews.hb.omtrdc.net/?s:sc:rsid=foxnewsglobalproduction&amp;s:sc:tracking_server=smetrics.foxnews.com&amp;h:sc:ssl=1&amp;s:user:mid=69099319612994832056547930341105758682&amp;&amp;&amp;s:sp:ovp=Akamai&amp;s:sp:channel=Fox+News&amp;s:sp:player_name=Fox+News+Android+Player&amp;s:sp:hb_version=android-2.1.0.154-42fb90&amp;l:sp:hb_api_lvl=4&amp;s:event:sid=1673312989776217636246&amp;l:event:duration=9945&amp;l:event:playhead=21071&amp;l:event:prev_ts=1673313004980&amp;s:event:type=play&amp;l:event:ts=1673313014925&amp;s:asset:name=Biden+accused+of+mishandling+classified+documents&amp;l:asset:length=200&amp;s:asset:publisher=foxnews&amp;s:asset:type=main&amp;s:asset:video_id=6318425658112&amp;s:stream:type=vod&amp;l:stream:startup_time=0&amp;l:stream:fps=0&amp;l:stream:bitrate=0&amp;l:stream:dropped_frames=0.</t>
         </is>
       </c>
       <c r="C149" t="inlineStr">
@@ -3695,7 +3695,7 @@
       </c>
       <c r="D149" t="inlineStr">
         <is>
-          <t>Pass: 'l:event:playhead' parameter found.</t>
+          <t>Pass: 's:event:type' parameter found with value play. URL: http://foxnews.hb.omtrdc.net/?s:sc:rsid=foxnewsglobalproduction&amp;s:sc:tracking_server=smetrics.foxnews.com&amp;h:sc:ssl=1&amp;s:user:mid=69099319612994832056547930341105758682&amp;&amp;&amp;s:sp:ovp=Akamai&amp;s:sp:channel=Fox+News&amp;s:sp:player_name=Fox+News+Android+Player&amp;s:sp:hb_version=android-2.1.0.154-42fb90&amp;l:sp:hb_api_lvl=4&amp;s:event:sid=1673312989776217636246&amp;l:event:duration=9945&amp;l:event:playhead=21071&amp;l:event:prev_ts=1673313004980&amp;s:event:type=play&amp;l:event:ts=1673313014925&amp;s:asset:name=Biden+accused+of+mishandling+classified+documents&amp;l:asset:length=200&amp;s:asset:publisher=foxnews&amp;s:asset:type=main&amp;s:asset:video_id=6318425658112&amp;s:stream:type=vod&amp;l:stream:startup_time=0&amp;l:stream:fps=0&amp;l:stream:bitrate=0&amp;l:stream:dropped_frames=0.</t>
         </is>
       </c>
     </row>
@@ -3707,7 +3707,7 @@
       </c>
       <c r="B150" t="inlineStr">
         <is>
-          <t>'l</t>
+          <t>parameter found. URL: http://foxnews.hb.omtrdc.net/?s:sc:rsid=foxnewsglobalproduction&amp;s:sc:tracking_server=smetrics.foxnews.com&amp;h:sc:ssl=1&amp;s:user:mid=69099319612994832056547930341105758682&amp;&amp;&amp;s:sp:ovp=Akamai&amp;s:sp:channel=Fox+News&amp;s:sp:player_name=Fox+News+Android+Player&amp;s:sp:hb_version=android-2.1.0.154-42fb90&amp;l:sp:hb_api_lvl=4&amp;s:event:sid=1673312989776217636246&amp;l:event:duration=9945&amp;l:event:playhead=21071&amp;l:event:prev_ts=1673313004980&amp;s:event:type=play&amp;l:event:ts=1673313014925&amp;s:asset:name=Biden+accused+of+mishandling+classified+documents&amp;l:asset:length=200&amp;s:asset:publisher=foxnews&amp;s:asset:type=main&amp;s:asset:video_id=6318425658112&amp;s:stream:type=vod&amp;l:stream:startup_time=0&amp;l:stream:fps=0&amp;l:stream:bitrate=0&amp;l:stream:dropped_frames=0.</t>
         </is>
       </c>
       <c r="C150" t="inlineStr">
@@ -3717,7 +3717,7 @@
       </c>
       <c r="D150" t="inlineStr">
         <is>
-          <t>Pass: 'l:event:prev_ts' parameter found.</t>
+          <t>Pass: 's:event:sid' parameter found. URL: http://foxnews.hb.omtrdc.net/?s:sc:rsid=foxnewsglobalproduction&amp;s:sc:tracking_server=smetrics.foxnews.com&amp;h:sc:ssl=1&amp;s:user:mid=69099319612994832056547930341105758682&amp;&amp;&amp;s:sp:ovp=Akamai&amp;s:sp:channel=Fox+News&amp;s:sp:player_name=Fox+News+Android+Player&amp;s:sp:hb_version=android-2.1.0.154-42fb90&amp;l:sp:hb_api_lvl=4&amp;s:event:sid=1673312989776217636246&amp;l:event:duration=9945&amp;l:event:playhead=21071&amp;l:event:prev_ts=1673313004980&amp;s:event:type=play&amp;l:event:ts=1673313014925&amp;s:asset:name=Biden+accused+of+mishandling+classified+documents&amp;l:asset:length=200&amp;s:asset:publisher=foxnews&amp;s:asset:type=main&amp;s:asset:video_id=6318425658112&amp;s:stream:type=vod&amp;l:stream:startup_time=0&amp;l:stream:fps=0&amp;l:stream:bitrate=0&amp;l:stream:dropped_frames=0.</t>
         </is>
       </c>
     </row>
@@ -3729,7 +3729,7 @@
       </c>
       <c r="B151" t="inlineStr">
         <is>
-          <t>'l</t>
+          <t>parameter found.</t>
         </is>
       </c>
       <c r="C151" t="inlineStr">
@@ -3739,7 +3739,7 @@
       </c>
       <c r="D151" t="inlineStr">
         <is>
-          <t>Pass: 'l:event:ts' parameter found.</t>
+          <t>Pass: 'l:event:duration' parameter found.</t>
         </is>
       </c>
     </row>
@@ -3751,7 +3751,7 @@
       </c>
       <c r="B152" t="inlineStr">
         <is>
-          <t>'s</t>
+          <t>parameter found.</t>
         </is>
       </c>
       <c r="C152" t="inlineStr">
@@ -3761,7 +3761,7 @@
       </c>
       <c r="D152" t="inlineStr">
         <is>
-          <t>Pass: 's:asset:name' parameter found.</t>
+          <t>Pass: 'l:event:prev_ts' parameter found.</t>
         </is>
       </c>
     </row>
@@ -3773,7 +3773,7 @@
       </c>
       <c r="B153" t="inlineStr">
         <is>
-          <t>'l</t>
+          <t>parameter found.</t>
         </is>
       </c>
       <c r="C153" t="inlineStr">
@@ -3783,7 +3783,7 @@
       </c>
       <c r="D153" t="inlineStr">
         <is>
-          <t>Pass: 'l:asset:length' parameter found.</t>
+          <t>Pass: 'l:event:ts' parameter found.</t>
         </is>
       </c>
     </row>
@@ -3795,7 +3795,7 @@
       </c>
       <c r="B154" t="inlineStr">
         <is>
-          <t>'s</t>
+          <t>parameter found.</t>
         </is>
       </c>
       <c r="C154" t="inlineStr">
@@ -3805,7 +3805,7 @@
       </c>
       <c r="D154" t="inlineStr">
         <is>
-          <t>Pass: 's:asset:publisher' parameter found.</t>
+          <t>Pass: 's:asset:name' parameter found.</t>
         </is>
       </c>
     </row>
@@ -3817,7 +3817,7 @@
       </c>
       <c r="B155" t="inlineStr">
         <is>
-          <t>'s</t>
+          <t>parameter found.</t>
         </is>
       </c>
       <c r="C155" t="inlineStr">
@@ -3827,7 +3827,7 @@
       </c>
       <c r="D155" t="inlineStr">
         <is>
-          <t>Pass: 's:asset:type' parameter found.</t>
+          <t>Pass: 'l:asset:length' parameter found.</t>
         </is>
       </c>
     </row>
@@ -3839,7 +3839,7 @@
       </c>
       <c r="B156" t="inlineStr">
         <is>
-          <t>'s</t>
+          <t>parameter found.</t>
         </is>
       </c>
       <c r="C156" t="inlineStr">
@@ -3849,19 +3849,19 @@
       </c>
       <c r="D156" t="inlineStr">
         <is>
-          <t>Pass: 's:sc:rsid' parameter found with value foxnewsglobalproduction. URL: http://foxnews.hb.omtrdc.net/?s:sc:rsid=foxnewsglobalproduction&amp;s:sc:tracking_server=smetrics.foxnews.com&amp;h:sc:ssl=1&amp;s:user:mid=69099319612994832056547930341105758682&amp;&amp;&amp;s:sp:ovp=Akamai&amp;s:sp:channel=Fox+News&amp;s:sp:player_name=Fox+News+Android+Player&amp;s:sp:hb_version=android-2.1.0.154-42fb90&amp;l:sp:hb_api_lvl=4&amp;s:event:sid=1673312989776217636246&amp;l:event:duration=9945&amp;l:event:playhead=21071&amp;l:event:prev_ts=1673313004980&amp;s:event:type=play&amp;l:event:ts=1673313014925&amp;s:asset:name=Biden+accused+of+mishandling+classified+documents&amp;l:asset:length=200&amp;s:asset:publisher=foxnews&amp;s:asset:type=main&amp;s:asset:video_id=6318425658112&amp;s:stream:type=vod&amp;l:stream:startup_time=0&amp;l:stream:fps=0&amp;l:stream:bitrate=0&amp;l:stream:dropped_frames=0.</t>
+          <t>Pass: 's:asset:publisher' parameter found.</t>
         </is>
       </c>
     </row>
     <row r="157">
       <c r="A157" t="inlineStr">
         <is>
-          <t>http://foxnews.hb.omtrdc.net/?s:sc:rsid=foxnewsglobalproduction&amp;s:sc:tracking_server=smetrics.foxnews.com&amp;h:sc:ssl=1&amp;s:user:mid=69099319612994832056547930341105758682&amp;&amp;&amp;s:sp:ovp=Akamai&amp;s:sp:channel=Fox+News&amp;s:sp:player_name=Fox+News+Android+Player&amp;s:sp:hb_version=android-2.1.0.154-42fb90&amp;l:sp:hb_api_lvl=4&amp;s:event:sid=1673312989776217636246&amp;l:event:duration=9909&amp;l:event:playhead=30711&amp;l:event:prev_ts=1673313014925&amp;s:event:type=play&amp;l:event:ts=1673313024834&amp;s:asset:name=Biden+accused+of+mishandling+classified+documents&amp;l:asset:length=200&amp;s:asset:publisher=foxnews&amp;s:asset:type=main&amp;s:asset:video_id=6318425658112&amp;s:stream:type=vod&amp;l:stream:startup_time=0&amp;l:stream:fps=0&amp;l:stream:bitrate=0&amp;l:stream:dropped_frames=0</t>
+          <t>http://foxnews.hb.omtrdc.net/?s:sc:rsid=foxnewsglobalproduction&amp;s:sc:tracking_server=smetrics.foxnews.com&amp;h:sc:ssl=1&amp;s:user:mid=69099319612994832056547930341105758682&amp;&amp;&amp;s:sp:ovp=Akamai&amp;s:sp:channel=Fox+News&amp;s:sp:player_name=Fox+News+Android+Player&amp;s:sp:hb_version=android-2.1.0.154-42fb90&amp;l:sp:hb_api_lvl=4&amp;s:event:sid=1673312989776217636246&amp;l:event:duration=9945&amp;l:event:playhead=21071&amp;l:event:prev_ts=1673313004980&amp;s:event:type=play&amp;l:event:ts=1673313014925&amp;s:asset:name=Biden+accused+of+mishandling+classified+documents&amp;l:asset:length=200&amp;s:asset:publisher=foxnews&amp;s:asset:type=main&amp;s:asset:video_id=6318425658112&amp;s:stream:type=vod&amp;l:stream:startup_time=0&amp;l:stream:fps=0&amp;l:stream:bitrate=0&amp;l:stream:dropped_frames=0</t>
         </is>
       </c>
       <c r="B157" t="inlineStr">
         <is>
-          <t>'s</t>
+          <t>parameter found.</t>
         </is>
       </c>
       <c r="C157" t="inlineStr">
@@ -3871,19 +3871,19 @@
       </c>
       <c r="D157" t="inlineStr">
         <is>
-          <t>Pass: 's:event:type' parameter found with value play. URL: http://foxnews.hb.omtrdc.net/?s:sc:rsid=foxnewsglobalproduction&amp;s:sc:tracking_server=smetrics.foxnews.com&amp;h:sc:ssl=1&amp;s:user:mid=69099319612994832056547930341105758682&amp;&amp;&amp;s:sp:ovp=Akamai&amp;s:sp:channel=Fox+News&amp;s:sp:player_name=Fox+News+Android+Player&amp;s:sp:hb_version=android-2.1.0.154-42fb90&amp;l:sp:hb_api_lvl=4&amp;s:event:sid=1673312989776217636246&amp;l:event:duration=9909&amp;l:event:playhead=30711&amp;l:event:prev_ts=1673313014925&amp;s:event:type=play&amp;l:event:ts=1673313024834&amp;s:asset:name=Biden+accused+of+mishandling+classified+documents&amp;l:asset:length=200&amp;s:asset:publisher=foxnews&amp;s:asset:type=main&amp;s:asset:video_id=6318425658112&amp;s:stream:type=vod&amp;l:stream:startup_time=0&amp;l:stream:fps=0&amp;l:stream:bitrate=0&amp;l:stream:dropped_frames=0.</t>
+          <t>Pass: 's:asset:type' parameter found.</t>
         </is>
       </c>
     </row>
     <row r="158">
       <c r="A158" t="inlineStr">
         <is>
-          <t>http://foxnews.hb.omtrdc.net/?s:sc:rsid=foxnewsglobalproduction&amp;s:sc:tracking_server=smetrics.foxnews.com&amp;h:sc:ssl=1&amp;s:user:mid=69099319612994832056547930341105758682&amp;&amp;&amp;s:sp:ovp=Akamai&amp;s:sp:channel=Fox+News&amp;s:sp:player_name=Fox+News+Android+Player&amp;s:sp:hb_version=android-2.1.0.154-42fb90&amp;l:sp:hb_api_lvl=4&amp;s:event:sid=1673312989776217636246&amp;l:event:duration=9909&amp;l:event:playhead=30711&amp;l:event:prev_ts=1673313014925&amp;s:event:type=play&amp;l:event:ts=1673313024834&amp;s:asset:name=Biden+accused+of+mishandling+classified+documents&amp;l:asset:length=200&amp;s:asset:publisher=foxnews&amp;s:asset:type=main&amp;s:asset:video_id=6318425658112&amp;s:stream:type=vod&amp;l:stream:startup_time=0&amp;l:stream:fps=0&amp;l:stream:bitrate=0&amp;l:stream:dropped_frames=0</t>
+          <t>http://foxnews.hb.omtrdc.net/?s:sc:rsid=foxnewsglobalproduction&amp;s:sc:tracking_server=smetrics.foxnews.com&amp;h:sc:ssl=1&amp;s:user:mid=69099319612994832056547930341105758682&amp;&amp;&amp;s:sp:ovp=Akamai&amp;s:sp:channel=Fox+News&amp;s:sp:player_name=Fox+News+Android+Player&amp;s:sp:hb_version=android-2.1.0.154-42fb90&amp;l:sp:hb_api_lvl=4&amp;s:event:sid=1673312989776217636246&amp;l:event:duration=9945&amp;l:event:playhead=21071&amp;l:event:prev_ts=1673313004980&amp;s:event:type=play&amp;l:event:ts=1673313014925&amp;s:asset:name=Biden+accused+of+mishandling+classified+documents&amp;l:asset:length=200&amp;s:asset:publisher=foxnews&amp;s:asset:type=main&amp;s:asset:video_id=6318425658112&amp;s:stream:type=vod&amp;l:stream:startup_time=0&amp;l:stream:fps=0&amp;l:stream:bitrate=0&amp;l:stream:dropped_frames=0</t>
         </is>
       </c>
       <c r="B158" t="inlineStr">
         <is>
-          <t>'s</t>
+          <t>parameter found with value foxnewsglobalproduction. URL: http://foxnews.hb.omtrdc.net/?s:sc:rsid=foxnewsglobalproduction&amp;s:sc:tracking_server=smetrics.foxnews.com&amp;h:sc:ssl=1&amp;s:user:mid=69099319612994832056547930341105758682&amp;&amp;&amp;s:sp:ovp=Akamai&amp;s:sp:channel=Fox+News&amp;s:sp:player_name=Fox+News+Android+Player&amp;s:sp:hb_version=android-2.1.0.154-42fb90&amp;l:sp:hb_api_lvl=4&amp;s:event:sid=1673312989776217636246&amp;l:event:duration=9945&amp;l:event:playhead=21071&amp;l:event:prev_ts=1673313004980&amp;s:event:type=play&amp;l:event:ts=1673313014925&amp;s:asset:name=Biden+accused+of+mishandling+classified+documents&amp;l:asset:length=200&amp;s:asset:publisher=foxnews&amp;s:asset:type=main&amp;s:asset:video_id=6318425658112&amp;s:stream:type=vod&amp;l:stream:startup_time=0&amp;l:stream:fps=0&amp;l:stream:bitrate=0&amp;l:stream:dropped_frames=0.</t>
         </is>
       </c>
       <c r="C158" t="inlineStr">
@@ -3893,7 +3893,7 @@
       </c>
       <c r="D158" t="inlineStr">
         <is>
-          <t>Pass: 's:event:sid' parameter found. URL: http://foxnews.hb.omtrdc.net/?s:sc:rsid=foxnewsglobalproduction&amp;s:sc:tracking_server=smetrics.foxnews.com&amp;h:sc:ssl=1&amp;s:user:mid=69099319612994832056547930341105758682&amp;&amp;&amp;s:sp:ovp=Akamai&amp;s:sp:channel=Fox+News&amp;s:sp:player_name=Fox+News+Android+Player&amp;s:sp:hb_version=android-2.1.0.154-42fb90&amp;l:sp:hb_api_lvl=4&amp;s:event:sid=1673312989776217636246&amp;l:event:duration=9909&amp;l:event:playhead=30711&amp;l:event:prev_ts=1673313014925&amp;s:event:type=play&amp;l:event:ts=1673313024834&amp;s:asset:name=Biden+accused+of+mishandling+classified+documents&amp;l:asset:length=200&amp;s:asset:publisher=foxnews&amp;s:asset:type=main&amp;s:asset:video_id=6318425658112&amp;s:stream:type=vod&amp;l:stream:startup_time=0&amp;l:stream:fps=0&amp;l:stream:bitrate=0&amp;l:stream:dropped_frames=0.</t>
+          <t>Pass: 's:sc:rsid' parameter found with value foxnewsglobalproduction. URL: http://foxnews.hb.omtrdc.net/?s:sc:rsid=foxnewsglobalproduction&amp;s:sc:tracking_server=smetrics.foxnews.com&amp;h:sc:ssl=1&amp;s:user:mid=69099319612994832056547930341105758682&amp;&amp;&amp;s:sp:ovp=Akamai&amp;s:sp:channel=Fox+News&amp;s:sp:player_name=Fox+News+Android+Player&amp;s:sp:hb_version=android-2.1.0.154-42fb90&amp;l:sp:hb_api_lvl=4&amp;s:event:sid=1673312989776217636246&amp;l:event:duration=9945&amp;l:event:playhead=21071&amp;l:event:prev_ts=1673313004980&amp;s:event:type=play&amp;l:event:ts=1673313014925&amp;s:asset:name=Biden+accused+of+mishandling+classified+documents&amp;l:asset:length=200&amp;s:asset:publisher=foxnews&amp;s:asset:type=main&amp;s:asset:video_id=6318425658112&amp;s:stream:type=vod&amp;l:stream:startup_time=0&amp;l:stream:fps=0&amp;l:stream:bitrate=0&amp;l:stream:dropped_frames=0.</t>
         </is>
       </c>
     </row>
@@ -3905,7 +3905,7 @@
       </c>
       <c r="B159" t="inlineStr">
         <is>
-          <t>'l</t>
+          <t>parameter found with value play. URL: http://foxnews.hb.omtrdc.net/?s:sc:rsid=foxnewsglobalproduction&amp;s:sc:tracking_server=smetrics.foxnews.com&amp;h:sc:ssl=1&amp;s:user:mid=69099319612994832056547930341105758682&amp;&amp;&amp;s:sp:ovp=Akamai&amp;s:sp:channel=Fox+News&amp;s:sp:player_name=Fox+News+Android+Player&amp;s:sp:hb_version=android-2.1.0.154-42fb90&amp;l:sp:hb_api_lvl=4&amp;s:event:sid=1673312989776217636246&amp;l:event:duration=9909&amp;l:event:playhead=30711&amp;l:event:prev_ts=1673313014925&amp;s:event:type=play&amp;l:event:ts=1673313024834&amp;s:asset:name=Biden+accused+of+mishandling+classified+documents&amp;l:asset:length=200&amp;s:asset:publisher=foxnews&amp;s:asset:type=main&amp;s:asset:video_id=6318425658112&amp;s:stream:type=vod&amp;l:stream:startup_time=0&amp;l:stream:fps=0&amp;l:stream:bitrate=0&amp;l:stream:dropped_frames=0.</t>
         </is>
       </c>
       <c r="C159" t="inlineStr">
@@ -3915,7 +3915,7 @@
       </c>
       <c r="D159" t="inlineStr">
         <is>
-          <t>Pass: 'l:event:duration' parameter found.</t>
+          <t>Pass: 's:event:type' parameter found with value play. URL: http://foxnews.hb.omtrdc.net/?s:sc:rsid=foxnewsglobalproduction&amp;s:sc:tracking_server=smetrics.foxnews.com&amp;h:sc:ssl=1&amp;s:user:mid=69099319612994832056547930341105758682&amp;&amp;&amp;s:sp:ovp=Akamai&amp;s:sp:channel=Fox+News&amp;s:sp:player_name=Fox+News+Android+Player&amp;s:sp:hb_version=android-2.1.0.154-42fb90&amp;l:sp:hb_api_lvl=4&amp;s:event:sid=1673312989776217636246&amp;l:event:duration=9909&amp;l:event:playhead=30711&amp;l:event:prev_ts=1673313014925&amp;s:event:type=play&amp;l:event:ts=1673313024834&amp;s:asset:name=Biden+accused+of+mishandling+classified+documents&amp;l:asset:length=200&amp;s:asset:publisher=foxnews&amp;s:asset:type=main&amp;s:asset:video_id=6318425658112&amp;s:stream:type=vod&amp;l:stream:startup_time=0&amp;l:stream:fps=0&amp;l:stream:bitrate=0&amp;l:stream:dropped_frames=0.</t>
         </is>
       </c>
     </row>
@@ -3927,7 +3927,7 @@
       </c>
       <c r="B160" t="inlineStr">
         <is>
-          <t>'l</t>
+          <t>parameter found with value play. URL: http://foxnews.hb.omtrdc.net/?s:sc:rsid=foxnewsglobalproduction&amp;s:sc:tracking_server=smetrics.foxnews.com&amp;h:sc:ssl=1&amp;s:user:mid=69099319612994832056547930341105758682&amp;&amp;&amp;s:sp:ovp=Akamai&amp;s:sp:channel=Fox+News&amp;s:sp:player_name=Fox+News+Android+Player&amp;s:sp:hb_version=android-2.1.0.154-42fb90&amp;l:sp:hb_api_lvl=4&amp;s:event:sid=1673312989776217636246&amp;l:event:duration=9909&amp;l:event:playhead=30711&amp;l:event:prev_ts=1673313014925&amp;s:event:type=play&amp;l:event:ts=1673313024834&amp;s:asset:name=Biden+accused+of+mishandling+classified+documents&amp;l:asset:length=200&amp;s:asset:publisher=foxnews&amp;s:asset:type=main&amp;s:asset:video_id=6318425658112&amp;s:stream:type=vod&amp;l:stream:startup_time=0&amp;l:stream:fps=0&amp;l:stream:bitrate=0&amp;l:stream:dropped_frames=0.</t>
         </is>
       </c>
       <c r="C160" t="inlineStr">
@@ -3937,7 +3937,7 @@
       </c>
       <c r="D160" t="inlineStr">
         <is>
-          <t>Pass: 'l:event:playhead' parameter found.</t>
+          <t>Pass: 's:event:type' parameter found with value play. URL: http://foxnews.hb.omtrdc.net/?s:sc:rsid=foxnewsglobalproduction&amp;s:sc:tracking_server=smetrics.foxnews.com&amp;h:sc:ssl=1&amp;s:user:mid=69099319612994832056547930341105758682&amp;&amp;&amp;s:sp:ovp=Akamai&amp;s:sp:channel=Fox+News&amp;s:sp:player_name=Fox+News+Android+Player&amp;s:sp:hb_version=android-2.1.0.154-42fb90&amp;l:sp:hb_api_lvl=4&amp;s:event:sid=1673312989776217636246&amp;l:event:duration=9909&amp;l:event:playhead=30711&amp;l:event:prev_ts=1673313014925&amp;s:event:type=play&amp;l:event:ts=1673313024834&amp;s:asset:name=Biden+accused+of+mishandling+classified+documents&amp;l:asset:length=200&amp;s:asset:publisher=foxnews&amp;s:asset:type=main&amp;s:asset:video_id=6318425658112&amp;s:stream:type=vod&amp;l:stream:startup_time=0&amp;l:stream:fps=0&amp;l:stream:bitrate=0&amp;l:stream:dropped_frames=0.</t>
         </is>
       </c>
     </row>
@@ -3949,7 +3949,7 @@
       </c>
       <c r="B161" t="inlineStr">
         <is>
-          <t>'l</t>
+          <t>parameter found. URL: http://foxnews.hb.omtrdc.net/?s:sc:rsid=foxnewsglobalproduction&amp;s:sc:tracking_server=smetrics.foxnews.com&amp;h:sc:ssl=1&amp;s:user:mid=69099319612994832056547930341105758682&amp;&amp;&amp;s:sp:ovp=Akamai&amp;s:sp:channel=Fox+News&amp;s:sp:player_name=Fox+News+Android+Player&amp;s:sp:hb_version=android-2.1.0.154-42fb90&amp;l:sp:hb_api_lvl=4&amp;s:event:sid=1673312989776217636246&amp;l:event:duration=9909&amp;l:event:playhead=30711&amp;l:event:prev_ts=1673313014925&amp;s:event:type=play&amp;l:event:ts=1673313024834&amp;s:asset:name=Biden+accused+of+mishandling+classified+documents&amp;l:asset:length=200&amp;s:asset:publisher=foxnews&amp;s:asset:type=main&amp;s:asset:video_id=6318425658112&amp;s:stream:type=vod&amp;l:stream:startup_time=0&amp;l:stream:fps=0&amp;l:stream:bitrate=0&amp;l:stream:dropped_frames=0.</t>
         </is>
       </c>
       <c r="C161" t="inlineStr">
@@ -3959,7 +3959,7 @@
       </c>
       <c r="D161" t="inlineStr">
         <is>
-          <t>Pass: 'l:event:prev_ts' parameter found.</t>
+          <t>Pass: 's:event:sid' parameter found. URL: http://foxnews.hb.omtrdc.net/?s:sc:rsid=foxnewsglobalproduction&amp;s:sc:tracking_server=smetrics.foxnews.com&amp;h:sc:ssl=1&amp;s:user:mid=69099319612994832056547930341105758682&amp;&amp;&amp;s:sp:ovp=Akamai&amp;s:sp:channel=Fox+News&amp;s:sp:player_name=Fox+News+Android+Player&amp;s:sp:hb_version=android-2.1.0.154-42fb90&amp;l:sp:hb_api_lvl=4&amp;s:event:sid=1673312989776217636246&amp;l:event:duration=9909&amp;l:event:playhead=30711&amp;l:event:prev_ts=1673313014925&amp;s:event:type=play&amp;l:event:ts=1673313024834&amp;s:asset:name=Biden+accused+of+mishandling+classified+documents&amp;l:asset:length=200&amp;s:asset:publisher=foxnews&amp;s:asset:type=main&amp;s:asset:video_id=6318425658112&amp;s:stream:type=vod&amp;l:stream:startup_time=0&amp;l:stream:fps=0&amp;l:stream:bitrate=0&amp;l:stream:dropped_frames=0.</t>
         </is>
       </c>
     </row>
@@ -3971,7 +3971,7 @@
       </c>
       <c r="B162" t="inlineStr">
         <is>
-          <t>'l</t>
+          <t>parameter found.</t>
         </is>
       </c>
       <c r="C162" t="inlineStr">
@@ -3981,7 +3981,7 @@
       </c>
       <c r="D162" t="inlineStr">
         <is>
-          <t>Pass: 'l:event:ts' parameter found.</t>
+          <t>Pass: 'l:event:duration' parameter found.</t>
         </is>
       </c>
     </row>
@@ -3993,7 +3993,7 @@
       </c>
       <c r="B163" t="inlineStr">
         <is>
-          <t>'s</t>
+          <t>parameter found.</t>
         </is>
       </c>
       <c r="C163" t="inlineStr">
@@ -4003,7 +4003,7 @@
       </c>
       <c r="D163" t="inlineStr">
         <is>
-          <t>Pass: 's:asset:name' parameter found.</t>
+          <t>Pass: 'l:event:prev_ts' parameter found.</t>
         </is>
       </c>
     </row>
@@ -4015,7 +4015,7 @@
       </c>
       <c r="B164" t="inlineStr">
         <is>
-          <t>'l</t>
+          <t>parameter found.</t>
         </is>
       </c>
       <c r="C164" t="inlineStr">
@@ -4025,7 +4025,7 @@
       </c>
       <c r="D164" t="inlineStr">
         <is>
-          <t>Pass: 'l:asset:length' parameter found.</t>
+          <t>Pass: 'l:event:ts' parameter found.</t>
         </is>
       </c>
     </row>
@@ -4037,7 +4037,7 @@
       </c>
       <c r="B165" t="inlineStr">
         <is>
-          <t>'s</t>
+          <t>parameter found.</t>
         </is>
       </c>
       <c r="C165" t="inlineStr">
@@ -4047,7 +4047,7 @@
       </c>
       <c r="D165" t="inlineStr">
         <is>
-          <t>Pass: 's:asset:publisher' parameter found.</t>
+          <t>Pass: 's:asset:name' parameter found.</t>
         </is>
       </c>
     </row>
@@ -4059,7 +4059,7 @@
       </c>
       <c r="B166" t="inlineStr">
         <is>
-          <t>'s</t>
+          <t>parameter found.</t>
         </is>
       </c>
       <c r="C166" t="inlineStr">
@@ -4069,7 +4069,7 @@
       </c>
       <c r="D166" t="inlineStr">
         <is>
-          <t>Pass: 's:asset:type' parameter found.</t>
+          <t>Pass: 'l:asset:length' parameter found.</t>
         </is>
       </c>
     </row>
@@ -4081,7 +4081,7 @@
       </c>
       <c r="B167" t="inlineStr">
         <is>
-          <t>'s</t>
+          <t>parameter found.</t>
         </is>
       </c>
       <c r="C167" t="inlineStr">
@@ -4091,19 +4091,19 @@
       </c>
       <c r="D167" t="inlineStr">
         <is>
-          <t>Pass: 's:sc:rsid' parameter found with value foxnewsglobalproduction. URL: http://foxnews.hb.omtrdc.net/?s:sc:rsid=foxnewsglobalproduction&amp;s:sc:tracking_server=smetrics.foxnews.com&amp;h:sc:ssl=1&amp;s:user:mid=69099319612994832056547930341105758682&amp;&amp;&amp;s:sp:ovp=Akamai&amp;s:sp:channel=Fox+News&amp;s:sp:player_name=Fox+News+Android+Player&amp;s:sp:hb_version=android-2.1.0.154-42fb90&amp;l:sp:hb_api_lvl=4&amp;s:event:sid=1673312989776217636246&amp;l:event:duration=9909&amp;l:event:playhead=30711&amp;l:event:prev_ts=1673313014925&amp;s:event:type=play&amp;l:event:ts=1673313024834&amp;s:asset:name=Biden+accused+of+mishandling+classified+documents&amp;l:asset:length=200&amp;s:asset:publisher=foxnews&amp;s:asset:type=main&amp;s:asset:video_id=6318425658112&amp;s:stream:type=vod&amp;l:stream:startup_time=0&amp;l:stream:fps=0&amp;l:stream:bitrate=0&amp;l:stream:dropped_frames=0.</t>
+          <t>Pass: 's:asset:publisher' parameter found.</t>
         </is>
       </c>
     </row>
     <row r="168">
       <c r="A168" t="inlineStr">
         <is>
-          <t>http://foxnews.hb.omtrdc.net/?s:sc:rsid=foxnewsglobalproduction&amp;s:sc:tracking_server=smetrics.foxnews.com&amp;h:sc:ssl=1&amp;s:user:mid=69099319612994832056547930341105758682&amp;&amp;&amp;s:sp:ovp=Akamai&amp;s:sp:channel=Fox+News&amp;s:sp:player_name=Fox+News+Android+Player&amp;s:sp:hb_version=android-2.1.0.154-42fb90&amp;l:sp:hb_api_lvl=4&amp;s:event:sid=1673312989776217636246&amp;l:event:duration=10104&amp;l:event:playhead=40827&amp;l:event:prev_ts=1673313024834&amp;s:event:type=play&amp;l:event:ts=1673313034938&amp;s:asset:name=Biden+accused+of+mishandling+classified+documents&amp;l:asset:length=200&amp;s:asset:publisher=foxnews&amp;s:asset:type=main&amp;s:asset:video_id=6318425658112&amp;s:stream:type=vod&amp;l:stream:startup_time=0&amp;l:stream:fps=0&amp;l:stream:bitrate=0&amp;l:stream:dropped_frames=0</t>
+          <t>http://foxnews.hb.omtrdc.net/?s:sc:rsid=foxnewsglobalproduction&amp;s:sc:tracking_server=smetrics.foxnews.com&amp;h:sc:ssl=1&amp;s:user:mid=69099319612994832056547930341105758682&amp;&amp;&amp;s:sp:ovp=Akamai&amp;s:sp:channel=Fox+News&amp;s:sp:player_name=Fox+News+Android+Player&amp;s:sp:hb_version=android-2.1.0.154-42fb90&amp;l:sp:hb_api_lvl=4&amp;s:event:sid=1673312989776217636246&amp;l:event:duration=9909&amp;l:event:playhead=30711&amp;l:event:prev_ts=1673313014925&amp;s:event:type=play&amp;l:event:ts=1673313024834&amp;s:asset:name=Biden+accused+of+mishandling+classified+documents&amp;l:asset:length=200&amp;s:asset:publisher=foxnews&amp;s:asset:type=main&amp;s:asset:video_id=6318425658112&amp;s:stream:type=vod&amp;l:stream:startup_time=0&amp;l:stream:fps=0&amp;l:stream:bitrate=0&amp;l:stream:dropped_frames=0</t>
         </is>
       </c>
       <c r="B168" t="inlineStr">
         <is>
-          <t>'s</t>
+          <t>parameter found.</t>
         </is>
       </c>
       <c r="C168" t="inlineStr">
@@ -4113,19 +4113,19 @@
       </c>
       <c r="D168" t="inlineStr">
         <is>
-          <t>Pass: 's:event:type' parameter found with value play. URL: http://foxnews.hb.omtrdc.net/?s:sc:rsid=foxnewsglobalproduction&amp;s:sc:tracking_server=smetrics.foxnews.com&amp;h:sc:ssl=1&amp;s:user:mid=69099319612994832056547930341105758682&amp;&amp;&amp;s:sp:ovp=Akamai&amp;s:sp:channel=Fox+News&amp;s:sp:player_name=Fox+News+Android+Player&amp;s:sp:hb_version=android-2.1.0.154-42fb90&amp;l:sp:hb_api_lvl=4&amp;s:event:sid=1673312989776217636246&amp;l:event:duration=10104&amp;l:event:playhead=40827&amp;l:event:prev_ts=1673313024834&amp;s:event:type=play&amp;l:event:ts=1673313034938&amp;s:asset:name=Biden+accused+of+mishandling+classified+documents&amp;l:asset:length=200&amp;s:asset:publisher=foxnews&amp;s:asset:type=main&amp;s:asset:video_id=6318425658112&amp;s:stream:type=vod&amp;l:stream:startup_time=0&amp;l:stream:fps=0&amp;l:stream:bitrate=0&amp;l:stream:dropped_frames=0.</t>
+          <t>Pass: 's:asset:type' parameter found.</t>
         </is>
       </c>
     </row>
     <row r="169">
       <c r="A169" t="inlineStr">
         <is>
-          <t>http://foxnews.hb.omtrdc.net/?s:sc:rsid=foxnewsglobalproduction&amp;s:sc:tracking_server=smetrics.foxnews.com&amp;h:sc:ssl=1&amp;s:user:mid=69099319612994832056547930341105758682&amp;&amp;&amp;s:sp:ovp=Akamai&amp;s:sp:channel=Fox+News&amp;s:sp:player_name=Fox+News+Android+Player&amp;s:sp:hb_version=android-2.1.0.154-42fb90&amp;l:sp:hb_api_lvl=4&amp;s:event:sid=1673312989776217636246&amp;l:event:duration=10104&amp;l:event:playhead=40827&amp;l:event:prev_ts=1673313024834&amp;s:event:type=play&amp;l:event:ts=1673313034938&amp;s:asset:name=Biden+accused+of+mishandling+classified+documents&amp;l:asset:length=200&amp;s:asset:publisher=foxnews&amp;s:asset:type=main&amp;s:asset:video_id=6318425658112&amp;s:stream:type=vod&amp;l:stream:startup_time=0&amp;l:stream:fps=0&amp;l:stream:bitrate=0&amp;l:stream:dropped_frames=0</t>
+          <t>http://foxnews.hb.omtrdc.net/?s:sc:rsid=foxnewsglobalproduction&amp;s:sc:tracking_server=smetrics.foxnews.com&amp;h:sc:ssl=1&amp;s:user:mid=69099319612994832056547930341105758682&amp;&amp;&amp;s:sp:ovp=Akamai&amp;s:sp:channel=Fox+News&amp;s:sp:player_name=Fox+News+Android+Player&amp;s:sp:hb_version=android-2.1.0.154-42fb90&amp;l:sp:hb_api_lvl=4&amp;s:event:sid=1673312989776217636246&amp;l:event:duration=9909&amp;l:event:playhead=30711&amp;l:event:prev_ts=1673313014925&amp;s:event:type=play&amp;l:event:ts=1673313024834&amp;s:asset:name=Biden+accused+of+mishandling+classified+documents&amp;l:asset:length=200&amp;s:asset:publisher=foxnews&amp;s:asset:type=main&amp;s:asset:video_id=6318425658112&amp;s:stream:type=vod&amp;l:stream:startup_time=0&amp;l:stream:fps=0&amp;l:stream:bitrate=0&amp;l:stream:dropped_frames=0</t>
         </is>
       </c>
       <c r="B169" t="inlineStr">
         <is>
-          <t>'s</t>
+          <t>parameter found with value foxnewsglobalproduction. URL: http://foxnews.hb.omtrdc.net/?s:sc:rsid=foxnewsglobalproduction&amp;s:sc:tracking_server=smetrics.foxnews.com&amp;h:sc:ssl=1&amp;s:user:mid=69099319612994832056547930341105758682&amp;&amp;&amp;s:sp:ovp=Akamai&amp;s:sp:channel=Fox+News&amp;s:sp:player_name=Fox+News+Android+Player&amp;s:sp:hb_version=android-2.1.0.154-42fb90&amp;l:sp:hb_api_lvl=4&amp;s:event:sid=1673312989776217636246&amp;l:event:duration=9909&amp;l:event:playhead=30711&amp;l:event:prev_ts=1673313014925&amp;s:event:type=play&amp;l:event:ts=1673313024834&amp;s:asset:name=Biden+accused+of+mishandling+classified+documents&amp;l:asset:length=200&amp;s:asset:publisher=foxnews&amp;s:asset:type=main&amp;s:asset:video_id=6318425658112&amp;s:stream:type=vod&amp;l:stream:startup_time=0&amp;l:stream:fps=0&amp;l:stream:bitrate=0&amp;l:stream:dropped_frames=0.</t>
         </is>
       </c>
       <c r="C169" t="inlineStr">
@@ -4135,7 +4135,7 @@
       </c>
       <c r="D169" t="inlineStr">
         <is>
-          <t>Pass: 's:event:sid' parameter found. URL: http://foxnews.hb.omtrdc.net/?s:sc:rsid=foxnewsglobalproduction&amp;s:sc:tracking_server=smetrics.foxnews.com&amp;h:sc:ssl=1&amp;s:user:mid=69099319612994832056547930341105758682&amp;&amp;&amp;s:sp:ovp=Akamai&amp;s:sp:channel=Fox+News&amp;s:sp:player_name=Fox+News+Android+Player&amp;s:sp:hb_version=android-2.1.0.154-42fb90&amp;l:sp:hb_api_lvl=4&amp;s:event:sid=1673312989776217636246&amp;l:event:duration=10104&amp;l:event:playhead=40827&amp;l:event:prev_ts=1673313024834&amp;s:event:type=play&amp;l:event:ts=1673313034938&amp;s:asset:name=Biden+accused+of+mishandling+classified+documents&amp;l:asset:length=200&amp;s:asset:publisher=foxnews&amp;s:asset:type=main&amp;s:asset:video_id=6318425658112&amp;s:stream:type=vod&amp;l:stream:startup_time=0&amp;l:stream:fps=0&amp;l:stream:bitrate=0&amp;l:stream:dropped_frames=0.</t>
+          <t>Pass: 's:sc:rsid' parameter found with value foxnewsglobalproduction. URL: http://foxnews.hb.omtrdc.net/?s:sc:rsid=foxnewsglobalproduction&amp;s:sc:tracking_server=smetrics.foxnews.com&amp;h:sc:ssl=1&amp;s:user:mid=69099319612994832056547930341105758682&amp;&amp;&amp;s:sp:ovp=Akamai&amp;s:sp:channel=Fox+News&amp;s:sp:player_name=Fox+News+Android+Player&amp;s:sp:hb_version=android-2.1.0.154-42fb90&amp;l:sp:hb_api_lvl=4&amp;s:event:sid=1673312989776217636246&amp;l:event:duration=9909&amp;l:event:playhead=30711&amp;l:event:prev_ts=1673313014925&amp;s:event:type=play&amp;l:event:ts=1673313024834&amp;s:asset:name=Biden+accused+of+mishandling+classified+documents&amp;l:asset:length=200&amp;s:asset:publisher=foxnews&amp;s:asset:type=main&amp;s:asset:video_id=6318425658112&amp;s:stream:type=vod&amp;l:stream:startup_time=0&amp;l:stream:fps=0&amp;l:stream:bitrate=0&amp;l:stream:dropped_frames=0.</t>
         </is>
       </c>
     </row>
@@ -4147,7 +4147,7 @@
       </c>
       <c r="B170" t="inlineStr">
         <is>
-          <t>'l</t>
+          <t>parameter found with value play. URL: http://foxnews.hb.omtrdc.net/?s:sc:rsid=foxnewsglobalproduction&amp;s:sc:tracking_server=smetrics.foxnews.com&amp;h:sc:ssl=1&amp;s:user:mid=69099319612994832056547930341105758682&amp;&amp;&amp;s:sp:ovp=Akamai&amp;s:sp:channel=Fox+News&amp;s:sp:player_name=Fox+News+Android+Player&amp;s:sp:hb_version=android-2.1.0.154-42fb90&amp;l:sp:hb_api_lvl=4&amp;s:event:sid=1673312989776217636246&amp;l:event:duration=10104&amp;l:event:playhead=40827&amp;l:event:prev_ts=1673313024834&amp;s:event:type=play&amp;l:event:ts=1673313034938&amp;s:asset:name=Biden+accused+of+mishandling+classified+documents&amp;l:asset:length=200&amp;s:asset:publisher=foxnews&amp;s:asset:type=main&amp;s:asset:video_id=6318425658112&amp;s:stream:type=vod&amp;l:stream:startup_time=0&amp;l:stream:fps=0&amp;l:stream:bitrate=0&amp;l:stream:dropped_frames=0.</t>
         </is>
       </c>
       <c r="C170" t="inlineStr">
@@ -4157,7 +4157,7 @@
       </c>
       <c r="D170" t="inlineStr">
         <is>
-          <t>Pass: 'l:event:duration' parameter found.</t>
+          <t>Pass: 's:event:type' parameter found with value play. URL: http://foxnews.hb.omtrdc.net/?s:sc:rsid=foxnewsglobalproduction&amp;s:sc:tracking_server=smetrics.foxnews.com&amp;h:sc:ssl=1&amp;s:user:mid=69099319612994832056547930341105758682&amp;&amp;&amp;s:sp:ovp=Akamai&amp;s:sp:channel=Fox+News&amp;s:sp:player_name=Fox+News+Android+Player&amp;s:sp:hb_version=android-2.1.0.154-42fb90&amp;l:sp:hb_api_lvl=4&amp;s:event:sid=1673312989776217636246&amp;l:event:duration=10104&amp;l:event:playhead=40827&amp;l:event:prev_ts=1673313024834&amp;s:event:type=play&amp;l:event:ts=1673313034938&amp;s:asset:name=Biden+accused+of+mishandling+classified+documents&amp;l:asset:length=200&amp;s:asset:publisher=foxnews&amp;s:asset:type=main&amp;s:asset:video_id=6318425658112&amp;s:stream:type=vod&amp;l:stream:startup_time=0&amp;l:stream:fps=0&amp;l:stream:bitrate=0&amp;l:stream:dropped_frames=0.</t>
         </is>
       </c>
     </row>
@@ -4169,7 +4169,7 @@
       </c>
       <c r="B171" t="inlineStr">
         <is>
-          <t>'l</t>
+          <t>parameter found with value play. URL: http://foxnews.hb.omtrdc.net/?s:sc:rsid=foxnewsglobalproduction&amp;s:sc:tracking_server=smetrics.foxnews.com&amp;h:sc:ssl=1&amp;s:user:mid=69099319612994832056547930341105758682&amp;&amp;&amp;s:sp:ovp=Akamai&amp;s:sp:channel=Fox+News&amp;s:sp:player_name=Fox+News+Android+Player&amp;s:sp:hb_version=android-2.1.0.154-42fb90&amp;l:sp:hb_api_lvl=4&amp;s:event:sid=1673312989776217636246&amp;l:event:duration=10104&amp;l:event:playhead=40827&amp;l:event:prev_ts=1673313024834&amp;s:event:type=play&amp;l:event:ts=1673313034938&amp;s:asset:name=Biden+accused+of+mishandling+classified+documents&amp;l:asset:length=200&amp;s:asset:publisher=foxnews&amp;s:asset:type=main&amp;s:asset:video_id=6318425658112&amp;s:stream:type=vod&amp;l:stream:startup_time=0&amp;l:stream:fps=0&amp;l:stream:bitrate=0&amp;l:stream:dropped_frames=0.</t>
         </is>
       </c>
       <c r="C171" t="inlineStr">
@@ -4179,7 +4179,7 @@
       </c>
       <c r="D171" t="inlineStr">
         <is>
-          <t>Pass: 'l:event:playhead' parameter found.</t>
+          <t>Pass: 's:event:type' parameter found with value play. URL: http://foxnews.hb.omtrdc.net/?s:sc:rsid=foxnewsglobalproduction&amp;s:sc:tracking_server=smetrics.foxnews.com&amp;h:sc:ssl=1&amp;s:user:mid=69099319612994832056547930341105758682&amp;&amp;&amp;s:sp:ovp=Akamai&amp;s:sp:channel=Fox+News&amp;s:sp:player_name=Fox+News+Android+Player&amp;s:sp:hb_version=android-2.1.0.154-42fb90&amp;l:sp:hb_api_lvl=4&amp;s:event:sid=1673312989776217636246&amp;l:event:duration=10104&amp;l:event:playhead=40827&amp;l:event:prev_ts=1673313024834&amp;s:event:type=play&amp;l:event:ts=1673313034938&amp;s:asset:name=Biden+accused+of+mishandling+classified+documents&amp;l:asset:length=200&amp;s:asset:publisher=foxnews&amp;s:asset:type=main&amp;s:asset:video_id=6318425658112&amp;s:stream:type=vod&amp;l:stream:startup_time=0&amp;l:stream:fps=0&amp;l:stream:bitrate=0&amp;l:stream:dropped_frames=0.</t>
         </is>
       </c>
     </row>
@@ -4191,7 +4191,7 @@
       </c>
       <c r="B172" t="inlineStr">
         <is>
-          <t>'l</t>
+          <t>parameter found. URL: http://foxnews.hb.omtrdc.net/?s:sc:rsid=foxnewsglobalproduction&amp;s:sc:tracking_server=smetrics.foxnews.com&amp;h:sc:ssl=1&amp;s:user:mid=69099319612994832056547930341105758682&amp;&amp;&amp;s:sp:ovp=Akamai&amp;s:sp:channel=Fox+News&amp;s:sp:player_name=Fox+News+Android+Player&amp;s:sp:hb_version=android-2.1.0.154-42fb90&amp;l:sp:hb_api_lvl=4&amp;s:event:sid=1673312989776217636246&amp;l:event:duration=10104&amp;l:event:playhead=40827&amp;l:event:prev_ts=1673313024834&amp;s:event:type=play&amp;l:event:ts=1673313034938&amp;s:asset:name=Biden+accused+of+mishandling+classified+documents&amp;l:asset:length=200&amp;s:asset:publisher=foxnews&amp;s:asset:type=main&amp;s:asset:video_id=6318425658112&amp;s:stream:type=vod&amp;l:stream:startup_time=0&amp;l:stream:fps=0&amp;l:stream:bitrate=0&amp;l:stream:dropped_frames=0.</t>
         </is>
       </c>
       <c r="C172" t="inlineStr">
@@ -4201,7 +4201,7 @@
       </c>
       <c r="D172" t="inlineStr">
         <is>
-          <t>Pass: 'l:event:prev_ts' parameter found.</t>
+          <t>Pass: 's:event:sid' parameter found. URL: http://foxnews.hb.omtrdc.net/?s:sc:rsid=foxnewsglobalproduction&amp;s:sc:tracking_server=smetrics.foxnews.com&amp;h:sc:ssl=1&amp;s:user:mid=69099319612994832056547930341105758682&amp;&amp;&amp;s:sp:ovp=Akamai&amp;s:sp:channel=Fox+News&amp;s:sp:player_name=Fox+News+Android+Player&amp;s:sp:hb_version=android-2.1.0.154-42fb90&amp;l:sp:hb_api_lvl=4&amp;s:event:sid=1673312989776217636246&amp;l:event:duration=10104&amp;l:event:playhead=40827&amp;l:event:prev_ts=1673313024834&amp;s:event:type=play&amp;l:event:ts=1673313034938&amp;s:asset:name=Biden+accused+of+mishandling+classified+documents&amp;l:asset:length=200&amp;s:asset:publisher=foxnews&amp;s:asset:type=main&amp;s:asset:video_id=6318425658112&amp;s:stream:type=vod&amp;l:stream:startup_time=0&amp;l:stream:fps=0&amp;l:stream:bitrate=0&amp;l:stream:dropped_frames=0.</t>
         </is>
       </c>
     </row>
@@ -4213,7 +4213,7 @@
       </c>
       <c r="B173" t="inlineStr">
         <is>
-          <t>'l</t>
+          <t>parameter found.</t>
         </is>
       </c>
       <c r="C173" t="inlineStr">
@@ -4223,7 +4223,7 @@
       </c>
       <c r="D173" t="inlineStr">
         <is>
-          <t>Pass: 'l:event:ts' parameter found.</t>
+          <t>Pass: 'l:event:duration' parameter found.</t>
         </is>
       </c>
     </row>
@@ -4235,7 +4235,7 @@
       </c>
       <c r="B174" t="inlineStr">
         <is>
-          <t>'s</t>
+          <t>parameter found.</t>
         </is>
       </c>
       <c r="C174" t="inlineStr">
@@ -4245,7 +4245,7 @@
       </c>
       <c r="D174" t="inlineStr">
         <is>
-          <t>Pass: 's:asset:name' parameter found.</t>
+          <t>Pass: 'l:event:prev_ts' parameter found.</t>
         </is>
       </c>
     </row>
@@ -4257,7 +4257,7 @@
       </c>
       <c r="B175" t="inlineStr">
         <is>
-          <t>'l</t>
+          <t>parameter found.</t>
         </is>
       </c>
       <c r="C175" t="inlineStr">
@@ -4267,7 +4267,7 @@
       </c>
       <c r="D175" t="inlineStr">
         <is>
-          <t>Pass: 'l:asset:length' parameter found.</t>
+          <t>Pass: 'l:event:ts' parameter found.</t>
         </is>
       </c>
     </row>
@@ -4279,7 +4279,7 @@
       </c>
       <c r="B176" t="inlineStr">
         <is>
-          <t>'s</t>
+          <t>parameter found.</t>
         </is>
       </c>
       <c r="C176" t="inlineStr">
@@ -4289,7 +4289,7 @@
       </c>
       <c r="D176" t="inlineStr">
         <is>
-          <t>Pass: 's:asset:publisher' parameter found.</t>
+          <t>Pass: 's:asset:name' parameter found.</t>
         </is>
       </c>
     </row>
@@ -4301,7 +4301,7 @@
       </c>
       <c r="B177" t="inlineStr">
         <is>
-          <t>'s</t>
+          <t>parameter found.</t>
         </is>
       </c>
       <c r="C177" t="inlineStr">
@@ -4311,7 +4311,7 @@
       </c>
       <c r="D177" t="inlineStr">
         <is>
-          <t>Pass: 's:asset:type' parameter found.</t>
+          <t>Pass: 'l:asset:length' parameter found.</t>
         </is>
       </c>
     </row>
@@ -4323,7 +4323,7 @@
       </c>
       <c r="B178" t="inlineStr">
         <is>
-          <t>'s</t>
+          <t>parameter found.</t>
         </is>
       </c>
       <c r="C178" t="inlineStr">
@@ -4332,6 +4332,50 @@
         </is>
       </c>
       <c r="D178" t="inlineStr">
+        <is>
+          <t>Pass: 's:asset:publisher' parameter found.</t>
+        </is>
+      </c>
+    </row>
+    <row r="179">
+      <c r="A179" t="inlineStr">
+        <is>
+          <t>http://foxnews.hb.omtrdc.net/?s:sc:rsid=foxnewsglobalproduction&amp;s:sc:tracking_server=smetrics.foxnews.com&amp;h:sc:ssl=1&amp;s:user:mid=69099319612994832056547930341105758682&amp;&amp;&amp;s:sp:ovp=Akamai&amp;s:sp:channel=Fox+News&amp;s:sp:player_name=Fox+News+Android+Player&amp;s:sp:hb_version=android-2.1.0.154-42fb90&amp;l:sp:hb_api_lvl=4&amp;s:event:sid=1673312989776217636246&amp;l:event:duration=10104&amp;l:event:playhead=40827&amp;l:event:prev_ts=1673313024834&amp;s:event:type=play&amp;l:event:ts=1673313034938&amp;s:asset:name=Biden+accused+of+mishandling+classified+documents&amp;l:asset:length=200&amp;s:asset:publisher=foxnews&amp;s:asset:type=main&amp;s:asset:video_id=6318425658112&amp;s:stream:type=vod&amp;l:stream:startup_time=0&amp;l:stream:fps=0&amp;l:stream:bitrate=0&amp;l:stream:dropped_frames=0</t>
+        </is>
+      </c>
+      <c r="B179" t="inlineStr">
+        <is>
+          <t>parameter found.</t>
+        </is>
+      </c>
+      <c r="C179" t="inlineStr">
+        <is>
+          <t>Pass</t>
+        </is>
+      </c>
+      <c r="D179" t="inlineStr">
+        <is>
+          <t>Pass: 's:asset:type' parameter found.</t>
+        </is>
+      </c>
+    </row>
+    <row r="180">
+      <c r="A180" t="inlineStr">
+        <is>
+          <t>http://foxnews.hb.omtrdc.net/?s:sc:rsid=foxnewsglobalproduction&amp;s:sc:tracking_server=smetrics.foxnews.com&amp;h:sc:ssl=1&amp;s:user:mid=69099319612994832056547930341105758682&amp;&amp;&amp;s:sp:ovp=Akamai&amp;s:sp:channel=Fox+News&amp;s:sp:player_name=Fox+News+Android+Player&amp;s:sp:hb_version=android-2.1.0.154-42fb90&amp;l:sp:hb_api_lvl=4&amp;s:event:sid=1673312989776217636246&amp;l:event:duration=10104&amp;l:event:playhead=40827&amp;l:event:prev_ts=1673313024834&amp;s:event:type=play&amp;l:event:ts=1673313034938&amp;s:asset:name=Biden+accused+of+mishandling+classified+documents&amp;l:asset:length=200&amp;s:asset:publisher=foxnews&amp;s:asset:type=main&amp;s:asset:video_id=6318425658112&amp;s:stream:type=vod&amp;l:stream:startup_time=0&amp;l:stream:fps=0&amp;l:stream:bitrate=0&amp;l:stream:dropped_frames=0</t>
+        </is>
+      </c>
+      <c r="B180" t="inlineStr">
+        <is>
+          <t>parameter found with value foxnewsglobalproduction. URL: http://foxnews.hb.omtrdc.net/?s:sc:rsid=foxnewsglobalproduction&amp;s:sc:tracking_server=smetrics.foxnews.com&amp;h:sc:ssl=1&amp;s:user:mid=69099319612994832056547930341105758682&amp;&amp;&amp;s:sp:ovp=Akamai&amp;s:sp:channel=Fox+News&amp;s:sp:player_name=Fox+News+Android+Player&amp;s:sp:hb_version=android-2.1.0.154-42fb90&amp;l:sp:hb_api_lvl=4&amp;s:event:sid=1673312989776217636246&amp;l:event:duration=10104&amp;l:event:playhead=40827&amp;l:event:prev_ts=1673313024834&amp;s:event:type=play&amp;l:event:ts=1673313034938&amp;s:asset:name=Biden+accused+of+mishandling+classified+documents&amp;l:asset:length=200&amp;s:asset:publisher=foxnews&amp;s:asset:type=main&amp;s:asset:video_id=6318425658112&amp;s:stream:type=vod&amp;l:stream:startup_time=0&amp;l:stream:fps=0&amp;l:stream:bitrate=0&amp;l:stream:dropped_frames=0.</t>
+        </is>
+      </c>
+      <c r="C180" t="inlineStr">
+        <is>
+          <t>Pass</t>
+        </is>
+      </c>
+      <c r="D180" t="inlineStr">
         <is>
           <t>Pass: 's:sc:rsid' parameter found with value foxnewsglobalproduction. URL: http://foxnews.hb.omtrdc.net/?s:sc:rsid=foxnewsglobalproduction&amp;s:sc:tracking_server=smetrics.foxnews.com&amp;h:sc:ssl=1&amp;s:user:mid=69099319612994832056547930341105758682&amp;&amp;&amp;s:sp:ovp=Akamai&amp;s:sp:channel=Fox+News&amp;s:sp:player_name=Fox+News+Android+Player&amp;s:sp:hb_version=android-2.1.0.154-42fb90&amp;l:sp:hb_api_lvl=4&amp;s:event:sid=1673312989776217636246&amp;l:event:duration=10104&amp;l:event:playhead=40827&amp;l:event:prev_ts=1673313024834&amp;s:event:type=play&amp;l:event:ts=1673313034938&amp;s:asset:name=Biden+accused+of+mishandling+classified+documents&amp;l:asset:length=200&amp;s:asset:publisher=foxnews&amp;s:asset:type=main&amp;s:asset:video_id=6318425658112&amp;s:stream:type=vod&amp;l:stream:startup_time=0&amp;l:stream:fps=0&amp;l:stream:bitrate=0&amp;l:stream:dropped_frames=0.</t>
         </is>

</xml_diff>

<commit_message>
Fix result structure and parameter extraction
</commit_message>
<xml_diff>
--- a/harmony_test_results.xlsx
+++ b/harmony_test_results.xlsx
@@ -451,7 +451,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>parameter missing. URL: http://foxnews.hb.omtrdc.net/settings/foxnews.xml?r=1673312989724. Please add the</t>
+          <t>s:event:type</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -473,7 +473,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>parameter missing. URL: http://foxnews.hb.omtrdc.net/settings/foxnews.xml?r=1673312989724. Please add the</t>
+          <t>s:event:type</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -495,7 +495,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>parameter missing. URL: http://foxnews.hb.omtrdc.net/settings/foxnews.xml?r=1673312989724. Please add this parameter.</t>
+          <t>s:event:sid</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -517,7 +517,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>parameter missing. Please add this parameter.</t>
+          <t>l:event:duration</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -539,7 +539,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>parameter missing. Please add this parameter.</t>
+          <t>l:event:prev_ts</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -561,7 +561,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>parameter missing. Please add this parameter.</t>
+          <t>l:event:ts</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -583,7 +583,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>parameter missing. Please add this parameter.</t>
+          <t>s:asset:name</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -605,7 +605,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>parameter missing. Please add this parameter.</t>
+          <t>l:asset:length</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -627,7 +627,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>parameter missing. Please add this parameter.</t>
+          <t>s:asset:publisher</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -649,7 +649,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>parameter missing. Please add this parameter.</t>
+          <t>s:asset:type</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -671,7 +671,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>parameter missing. URL: http://foxnews.hb.omtrdc.net/settings/foxnews.xml?r=1673312989724. Please add the</t>
+          <t>s:sc:rsid</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -693,7 +693,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>parameter found with value start. URL: http://foxnews.hb.omtrdc.net/?s:sc:rsid=foxnewsglobalproduction&amp;s:sc:tracking_server=smetrics.foxnews.com&amp;h:sc:ssl=1&amp;&amp;&amp;&amp;s:sp:ovp=Akamai&amp;s:sp:channel=Fox+News&amp;s:sp:player_name=Fox+News+Android+Player&amp;s:sp:hb_version=android-2.1.0.154-42fb90&amp;l:sp:hb_api_lvl=4&amp;s:event:sid=1673312989776217636246&amp;l:event:duration=0&amp;l:event:playhead=0&amp;l:event:prev_ts=-1&amp;s:event:type=start&amp;l:event:ts=1673312989797&amp;s:asset:name=Biden+accused+of+mishandling+classified+documents&amp;l:asset:length=200&amp;s:asset:publisher=foxnews&amp;s:asset:type=main&amp;s:asset:video_id=6318425658112&amp;s:stream:type=vod&amp;l:stream:startup_time=0&amp;l:stream:fps=0&amp;l:stream:bitrate=0&amp;l:stream:dropped_frames=0&amp;s:meta:a.media.asset=6318425658112&amp;s:meta:streamType=vod&amp;s:meta:length=200&amp;s:meta:app_id=Fox+News+amazon+tv+4.57.0+%282022121901%29&amp;s:meta:a.media.pass.mvpd=&amp;s:meta:s%3Aasset%3Aname=Biden+accused+of+mishandling+classified+documents&amp;s:meta:video_id=6318425658112&amp;s:meta:a.media.network=Fox+News.</t>
+          <t>s:event:type</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -715,7 +715,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>parameter found with value start. URL: http://foxnews.hb.omtrdc.net/?s:sc:rsid=foxnewsglobalproduction&amp;s:sc:tracking_server=smetrics.foxnews.com&amp;h:sc:ssl=1&amp;&amp;&amp;&amp;s:sp:ovp=Akamai&amp;s:sp:channel=Fox+News&amp;s:sp:player_name=Fox+News+Android+Player&amp;s:sp:hb_version=android-2.1.0.154-42fb90&amp;l:sp:hb_api_lvl=4&amp;s:event:sid=1673312989776217636246&amp;l:event:duration=0&amp;l:event:playhead=0&amp;l:event:prev_ts=-1&amp;s:event:type=start&amp;l:event:ts=1673312989797&amp;s:asset:name=Biden+accused+of+mishandling+classified+documents&amp;l:asset:length=200&amp;s:asset:publisher=foxnews&amp;s:asset:type=main&amp;s:asset:video_id=6318425658112&amp;s:stream:type=vod&amp;l:stream:startup_time=0&amp;l:stream:fps=0&amp;l:stream:bitrate=0&amp;l:stream:dropped_frames=0&amp;s:meta:a.media.asset=6318425658112&amp;s:meta:streamType=vod&amp;s:meta:length=200&amp;s:meta:app_id=Fox+News+amazon+tv+4.57.0+%282022121901%29&amp;s:meta:a.media.pass.mvpd=&amp;s:meta:s%3Aasset%3Aname=Biden+accused+of+mishandling+classified+documents&amp;s:meta:video_id=6318425658112&amp;s:meta:a.media.network=Fox+News.</t>
+          <t>s:event:type</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -737,7 +737,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>parameter found. URL: http://foxnews.hb.omtrdc.net/?s:sc:rsid=foxnewsglobalproduction&amp;s:sc:tracking_server=smetrics.foxnews.com&amp;h:sc:ssl=1&amp;&amp;&amp;&amp;s:sp:ovp=Akamai&amp;s:sp:channel=Fox+News&amp;s:sp:player_name=Fox+News+Android+Player&amp;s:sp:hb_version=android-2.1.0.154-42fb90&amp;l:sp:hb_api_lvl=4&amp;s:event:sid=1673312989776217636246&amp;l:event:duration=0&amp;l:event:playhead=0&amp;l:event:prev_ts=-1&amp;s:event:type=start&amp;l:event:ts=1673312989797&amp;s:asset:name=Biden+accused+of+mishandling+classified+documents&amp;l:asset:length=200&amp;s:asset:publisher=foxnews&amp;s:asset:type=main&amp;s:asset:video_id=6318425658112&amp;s:stream:type=vod&amp;l:stream:startup_time=0&amp;l:stream:fps=0&amp;l:stream:bitrate=0&amp;l:stream:dropped_frames=0&amp;s:meta:a.media.asset=6318425658112&amp;s:meta:streamType=vod&amp;s:meta:length=200&amp;s:meta:app_id=Fox+News+amazon+tv+4.57.0+%282022121901%29&amp;s:meta:a.media.pass.mvpd=&amp;s:meta:s%3Aasset%3Aname=Biden+accused+of+mishandling+classified+documents&amp;s:meta:video_id=6318425658112&amp;s:meta:a.media.network=Fox+News.</t>
+          <t>s:event:sid</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -759,7 +759,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>parameter found.</t>
+          <t>l:event:duration</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -781,7 +781,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>parameter found.</t>
+          <t>l:event:prev_ts</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
@@ -803,7 +803,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>parameter found.</t>
+          <t>l:event:ts</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
@@ -825,7 +825,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>parameter found.</t>
+          <t>s:asset:name</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
@@ -847,7 +847,7 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>parameter found.</t>
+          <t>l:asset:length</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
@@ -869,7 +869,7 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>parameter found.</t>
+          <t>s:asset:publisher</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
@@ -891,7 +891,7 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>parameter found.</t>
+          <t>s:asset:type</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
@@ -913,7 +913,7 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>parameter found with value foxnewsglobalproduction. URL: http://foxnews.hb.omtrdc.net/?s:sc:rsid=foxnewsglobalproduction&amp;s:sc:tracking_server=smetrics.foxnews.com&amp;h:sc:ssl=1&amp;&amp;&amp;&amp;s:sp:ovp=Akamai&amp;s:sp:channel=Fox+News&amp;s:sp:player_name=Fox+News+Android+Player&amp;s:sp:hb_version=android-2.1.0.154-42fb90&amp;l:sp:hb_api_lvl=4&amp;s:event:sid=1673312989776217636246&amp;l:event:duration=0&amp;l:event:playhead=0&amp;l:event:prev_ts=-1&amp;s:event:type=start&amp;l:event:ts=1673312989797&amp;s:asset:name=Biden+accused+of+mishandling+classified+documents&amp;l:asset:length=200&amp;s:asset:publisher=foxnews&amp;s:asset:type=main&amp;s:asset:video_id=6318425658112&amp;s:stream:type=vod&amp;l:stream:startup_time=0&amp;l:stream:fps=0&amp;l:stream:bitrate=0&amp;l:stream:dropped_frames=0&amp;s:meta:a.media.asset=6318425658112&amp;s:meta:streamType=vod&amp;s:meta:length=200&amp;s:meta:app_id=Fox+News+amazon+tv+4.57.0+%282022121901%29&amp;s:meta:a.media.pass.mvpd=&amp;s:meta:s%3Aasset%3Aname=Biden+accused+of+mishandling+classified+documents&amp;s:meta:video_id=6318425658112&amp;s:meta:a.media.network=Fox+News.</t>
+          <t>s:sc:rsid</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
@@ -935,7 +935,7 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>parameter found with value start. URL: http://foxnews.hb.omtrdc.net/?s:sc:rsid=foxnewsglobalproduction&amp;s:sc:tracking_server=smetrics.foxnews.com&amp;h:sc:ssl=1&amp;&amp;&amp;&amp;s:sp:ovp=Akamai&amp;s:sp:channel=Fox+News&amp;s:sp:player_name=Fox+News+Android+Player&amp;s:sp:hb_version=android-2.1.0.154-42fb90&amp;l:sp:hb_api_lvl=4&amp;s:event:sid=1673312989776217636246&amp;l:event:duration=45&amp;l:event:playhead=0&amp;l:event:prev_ts=1673312989797&amp;s:event:type=start&amp;l:event:ts=1673312989842&amp;s:asset:name=Biden+accused+of+mishandling+classified+documents&amp;l:asset:length=200&amp;s:asset:publisher=foxnews&amp;s:asset:type=main&amp;s:asset:video_id=6318425658112&amp;s:stream:type=vod&amp;l:stream:startup_time=0&amp;l:stream:fps=0&amp;l:stream:bitrate=0&amp;l:stream:dropped_frames=0&amp;s:meta:a.media.asset=6318425658112&amp;s:meta:streamType=vod&amp;s:meta:length=200&amp;s:meta:app_id=Fox+News+amazon+tv+4.57.0+%282022121901%29&amp;s:meta:a.media.pass.mvpd=&amp;s:meta:s%3Aasset%3Aname=Biden+accused+of+mishandling+classified+documents&amp;s:meta:video_id=6318425658112&amp;s:meta:a.media.network=Fox+News.</t>
+          <t>s:event:type</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
@@ -957,7 +957,7 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>parameter found with value start. URL: http://foxnews.hb.omtrdc.net/?s:sc:rsid=foxnewsglobalproduction&amp;s:sc:tracking_server=smetrics.foxnews.com&amp;h:sc:ssl=1&amp;&amp;&amp;&amp;s:sp:ovp=Akamai&amp;s:sp:channel=Fox+News&amp;s:sp:player_name=Fox+News+Android+Player&amp;s:sp:hb_version=android-2.1.0.154-42fb90&amp;l:sp:hb_api_lvl=4&amp;s:event:sid=1673312989776217636246&amp;l:event:duration=45&amp;l:event:playhead=0&amp;l:event:prev_ts=1673312989797&amp;s:event:type=start&amp;l:event:ts=1673312989842&amp;s:asset:name=Biden+accused+of+mishandling+classified+documents&amp;l:asset:length=200&amp;s:asset:publisher=foxnews&amp;s:asset:type=main&amp;s:asset:video_id=6318425658112&amp;s:stream:type=vod&amp;l:stream:startup_time=0&amp;l:stream:fps=0&amp;l:stream:bitrate=0&amp;l:stream:dropped_frames=0&amp;s:meta:a.media.asset=6318425658112&amp;s:meta:streamType=vod&amp;s:meta:length=200&amp;s:meta:app_id=Fox+News+amazon+tv+4.57.0+%282022121901%29&amp;s:meta:a.media.pass.mvpd=&amp;s:meta:s%3Aasset%3Aname=Biden+accused+of+mishandling+classified+documents&amp;s:meta:video_id=6318425658112&amp;s:meta:a.media.network=Fox+News.</t>
+          <t>s:event:type</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
@@ -979,7 +979,7 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>parameter found. URL: http://foxnews.hb.omtrdc.net/?s:sc:rsid=foxnewsglobalproduction&amp;s:sc:tracking_server=smetrics.foxnews.com&amp;h:sc:ssl=1&amp;&amp;&amp;&amp;s:sp:ovp=Akamai&amp;s:sp:channel=Fox+News&amp;s:sp:player_name=Fox+News+Android+Player&amp;s:sp:hb_version=android-2.1.0.154-42fb90&amp;l:sp:hb_api_lvl=4&amp;s:event:sid=1673312989776217636246&amp;l:event:duration=45&amp;l:event:playhead=0&amp;l:event:prev_ts=1673312989797&amp;s:event:type=start&amp;l:event:ts=1673312989842&amp;s:asset:name=Biden+accused+of+mishandling+classified+documents&amp;l:asset:length=200&amp;s:asset:publisher=foxnews&amp;s:asset:type=main&amp;s:asset:video_id=6318425658112&amp;s:stream:type=vod&amp;l:stream:startup_time=0&amp;l:stream:fps=0&amp;l:stream:bitrate=0&amp;l:stream:dropped_frames=0&amp;s:meta:a.media.asset=6318425658112&amp;s:meta:streamType=vod&amp;s:meta:length=200&amp;s:meta:app_id=Fox+News+amazon+tv+4.57.0+%282022121901%29&amp;s:meta:a.media.pass.mvpd=&amp;s:meta:s%3Aasset%3Aname=Biden+accused+of+mishandling+classified+documents&amp;s:meta:video_id=6318425658112&amp;s:meta:a.media.network=Fox+News.</t>
+          <t>s:event:sid</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
@@ -1001,7 +1001,7 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>parameter found.</t>
+          <t>l:event:duration</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
@@ -1023,7 +1023,7 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>parameter found.</t>
+          <t>l:event:prev_ts</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
@@ -1045,7 +1045,7 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>parameter found.</t>
+          <t>l:event:ts</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
@@ -1067,7 +1067,7 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>parameter found.</t>
+          <t>s:asset:name</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
@@ -1089,7 +1089,7 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>parameter found.</t>
+          <t>l:asset:length</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
@@ -1111,7 +1111,7 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>parameter found.</t>
+          <t>s:asset:publisher</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
@@ -1133,7 +1133,7 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>parameter found.</t>
+          <t>s:asset:type</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
@@ -1155,7 +1155,7 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>parameter found with value foxnewsglobalproduction. URL: http://foxnews.hb.omtrdc.net/?s:sc:rsid=foxnewsglobalproduction&amp;s:sc:tracking_server=smetrics.foxnews.com&amp;h:sc:ssl=1&amp;&amp;&amp;&amp;s:sp:ovp=Akamai&amp;s:sp:channel=Fox+News&amp;s:sp:player_name=Fox+News+Android+Player&amp;s:sp:hb_version=android-2.1.0.154-42fb90&amp;l:sp:hb_api_lvl=4&amp;s:event:sid=1673312989776217636246&amp;l:event:duration=45&amp;l:event:playhead=0&amp;l:event:prev_ts=1673312989797&amp;s:event:type=start&amp;l:event:ts=1673312989842&amp;s:asset:name=Biden+accused+of+mishandling+classified+documents&amp;l:asset:length=200&amp;s:asset:publisher=foxnews&amp;s:asset:type=main&amp;s:asset:video_id=6318425658112&amp;s:stream:type=vod&amp;l:stream:startup_time=0&amp;l:stream:fps=0&amp;l:stream:bitrate=0&amp;l:stream:dropped_frames=0&amp;s:meta:a.media.asset=6318425658112&amp;s:meta:streamType=vod&amp;s:meta:length=200&amp;s:meta:app_id=Fox+News+amazon+tv+4.57.0+%282022121901%29&amp;s:meta:a.media.pass.mvpd=&amp;s:meta:s%3Aasset%3Aname=Biden+accused+of+mishandling+classified+documents&amp;s:meta:video_id=6318425658112&amp;s:meta:a.media.network=Fox+News.</t>
+          <t>s:sc:rsid</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
@@ -1177,7 +1177,7 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>parameter found with value buffer. URL: http://foxnews.hb.omtrdc.net/?s:sc:rsid=foxnewsglobalproduction&amp;s:sc:tracking_server=smetrics.foxnews.com&amp;h:sc:ssl=1&amp;&amp;&amp;&amp;s:sp:ovp=Akamai&amp;s:sp:channel=Fox+News&amp;s:sp:player_name=Fox+News+Android+Player&amp;s:sp:hb_version=android-2.1.0.154-42fb90&amp;l:sp:hb_api_lvl=4&amp;s:event:sid=1673312989776217636246&amp;l:event:duration=0&amp;l:event:playhead=0&amp;l:event:prev_ts=-1&amp;s:event:type=buffer&amp;l:event:ts=1673312989842&amp;s:asset:name=Biden+accused+of+mishandling+classified+documents&amp;l:asset:length=200&amp;s:asset:publisher=foxnews&amp;s:asset:type=main&amp;s:asset:video_id=6318425658112&amp;s:stream:type=vod&amp;l:stream:startup_time=0&amp;l:stream:fps=0&amp;l:stream:bitrate=0&amp;l:stream:dropped_frames=0.</t>
+          <t>s:event:type</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
@@ -1199,7 +1199,7 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>parameter found with value buffer. URL: http://foxnews.hb.omtrdc.net/?s:sc:rsid=foxnewsglobalproduction&amp;s:sc:tracking_server=smetrics.foxnews.com&amp;h:sc:ssl=1&amp;&amp;&amp;&amp;s:sp:ovp=Akamai&amp;s:sp:channel=Fox+News&amp;s:sp:player_name=Fox+News+Android+Player&amp;s:sp:hb_version=android-2.1.0.154-42fb90&amp;l:sp:hb_api_lvl=4&amp;s:event:sid=1673312989776217636246&amp;l:event:duration=0&amp;l:event:playhead=0&amp;l:event:prev_ts=-1&amp;s:event:type=buffer&amp;l:event:ts=1673312989842&amp;s:asset:name=Biden+accused+of+mishandling+classified+documents&amp;l:asset:length=200&amp;s:asset:publisher=foxnews&amp;s:asset:type=main&amp;s:asset:video_id=6318425658112&amp;s:stream:type=vod&amp;l:stream:startup_time=0&amp;l:stream:fps=0&amp;l:stream:bitrate=0&amp;l:stream:dropped_frames=0.</t>
+          <t>s:event:type</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
@@ -1221,7 +1221,7 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>parameter found. URL: http://foxnews.hb.omtrdc.net/?s:sc:rsid=foxnewsglobalproduction&amp;s:sc:tracking_server=smetrics.foxnews.com&amp;h:sc:ssl=1&amp;&amp;&amp;&amp;s:sp:ovp=Akamai&amp;s:sp:channel=Fox+News&amp;s:sp:player_name=Fox+News+Android+Player&amp;s:sp:hb_version=android-2.1.0.154-42fb90&amp;l:sp:hb_api_lvl=4&amp;s:event:sid=1673312989776217636246&amp;l:event:duration=0&amp;l:event:playhead=0&amp;l:event:prev_ts=-1&amp;s:event:type=buffer&amp;l:event:ts=1673312989842&amp;s:asset:name=Biden+accused+of+mishandling+classified+documents&amp;l:asset:length=200&amp;s:asset:publisher=foxnews&amp;s:asset:type=main&amp;s:asset:video_id=6318425658112&amp;s:stream:type=vod&amp;l:stream:startup_time=0&amp;l:stream:fps=0&amp;l:stream:bitrate=0&amp;l:stream:dropped_frames=0.</t>
+          <t>s:event:sid</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
@@ -1243,7 +1243,7 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>parameter found.</t>
+          <t>l:event:duration</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
@@ -1265,7 +1265,7 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>parameter found.</t>
+          <t>l:event:prev_ts</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
@@ -1287,7 +1287,7 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>parameter found.</t>
+          <t>l:event:ts</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
@@ -1309,7 +1309,7 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>parameter found.</t>
+          <t>s:asset:name</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
@@ -1331,7 +1331,7 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>parameter found.</t>
+          <t>l:asset:length</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
@@ -1353,7 +1353,7 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>parameter found.</t>
+          <t>s:asset:publisher</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
@@ -1375,7 +1375,7 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>parameter found.</t>
+          <t>s:asset:type</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
@@ -1397,7 +1397,7 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>parameter found with value foxnewsglobalproduction. URL: http://foxnews.hb.omtrdc.net/?s:sc:rsid=foxnewsglobalproduction&amp;s:sc:tracking_server=smetrics.foxnews.com&amp;h:sc:ssl=1&amp;&amp;&amp;&amp;s:sp:ovp=Akamai&amp;s:sp:channel=Fox+News&amp;s:sp:player_name=Fox+News+Android+Player&amp;s:sp:hb_version=android-2.1.0.154-42fb90&amp;l:sp:hb_api_lvl=4&amp;s:event:sid=1673312989776217636246&amp;l:event:duration=0&amp;l:event:playhead=0&amp;l:event:prev_ts=-1&amp;s:event:type=buffer&amp;l:event:ts=1673312989842&amp;s:asset:name=Biden+accused+of+mishandling+classified+documents&amp;l:asset:length=200&amp;s:asset:publisher=foxnews&amp;s:asset:type=main&amp;s:asset:video_id=6318425658112&amp;s:stream:type=vod&amp;l:stream:startup_time=0&amp;l:stream:fps=0&amp;l:stream:bitrate=0&amp;l:stream:dropped_frames=0.</t>
+          <t>s:sc:rsid</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
@@ -1419,7 +1419,7 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>parameter missing. URL: https://smetrics.foxnews.com/id?mid=69099319612994832056547930341105758682&amp;mcorgid=foxnews. Please add the</t>
+          <t>app_build</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
@@ -1441,7 +1441,7 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>parameter missing. URL: https://smetrics.foxnews.com/id?mid=69099319612994832056547930341105758682&amp;mcorgid=foxnews. Please add the</t>
+          <t>app_name</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
@@ -1463,7 +1463,7 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>parameter missing. URL: https://smetrics.foxnews.com/id?mid=69099319612994832056547930341105758682&amp;mcorgid=foxnews. Please add the</t>
+          <t>app_version</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
@@ -1485,7 +1485,7 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>parameter missing. URL: https://smetrics.foxnews.com/id?mid=69099319612994832056547930341105758682&amp;mcorgid=foxnews. Please add the</t>
+          <t>s:event:type</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
@@ -1507,7 +1507,7 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>parameter missing. URL: https://smetrics.foxnews.com/id?mid=69099319612994832056547930341105758682&amp;mcorgid=foxnews. Please add the</t>
+          <t>s:event:type</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
@@ -1529,7 +1529,7 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>parameter missing. URL: https://smetrics.foxnews.com/id?mid=69099319612994832056547930341105758682&amp;mcorgid=foxnews. Please add this parameter.</t>
+          <t>s:event:sid</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
@@ -1551,7 +1551,7 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>parameter missing. Please add this parameter.</t>
+          <t>l:event:duration</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
@@ -1573,7 +1573,7 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>parameter missing. Please add this parameter.</t>
+          <t>l:event:playhead</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
@@ -1595,7 +1595,7 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>parameter missing. Please add this parameter.</t>
+          <t>l:event:prev_ts</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
@@ -1617,7 +1617,7 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>parameter missing. Please add this parameter.</t>
+          <t>l:event:ts</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
@@ -1639,7 +1639,7 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>parameter missing. Please add this parameter.</t>
+          <t>s:asset:name</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
@@ -1661,7 +1661,7 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>parameter missing. Please add this parameter.</t>
+          <t>l:asset:length</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
@@ -1683,7 +1683,7 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>parameter missing. Please add this parameter.</t>
+          <t>s:asset:publisher</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
@@ -1705,7 +1705,7 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>parameter missing. Please add this parameter.</t>
+          <t>s:asset:type</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
@@ -1727,7 +1727,7 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>variations found with value 69099319612994832056547930341105758682. URL: https://smetrics.foxnews.com/id?mid=69099319612994832056547930341105758682&amp;mcorgid=foxnews.</t>
+          <t>mid</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
@@ -1749,7 +1749,7 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>parameter missing. URL: https://smetrics.foxnews.com/id?mid=69099319612994832056547930341105758682&amp;mcorgid=foxnews. Please add the</t>
+          <t>page_type</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
@@ -1771,7 +1771,7 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>parameter missing. URL: https://smetrics.foxnews.com/id?mid=69099319612994832056547930341105758682&amp;mcorgid=foxnews. Please add the</t>
+          <t>primary_business_unit</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
@@ -1793,7 +1793,7 @@
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>parameter missing. Please add the</t>
+          <t>user_fox_anonymous_profile_id</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
@@ -1815,7 +1815,7 @@
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>parameter missing. URL: https://smetrics.foxnews.com/b/ss/foxnewsglobalproduction/0/JAVA-4.17.9-AN/s40450848. Please add the</t>
+          <t>app_build</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
@@ -1837,7 +1837,7 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>parameter missing. URL: https://smetrics.foxnews.com/b/ss/foxnewsglobalproduction/0/JAVA-4.17.9-AN/s40450848. Please add the</t>
+          <t>app_name</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
@@ -1859,7 +1859,7 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>parameter missing. URL: https://smetrics.foxnews.com/b/ss/foxnewsglobalproduction/0/JAVA-4.17.9-AN/s40450848. Please add the</t>
+          <t>app_version</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
@@ -1881,7 +1881,7 @@
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>parameter missing. URL: https://smetrics.foxnews.com/b/ss/foxnewsglobalproduction/0/JAVA-4.17.9-AN/s40450848. Please add the</t>
+          <t>s:event:type</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
@@ -1903,7 +1903,7 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>parameter missing. URL: https://smetrics.foxnews.com/b/ss/foxnewsglobalproduction/0/JAVA-4.17.9-AN/s40450848. Please add the</t>
+          <t>s:event:type</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
@@ -1925,7 +1925,7 @@
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>parameter missing. URL: https://smetrics.foxnews.com/b/ss/foxnewsglobalproduction/0/JAVA-4.17.9-AN/s40450848. Please add this parameter.</t>
+          <t>s:event:sid</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
@@ -1947,7 +1947,7 @@
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>parameter missing. Please add this parameter.</t>
+          <t>l:event:duration</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
@@ -1969,7 +1969,7 @@
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>parameter missing. Please add this parameter.</t>
+          <t>l:event:playhead</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
@@ -1991,7 +1991,7 @@
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>parameter missing. Please add this parameter.</t>
+          <t>l:event:prev_ts</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
@@ -2013,7 +2013,7 @@
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>parameter missing. Please add this parameter.</t>
+          <t>l:event:ts</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
@@ -2035,7 +2035,7 @@
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>parameter missing. Please add this parameter.</t>
+          <t>s:asset:name</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
@@ -2057,7 +2057,7 @@
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>parameter missing. Please add this parameter.</t>
+          <t>l:asset:length</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
@@ -2079,7 +2079,7 @@
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>parameter missing. Please add this parameter.</t>
+          <t>s:asset:publisher</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
@@ -2101,7 +2101,7 @@
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>parameter missing. Please add this parameter.</t>
+          <t>s:asset:type</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
@@ -2123,7 +2123,7 @@
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>variations found with value 69099319612994832056547930341105758682. URL: https://smetrics.foxnews.com/b/ss/foxnewsglobalproduction/0/JAVA-4.17.9-AN/s40450848.</t>
+          <t>mid</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
@@ -2145,7 +2145,7 @@
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>parameter missing. URL: https://smetrics.foxnews.com/b/ss/foxnewsglobalproduction/0/JAVA-4.17.9-AN/s40450848. Please add the</t>
+          <t>page_type</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
@@ -2167,7 +2167,7 @@
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>parameter missing. URL: https://smetrics.foxnews.com/b/ss/foxnewsglobalproduction/0/JAVA-4.17.9-AN/s40450848. Please add the</t>
+          <t>primary_business_unit</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
@@ -2189,7 +2189,7 @@
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>parameter missing. Please add the</t>
+          <t>user_fox_anonymous_profile_id</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
@@ -2211,7 +2211,7 @@
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>parameter found with value aa_start. URL: http://foxnews.hb.omtrdc.net/?s:sc:rsid=foxnewsglobalproduction&amp;s:sc:tracking_server=smetrics.foxnews.com&amp;h:sc:ssl=1&amp;s:user:mid=69099319612994832056547930341105758682&amp;&amp;&amp;s:sp:ovp=Akamai&amp;s:sp:channel=Fox+News&amp;s:sp:player_name=Fox+News+Android+Player&amp;s:sp:hb_version=android-2.1.0.154-42fb90&amp;l:sp:hb_api_lvl=4&amp;s:event:sid=1673312989776217636246&amp;l:event:duration=0&amp;l:event:playhead=0&amp;l:event:prev_ts=-1&amp;s:event:type=aa_start&amp;l:event:ts=1673312991238&amp;s:asset:name=Biden+accused+of+mishandling+classified+documents&amp;l:asset:length=200&amp;s:asset:publisher=foxnews&amp;s:asset:type=main&amp;s:asset:video_id=6318425658112&amp;s:stream:type=vod&amp;l:stream:startup_time=0&amp;l:stream:fps=0&amp;l:stream:bitrate=0&amp;l:stream:dropped_frames=0.</t>
+          <t>s:event:type</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
@@ -2233,7 +2233,7 @@
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>parameter found with value aa_start. URL: http://foxnews.hb.omtrdc.net/?s:sc:rsid=foxnewsglobalproduction&amp;s:sc:tracking_server=smetrics.foxnews.com&amp;h:sc:ssl=1&amp;s:user:mid=69099319612994832056547930341105758682&amp;&amp;&amp;s:sp:ovp=Akamai&amp;s:sp:channel=Fox+News&amp;s:sp:player_name=Fox+News+Android+Player&amp;s:sp:hb_version=android-2.1.0.154-42fb90&amp;l:sp:hb_api_lvl=4&amp;s:event:sid=1673312989776217636246&amp;l:event:duration=0&amp;l:event:playhead=0&amp;l:event:prev_ts=-1&amp;s:event:type=aa_start&amp;l:event:ts=1673312991238&amp;s:asset:name=Biden+accused+of+mishandling+classified+documents&amp;l:asset:length=200&amp;s:asset:publisher=foxnews&amp;s:asset:type=main&amp;s:asset:video_id=6318425658112&amp;s:stream:type=vod&amp;l:stream:startup_time=0&amp;l:stream:fps=0&amp;l:stream:bitrate=0&amp;l:stream:dropped_frames=0.</t>
+          <t>s:event:type</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
@@ -2255,7 +2255,7 @@
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>parameter found. URL: http://foxnews.hb.omtrdc.net/?s:sc:rsid=foxnewsglobalproduction&amp;s:sc:tracking_server=smetrics.foxnews.com&amp;h:sc:ssl=1&amp;s:user:mid=69099319612994832056547930341105758682&amp;&amp;&amp;s:sp:ovp=Akamai&amp;s:sp:channel=Fox+News&amp;s:sp:player_name=Fox+News+Android+Player&amp;s:sp:hb_version=android-2.1.0.154-42fb90&amp;l:sp:hb_api_lvl=4&amp;s:event:sid=1673312989776217636246&amp;l:event:duration=0&amp;l:event:playhead=0&amp;l:event:prev_ts=-1&amp;s:event:type=aa_start&amp;l:event:ts=1673312991238&amp;s:asset:name=Biden+accused+of+mishandling+classified+documents&amp;l:asset:length=200&amp;s:asset:publisher=foxnews&amp;s:asset:type=main&amp;s:asset:video_id=6318425658112&amp;s:stream:type=vod&amp;l:stream:startup_time=0&amp;l:stream:fps=0&amp;l:stream:bitrate=0&amp;l:stream:dropped_frames=0.</t>
+          <t>s:event:sid</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
@@ -2277,7 +2277,7 @@
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>parameter found.</t>
+          <t>l:event:duration</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
@@ -2299,7 +2299,7 @@
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>parameter found.</t>
+          <t>l:event:prev_ts</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
@@ -2321,7 +2321,7 @@
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>parameter found.</t>
+          <t>l:event:ts</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
@@ -2343,7 +2343,7 @@
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>parameter found.</t>
+          <t>s:asset:name</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
@@ -2365,7 +2365,7 @@
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>parameter found.</t>
+          <t>l:asset:length</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
@@ -2387,7 +2387,7 @@
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>parameter found.</t>
+          <t>s:asset:publisher</t>
         </is>
       </c>
       <c r="C90" t="inlineStr">
@@ -2409,7 +2409,7 @@
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>parameter found.</t>
+          <t>s:asset:type</t>
         </is>
       </c>
       <c r="C91" t="inlineStr">
@@ -2431,7 +2431,7 @@
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>parameter found with value foxnewsglobalproduction. URL: http://foxnews.hb.omtrdc.net/?s:sc:rsid=foxnewsglobalproduction&amp;s:sc:tracking_server=smetrics.foxnews.com&amp;h:sc:ssl=1&amp;s:user:mid=69099319612994832056547930341105758682&amp;&amp;&amp;s:sp:ovp=Akamai&amp;s:sp:channel=Fox+News&amp;s:sp:player_name=Fox+News+Android+Player&amp;s:sp:hb_version=android-2.1.0.154-42fb90&amp;l:sp:hb_api_lvl=4&amp;s:event:sid=1673312989776217636246&amp;l:event:duration=0&amp;l:event:playhead=0&amp;l:event:prev_ts=-1&amp;s:event:type=aa_start&amp;l:event:ts=1673312991238&amp;s:asset:name=Biden+accused+of+mishandling+classified+documents&amp;l:asset:length=200&amp;s:asset:publisher=foxnews&amp;s:asset:type=main&amp;s:asset:video_id=6318425658112&amp;s:stream:type=vod&amp;l:stream:startup_time=0&amp;l:stream:fps=0&amp;l:stream:bitrate=0&amp;l:stream:dropped_frames=0.</t>
+          <t>s:sc:rsid</t>
         </is>
       </c>
       <c r="C92" t="inlineStr">
@@ -2453,7 +2453,7 @@
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>parameter found with value buffer. URL: http://foxnews.hb.omtrdc.net/?s:sc:rsid=foxnewsglobalproduction&amp;s:sc:tracking_server=smetrics.foxnews.com&amp;h:sc:ssl=1&amp;s:user:mid=69099319612994832056547930341105758682&amp;&amp;&amp;s:sp:ovp=Akamai&amp;s:sp:channel=Fox+News&amp;s:sp:player_name=Fox+News+Android+Player&amp;s:sp:hb_version=android-2.1.0.154-42fb90&amp;l:sp:hb_api_lvl=4&amp;s:event:sid=1673312989776217636246&amp;l:event:duration=3908&amp;l:event:playhead=0&amp;l:event:prev_ts=1673312989842&amp;s:event:type=buffer&amp;l:event:ts=1673312993750&amp;s:asset:name=Biden+accused+of+mishandling+classified+documents&amp;l:asset:length=200&amp;s:asset:publisher=foxnews&amp;s:asset:type=main&amp;s:asset:video_id=6318425658112&amp;s:stream:type=vod&amp;l:stream:startup_time=0&amp;l:stream:fps=0&amp;l:stream:bitrate=0&amp;l:stream:dropped_frames=0.</t>
+          <t>s:event:type</t>
         </is>
       </c>
       <c r="C93" t="inlineStr">
@@ -2475,7 +2475,7 @@
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>parameter found with value buffer. URL: http://foxnews.hb.omtrdc.net/?s:sc:rsid=foxnewsglobalproduction&amp;s:sc:tracking_server=smetrics.foxnews.com&amp;h:sc:ssl=1&amp;s:user:mid=69099319612994832056547930341105758682&amp;&amp;&amp;s:sp:ovp=Akamai&amp;s:sp:channel=Fox+News&amp;s:sp:player_name=Fox+News+Android+Player&amp;s:sp:hb_version=android-2.1.0.154-42fb90&amp;l:sp:hb_api_lvl=4&amp;s:event:sid=1673312989776217636246&amp;l:event:duration=3908&amp;l:event:playhead=0&amp;l:event:prev_ts=1673312989842&amp;s:event:type=buffer&amp;l:event:ts=1673312993750&amp;s:asset:name=Biden+accused+of+mishandling+classified+documents&amp;l:asset:length=200&amp;s:asset:publisher=foxnews&amp;s:asset:type=main&amp;s:asset:video_id=6318425658112&amp;s:stream:type=vod&amp;l:stream:startup_time=0&amp;l:stream:fps=0&amp;l:stream:bitrate=0&amp;l:stream:dropped_frames=0.</t>
+          <t>s:event:type</t>
         </is>
       </c>
       <c r="C94" t="inlineStr">
@@ -2497,7 +2497,7 @@
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>parameter found. URL: http://foxnews.hb.omtrdc.net/?s:sc:rsid=foxnewsglobalproduction&amp;s:sc:tracking_server=smetrics.foxnews.com&amp;h:sc:ssl=1&amp;s:user:mid=69099319612994832056547930341105758682&amp;&amp;&amp;s:sp:ovp=Akamai&amp;s:sp:channel=Fox+News&amp;s:sp:player_name=Fox+News+Android+Player&amp;s:sp:hb_version=android-2.1.0.154-42fb90&amp;l:sp:hb_api_lvl=4&amp;s:event:sid=1673312989776217636246&amp;l:event:duration=3908&amp;l:event:playhead=0&amp;l:event:prev_ts=1673312989842&amp;s:event:type=buffer&amp;l:event:ts=1673312993750&amp;s:asset:name=Biden+accused+of+mishandling+classified+documents&amp;l:asset:length=200&amp;s:asset:publisher=foxnews&amp;s:asset:type=main&amp;s:asset:video_id=6318425658112&amp;s:stream:type=vod&amp;l:stream:startup_time=0&amp;l:stream:fps=0&amp;l:stream:bitrate=0&amp;l:stream:dropped_frames=0.</t>
+          <t>s:event:sid</t>
         </is>
       </c>
       <c r="C95" t="inlineStr">
@@ -2519,7 +2519,7 @@
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>parameter found.</t>
+          <t>l:event:duration</t>
         </is>
       </c>
       <c r="C96" t="inlineStr">
@@ -2541,7 +2541,7 @@
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>parameter found.</t>
+          <t>l:event:prev_ts</t>
         </is>
       </c>
       <c r="C97" t="inlineStr">
@@ -2563,7 +2563,7 @@
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>parameter found.</t>
+          <t>l:event:ts</t>
         </is>
       </c>
       <c r="C98" t="inlineStr">
@@ -2585,7 +2585,7 @@
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>parameter found.</t>
+          <t>s:asset:name</t>
         </is>
       </c>
       <c r="C99" t="inlineStr">
@@ -2607,7 +2607,7 @@
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>parameter found.</t>
+          <t>l:asset:length</t>
         </is>
       </c>
       <c r="C100" t="inlineStr">
@@ -2629,7 +2629,7 @@
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>parameter found.</t>
+          <t>s:asset:publisher</t>
         </is>
       </c>
       <c r="C101" t="inlineStr">
@@ -2651,7 +2651,7 @@
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>parameter found.</t>
+          <t>s:asset:type</t>
         </is>
       </c>
       <c r="C102" t="inlineStr">
@@ -2673,7 +2673,7 @@
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>parameter found with value foxnewsglobalproduction. URL: http://foxnews.hb.omtrdc.net/?s:sc:rsid=foxnewsglobalproduction&amp;s:sc:tracking_server=smetrics.foxnews.com&amp;h:sc:ssl=1&amp;s:user:mid=69099319612994832056547930341105758682&amp;&amp;&amp;s:sp:ovp=Akamai&amp;s:sp:channel=Fox+News&amp;s:sp:player_name=Fox+News+Android+Player&amp;s:sp:hb_version=android-2.1.0.154-42fb90&amp;l:sp:hb_api_lvl=4&amp;s:event:sid=1673312989776217636246&amp;l:event:duration=3908&amp;l:event:playhead=0&amp;l:event:prev_ts=1673312989842&amp;s:event:type=buffer&amp;l:event:ts=1673312993750&amp;s:asset:name=Biden+accused+of+mishandling+classified+documents&amp;l:asset:length=200&amp;s:asset:publisher=foxnews&amp;s:asset:type=main&amp;s:asset:video_id=6318425658112&amp;s:stream:type=vod&amp;l:stream:startup_time=0&amp;l:stream:fps=0&amp;l:stream:bitrate=0&amp;l:stream:dropped_frames=0.</t>
+          <t>s:sc:rsid</t>
         </is>
       </c>
       <c r="C103" t="inlineStr">
@@ -2695,7 +2695,7 @@
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>parameter found with value pause. URL: http://foxnews.hb.omtrdc.net/?s:sc:rsid=foxnewsglobalproduction&amp;s:sc:tracking_server=smetrics.foxnews.com&amp;h:sc:ssl=1&amp;s:user:mid=69099319612994832056547930341105758682&amp;&amp;&amp;s:sp:ovp=Akamai&amp;s:sp:channel=Fox+News&amp;s:sp:player_name=Fox+News+Android+Player&amp;s:sp:hb_version=android-2.1.0.154-42fb90&amp;l:sp:hb_api_lvl=4&amp;s:event:sid=1673312989776217636246&amp;l:event:duration=338&amp;l:event:playhead=227&amp;l:event:prev_ts=-1&amp;s:event:type=pause&amp;l:event:ts=1673312994087&amp;s:asset:name=Biden+accused+of+mishandling+classified+documents&amp;l:asset:length=200&amp;s:asset:publisher=foxnews&amp;s:asset:type=main&amp;s:asset:video_id=6318425658112&amp;s:stream:type=vod&amp;l:stream:startup_time=0&amp;l:stream:fps=0&amp;l:stream:bitrate=0&amp;l:stream:dropped_frames=0.</t>
+          <t>s:event:type</t>
         </is>
       </c>
       <c r="C104" t="inlineStr">
@@ -2717,7 +2717,7 @@
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>parameter found with value pause. URL: http://foxnews.hb.omtrdc.net/?s:sc:rsid=foxnewsglobalproduction&amp;s:sc:tracking_server=smetrics.foxnews.com&amp;h:sc:ssl=1&amp;s:user:mid=69099319612994832056547930341105758682&amp;&amp;&amp;s:sp:ovp=Akamai&amp;s:sp:channel=Fox+News&amp;s:sp:player_name=Fox+News+Android+Player&amp;s:sp:hb_version=android-2.1.0.154-42fb90&amp;l:sp:hb_api_lvl=4&amp;s:event:sid=1673312989776217636246&amp;l:event:duration=338&amp;l:event:playhead=227&amp;l:event:prev_ts=-1&amp;s:event:type=pause&amp;l:event:ts=1673312994087&amp;s:asset:name=Biden+accused+of+mishandling+classified+documents&amp;l:asset:length=200&amp;s:asset:publisher=foxnews&amp;s:asset:type=main&amp;s:asset:video_id=6318425658112&amp;s:stream:type=vod&amp;l:stream:startup_time=0&amp;l:stream:fps=0&amp;l:stream:bitrate=0&amp;l:stream:dropped_frames=0.</t>
+          <t>s:event:type</t>
         </is>
       </c>
       <c r="C105" t="inlineStr">
@@ -2739,7 +2739,7 @@
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>parameter found. URL: http://foxnews.hb.omtrdc.net/?s:sc:rsid=foxnewsglobalproduction&amp;s:sc:tracking_server=smetrics.foxnews.com&amp;h:sc:ssl=1&amp;s:user:mid=69099319612994832056547930341105758682&amp;&amp;&amp;s:sp:ovp=Akamai&amp;s:sp:channel=Fox+News&amp;s:sp:player_name=Fox+News+Android+Player&amp;s:sp:hb_version=android-2.1.0.154-42fb90&amp;l:sp:hb_api_lvl=4&amp;s:event:sid=1673312989776217636246&amp;l:event:duration=338&amp;l:event:playhead=227&amp;l:event:prev_ts=-1&amp;s:event:type=pause&amp;l:event:ts=1673312994087&amp;s:asset:name=Biden+accused+of+mishandling+classified+documents&amp;l:asset:length=200&amp;s:asset:publisher=foxnews&amp;s:asset:type=main&amp;s:asset:video_id=6318425658112&amp;s:stream:type=vod&amp;l:stream:startup_time=0&amp;l:stream:fps=0&amp;l:stream:bitrate=0&amp;l:stream:dropped_frames=0.</t>
+          <t>s:event:sid</t>
         </is>
       </c>
       <c r="C106" t="inlineStr">
@@ -2761,7 +2761,7 @@
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>parameter found.</t>
+          <t>l:event:duration</t>
         </is>
       </c>
       <c r="C107" t="inlineStr">
@@ -2783,7 +2783,7 @@
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>parameter found.</t>
+          <t>l:event:prev_ts</t>
         </is>
       </c>
       <c r="C108" t="inlineStr">
@@ -2805,7 +2805,7 @@
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>parameter found.</t>
+          <t>l:event:ts</t>
         </is>
       </c>
       <c r="C109" t="inlineStr">
@@ -2827,7 +2827,7 @@
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>parameter found.</t>
+          <t>s:asset:name</t>
         </is>
       </c>
       <c r="C110" t="inlineStr">
@@ -2849,7 +2849,7 @@
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>parameter found.</t>
+          <t>l:asset:length</t>
         </is>
       </c>
       <c r="C111" t="inlineStr">
@@ -2871,7 +2871,7 @@
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>parameter found.</t>
+          <t>s:asset:publisher</t>
         </is>
       </c>
       <c r="C112" t="inlineStr">
@@ -2893,7 +2893,7 @@
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>parameter found.</t>
+          <t>s:asset:type</t>
         </is>
       </c>
       <c r="C113" t="inlineStr">
@@ -2915,7 +2915,7 @@
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>parameter found with value foxnewsglobalproduction. URL: http://foxnews.hb.omtrdc.net/?s:sc:rsid=foxnewsglobalproduction&amp;s:sc:tracking_server=smetrics.foxnews.com&amp;h:sc:ssl=1&amp;s:user:mid=69099319612994832056547930341105758682&amp;&amp;&amp;s:sp:ovp=Akamai&amp;s:sp:channel=Fox+News&amp;s:sp:player_name=Fox+News+Android+Player&amp;s:sp:hb_version=android-2.1.0.154-42fb90&amp;l:sp:hb_api_lvl=4&amp;s:event:sid=1673312989776217636246&amp;l:event:duration=338&amp;l:event:playhead=227&amp;l:event:prev_ts=-1&amp;s:event:type=pause&amp;l:event:ts=1673312994087&amp;s:asset:name=Biden+accused+of+mishandling+classified+documents&amp;l:asset:length=200&amp;s:asset:publisher=foxnews&amp;s:asset:type=main&amp;s:asset:video_id=6318425658112&amp;s:stream:type=vod&amp;l:stream:startup_time=0&amp;l:stream:fps=0&amp;l:stream:bitrate=0&amp;l:stream:dropped_frames=0.</t>
+          <t>s:sc:rsid</t>
         </is>
       </c>
       <c r="C114" t="inlineStr">
@@ -2937,7 +2937,7 @@
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>parameter found with value play. URL: http://foxnews.hb.omtrdc.net/?s:sc:rsid=foxnewsglobalproduction&amp;s:sc:tracking_server=smetrics.foxnews.com&amp;h:sc:ssl=1&amp;s:user:mid=69099319612994832056547930341105758682&amp;&amp;&amp;s:sp:ovp=Akamai&amp;s:sp:channel=Fox+News&amp;s:sp:player_name=Fox+News+Android+Player&amp;s:sp:hb_version=android-2.1.0.154-42fb90&amp;l:sp:hb_api_lvl=4&amp;s:event:sid=1673312989776217636246&amp;l:event:duration=0&amp;l:event:playhead=227&amp;l:event:prev_ts=-1&amp;s:event:type=play&amp;l:event:ts=1673312994087&amp;s:asset:name=Biden+accused+of+mishandling+classified+documents&amp;l:asset:length=200&amp;s:asset:publisher=foxnews&amp;s:asset:type=main&amp;s:asset:video_id=6318425658112&amp;s:stream:type=vod&amp;l:stream:startup_time=0&amp;l:stream:fps=0&amp;l:stream:bitrate=0&amp;l:stream:dropped_frames=0.</t>
+          <t>s:event:type</t>
         </is>
       </c>
       <c r="C115" t="inlineStr">
@@ -2959,7 +2959,7 @@
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>parameter found with value play. URL: http://foxnews.hb.omtrdc.net/?s:sc:rsid=foxnewsglobalproduction&amp;s:sc:tracking_server=smetrics.foxnews.com&amp;h:sc:ssl=1&amp;s:user:mid=69099319612994832056547930341105758682&amp;&amp;&amp;s:sp:ovp=Akamai&amp;s:sp:channel=Fox+News&amp;s:sp:player_name=Fox+News+Android+Player&amp;s:sp:hb_version=android-2.1.0.154-42fb90&amp;l:sp:hb_api_lvl=4&amp;s:event:sid=1673312989776217636246&amp;l:event:duration=0&amp;l:event:playhead=227&amp;l:event:prev_ts=-1&amp;s:event:type=play&amp;l:event:ts=1673312994087&amp;s:asset:name=Biden+accused+of+mishandling+classified+documents&amp;l:asset:length=200&amp;s:asset:publisher=foxnews&amp;s:asset:type=main&amp;s:asset:video_id=6318425658112&amp;s:stream:type=vod&amp;l:stream:startup_time=0&amp;l:stream:fps=0&amp;l:stream:bitrate=0&amp;l:stream:dropped_frames=0.</t>
+          <t>s:event:type</t>
         </is>
       </c>
       <c r="C116" t="inlineStr">
@@ -2981,7 +2981,7 @@
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>parameter found. URL: http://foxnews.hb.omtrdc.net/?s:sc:rsid=foxnewsglobalproduction&amp;s:sc:tracking_server=smetrics.foxnews.com&amp;h:sc:ssl=1&amp;s:user:mid=69099319612994832056547930341105758682&amp;&amp;&amp;s:sp:ovp=Akamai&amp;s:sp:channel=Fox+News&amp;s:sp:player_name=Fox+News+Android+Player&amp;s:sp:hb_version=android-2.1.0.154-42fb90&amp;l:sp:hb_api_lvl=4&amp;s:event:sid=1673312989776217636246&amp;l:event:duration=0&amp;l:event:playhead=227&amp;l:event:prev_ts=-1&amp;s:event:type=play&amp;l:event:ts=1673312994087&amp;s:asset:name=Biden+accused+of+mishandling+classified+documents&amp;l:asset:length=200&amp;s:asset:publisher=foxnews&amp;s:asset:type=main&amp;s:asset:video_id=6318425658112&amp;s:stream:type=vod&amp;l:stream:startup_time=0&amp;l:stream:fps=0&amp;l:stream:bitrate=0&amp;l:stream:dropped_frames=0.</t>
+          <t>s:event:sid</t>
         </is>
       </c>
       <c r="C117" t="inlineStr">
@@ -3003,7 +3003,7 @@
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>parameter found.</t>
+          <t>l:event:duration</t>
         </is>
       </c>
       <c r="C118" t="inlineStr">
@@ -3025,7 +3025,7 @@
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>parameter found.</t>
+          <t>l:event:prev_ts</t>
         </is>
       </c>
       <c r="C119" t="inlineStr">
@@ -3047,7 +3047,7 @@
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>parameter found.</t>
+          <t>l:event:ts</t>
         </is>
       </c>
       <c r="C120" t="inlineStr">
@@ -3069,7 +3069,7 @@
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>parameter found.</t>
+          <t>s:asset:name</t>
         </is>
       </c>
       <c r="C121" t="inlineStr">
@@ -3091,7 +3091,7 @@
       </c>
       <c r="B122" t="inlineStr">
         <is>
-          <t>parameter found.</t>
+          <t>l:asset:length</t>
         </is>
       </c>
       <c r="C122" t="inlineStr">
@@ -3113,7 +3113,7 @@
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t>parameter found.</t>
+          <t>s:asset:publisher</t>
         </is>
       </c>
       <c r="C123" t="inlineStr">
@@ -3135,7 +3135,7 @@
       </c>
       <c r="B124" t="inlineStr">
         <is>
-          <t>parameter found.</t>
+          <t>s:asset:type</t>
         </is>
       </c>
       <c r="C124" t="inlineStr">
@@ -3157,7 +3157,7 @@
       </c>
       <c r="B125" t="inlineStr">
         <is>
-          <t>parameter found with value foxnewsglobalproduction. URL: http://foxnews.hb.omtrdc.net/?s:sc:rsid=foxnewsglobalproduction&amp;s:sc:tracking_server=smetrics.foxnews.com&amp;h:sc:ssl=1&amp;s:user:mid=69099319612994832056547930341105758682&amp;&amp;&amp;s:sp:ovp=Akamai&amp;s:sp:channel=Fox+News&amp;s:sp:player_name=Fox+News+Android+Player&amp;s:sp:hb_version=android-2.1.0.154-42fb90&amp;l:sp:hb_api_lvl=4&amp;s:event:sid=1673312989776217636246&amp;l:event:duration=0&amp;l:event:playhead=227&amp;l:event:prev_ts=-1&amp;s:event:type=play&amp;l:event:ts=1673312994087&amp;s:asset:name=Biden+accused+of+mishandling+classified+documents&amp;l:asset:length=200&amp;s:asset:publisher=foxnews&amp;s:asset:type=main&amp;s:asset:video_id=6318425658112&amp;s:stream:type=vod&amp;l:stream:startup_time=0&amp;l:stream:fps=0&amp;l:stream:bitrate=0&amp;l:stream:dropped_frames=0.</t>
+          <t>s:sc:rsid</t>
         </is>
       </c>
       <c r="C125" t="inlineStr">
@@ -3179,7 +3179,7 @@
       </c>
       <c r="B126" t="inlineStr">
         <is>
-          <t>parameter found with value play. URL: http://foxnews.hb.omtrdc.net/?s:sc:rsid=foxnewsglobalproduction&amp;s:sc:tracking_server=smetrics.foxnews.com&amp;h:sc:ssl=1&amp;s:user:mid=69099319612994832056547930341105758682&amp;&amp;&amp;s:sp:ovp=Akamai&amp;s:sp:channel=Fox+News&amp;s:sp:player_name=Fox+News+Android+Player&amp;s:sp:hb_version=android-2.1.0.154-42fb90&amp;l:sp:hb_api_lvl=4&amp;s:event:sid=1673312989776217636246&amp;l:event:duration=1001&amp;l:event:playhead=1217&amp;l:event:prev_ts=1673312994087&amp;s:event:type=play&amp;l:event:ts=1673312995088&amp;s:asset:name=Biden+accused+of+mishandling+classified+documents&amp;l:asset:length=200&amp;s:asset:publisher=foxnews&amp;s:asset:type=main&amp;s:asset:video_id=6318425658112&amp;s:stream:type=vod&amp;l:stream:startup_time=0&amp;l:stream:fps=0&amp;l:stream:bitrate=0&amp;l:stream:dropped_frames=0.</t>
+          <t>s:event:type</t>
         </is>
       </c>
       <c r="C126" t="inlineStr">
@@ -3201,7 +3201,7 @@
       </c>
       <c r="B127" t="inlineStr">
         <is>
-          <t>parameter found with value play. URL: http://foxnews.hb.omtrdc.net/?s:sc:rsid=foxnewsglobalproduction&amp;s:sc:tracking_server=smetrics.foxnews.com&amp;h:sc:ssl=1&amp;s:user:mid=69099319612994832056547930341105758682&amp;&amp;&amp;s:sp:ovp=Akamai&amp;s:sp:channel=Fox+News&amp;s:sp:player_name=Fox+News+Android+Player&amp;s:sp:hb_version=android-2.1.0.154-42fb90&amp;l:sp:hb_api_lvl=4&amp;s:event:sid=1673312989776217636246&amp;l:event:duration=1001&amp;l:event:playhead=1217&amp;l:event:prev_ts=1673312994087&amp;s:event:type=play&amp;l:event:ts=1673312995088&amp;s:asset:name=Biden+accused+of+mishandling+classified+documents&amp;l:asset:length=200&amp;s:asset:publisher=foxnews&amp;s:asset:type=main&amp;s:asset:video_id=6318425658112&amp;s:stream:type=vod&amp;l:stream:startup_time=0&amp;l:stream:fps=0&amp;l:stream:bitrate=0&amp;l:stream:dropped_frames=0.</t>
+          <t>s:event:type</t>
         </is>
       </c>
       <c r="C127" t="inlineStr">
@@ -3223,7 +3223,7 @@
       </c>
       <c r="B128" t="inlineStr">
         <is>
-          <t>parameter found. URL: http://foxnews.hb.omtrdc.net/?s:sc:rsid=foxnewsglobalproduction&amp;s:sc:tracking_server=smetrics.foxnews.com&amp;h:sc:ssl=1&amp;s:user:mid=69099319612994832056547930341105758682&amp;&amp;&amp;s:sp:ovp=Akamai&amp;s:sp:channel=Fox+News&amp;s:sp:player_name=Fox+News+Android+Player&amp;s:sp:hb_version=android-2.1.0.154-42fb90&amp;l:sp:hb_api_lvl=4&amp;s:event:sid=1673312989776217636246&amp;l:event:duration=1001&amp;l:event:playhead=1217&amp;l:event:prev_ts=1673312994087&amp;s:event:type=play&amp;l:event:ts=1673312995088&amp;s:asset:name=Biden+accused+of+mishandling+classified+documents&amp;l:asset:length=200&amp;s:asset:publisher=foxnews&amp;s:asset:type=main&amp;s:asset:video_id=6318425658112&amp;s:stream:type=vod&amp;l:stream:startup_time=0&amp;l:stream:fps=0&amp;l:stream:bitrate=0&amp;l:stream:dropped_frames=0.</t>
+          <t>s:event:sid</t>
         </is>
       </c>
       <c r="C128" t="inlineStr">
@@ -3245,7 +3245,7 @@
       </c>
       <c r="B129" t="inlineStr">
         <is>
-          <t>parameter found.</t>
+          <t>l:event:duration</t>
         </is>
       </c>
       <c r="C129" t="inlineStr">
@@ -3267,7 +3267,7 @@
       </c>
       <c r="B130" t="inlineStr">
         <is>
-          <t>parameter found.</t>
+          <t>l:event:prev_ts</t>
         </is>
       </c>
       <c r="C130" t="inlineStr">
@@ -3289,7 +3289,7 @@
       </c>
       <c r="B131" t="inlineStr">
         <is>
-          <t>parameter found.</t>
+          <t>l:event:ts</t>
         </is>
       </c>
       <c r="C131" t="inlineStr">
@@ -3311,7 +3311,7 @@
       </c>
       <c r="B132" t="inlineStr">
         <is>
-          <t>parameter found.</t>
+          <t>s:asset:name</t>
         </is>
       </c>
       <c r="C132" t="inlineStr">
@@ -3333,7 +3333,7 @@
       </c>
       <c r="B133" t="inlineStr">
         <is>
-          <t>parameter found.</t>
+          <t>l:asset:length</t>
         </is>
       </c>
       <c r="C133" t="inlineStr">
@@ -3355,7 +3355,7 @@
       </c>
       <c r="B134" t="inlineStr">
         <is>
-          <t>parameter found.</t>
+          <t>s:asset:publisher</t>
         </is>
       </c>
       <c r="C134" t="inlineStr">
@@ -3377,7 +3377,7 @@
       </c>
       <c r="B135" t="inlineStr">
         <is>
-          <t>parameter found.</t>
+          <t>s:asset:type</t>
         </is>
       </c>
       <c r="C135" t="inlineStr">
@@ -3399,7 +3399,7 @@
       </c>
       <c r="B136" t="inlineStr">
         <is>
-          <t>parameter found with value foxnewsglobalproduction. URL: http://foxnews.hb.omtrdc.net/?s:sc:rsid=foxnewsglobalproduction&amp;s:sc:tracking_server=smetrics.foxnews.com&amp;h:sc:ssl=1&amp;s:user:mid=69099319612994832056547930341105758682&amp;&amp;&amp;s:sp:ovp=Akamai&amp;s:sp:channel=Fox+News&amp;s:sp:player_name=Fox+News+Android+Player&amp;s:sp:hb_version=android-2.1.0.154-42fb90&amp;l:sp:hb_api_lvl=4&amp;s:event:sid=1673312989776217636246&amp;l:event:duration=1001&amp;l:event:playhead=1217&amp;l:event:prev_ts=1673312994087&amp;s:event:type=play&amp;l:event:ts=1673312995088&amp;s:asset:name=Biden+accused+of+mishandling+classified+documents&amp;l:asset:length=200&amp;s:asset:publisher=foxnews&amp;s:asset:type=main&amp;s:asset:video_id=6318425658112&amp;s:stream:type=vod&amp;l:stream:startup_time=0&amp;l:stream:fps=0&amp;l:stream:bitrate=0&amp;l:stream:dropped_frames=0.</t>
+          <t>s:sc:rsid</t>
         </is>
       </c>
       <c r="C136" t="inlineStr">
@@ -3421,7 +3421,7 @@
       </c>
       <c r="B137" t="inlineStr">
         <is>
-          <t>parameter found with value play. URL: http://foxnews.hb.omtrdc.net/?s:sc:rsid=foxnewsglobalproduction&amp;s:sc:tracking_server=smetrics.foxnews.com&amp;h:sc:ssl=1&amp;s:user:mid=69099319612994832056547930341105758682&amp;&amp;&amp;s:sp:ovp=Akamai&amp;s:sp:channel=Fox+News&amp;s:sp:player_name=Fox+News+Android+Player&amp;s:sp:hb_version=android-2.1.0.154-42fb90&amp;l:sp:hb_api_lvl=4&amp;s:event:sid=1673312989776217636246&amp;l:event:duration=9892&amp;l:event:playhead=11124&amp;l:event:prev_ts=1673312995088&amp;s:event:type=play&amp;l:event:ts=1673313004980&amp;s:asset:name=Biden+accused+of+mishandling+classified+documents&amp;l:asset:length=200&amp;s:asset:publisher=foxnews&amp;s:asset:type=main&amp;s:asset:video_id=6318425658112&amp;s:stream:type=vod&amp;l:stream:startup_time=0&amp;l:stream:fps=0&amp;l:stream:bitrate=0&amp;l:stream:dropped_frames=0.</t>
+          <t>s:event:type</t>
         </is>
       </c>
       <c r="C137" t="inlineStr">
@@ -3443,7 +3443,7 @@
       </c>
       <c r="B138" t="inlineStr">
         <is>
-          <t>parameter found with value play. URL: http://foxnews.hb.omtrdc.net/?s:sc:rsid=foxnewsglobalproduction&amp;s:sc:tracking_server=smetrics.foxnews.com&amp;h:sc:ssl=1&amp;s:user:mid=69099319612994832056547930341105758682&amp;&amp;&amp;s:sp:ovp=Akamai&amp;s:sp:channel=Fox+News&amp;s:sp:player_name=Fox+News+Android+Player&amp;s:sp:hb_version=android-2.1.0.154-42fb90&amp;l:sp:hb_api_lvl=4&amp;s:event:sid=1673312989776217636246&amp;l:event:duration=9892&amp;l:event:playhead=11124&amp;l:event:prev_ts=1673312995088&amp;s:event:type=play&amp;l:event:ts=1673313004980&amp;s:asset:name=Biden+accused+of+mishandling+classified+documents&amp;l:asset:length=200&amp;s:asset:publisher=foxnews&amp;s:asset:type=main&amp;s:asset:video_id=6318425658112&amp;s:stream:type=vod&amp;l:stream:startup_time=0&amp;l:stream:fps=0&amp;l:stream:bitrate=0&amp;l:stream:dropped_frames=0.</t>
+          <t>s:event:type</t>
         </is>
       </c>
       <c r="C138" t="inlineStr">
@@ -3465,7 +3465,7 @@
       </c>
       <c r="B139" t="inlineStr">
         <is>
-          <t>parameter found. URL: http://foxnews.hb.omtrdc.net/?s:sc:rsid=foxnewsglobalproduction&amp;s:sc:tracking_server=smetrics.foxnews.com&amp;h:sc:ssl=1&amp;s:user:mid=69099319612994832056547930341105758682&amp;&amp;&amp;s:sp:ovp=Akamai&amp;s:sp:channel=Fox+News&amp;s:sp:player_name=Fox+News+Android+Player&amp;s:sp:hb_version=android-2.1.0.154-42fb90&amp;l:sp:hb_api_lvl=4&amp;s:event:sid=1673312989776217636246&amp;l:event:duration=9892&amp;l:event:playhead=11124&amp;l:event:prev_ts=1673312995088&amp;s:event:type=play&amp;l:event:ts=1673313004980&amp;s:asset:name=Biden+accused+of+mishandling+classified+documents&amp;l:asset:length=200&amp;s:asset:publisher=foxnews&amp;s:asset:type=main&amp;s:asset:video_id=6318425658112&amp;s:stream:type=vod&amp;l:stream:startup_time=0&amp;l:stream:fps=0&amp;l:stream:bitrate=0&amp;l:stream:dropped_frames=0.</t>
+          <t>s:event:sid</t>
         </is>
       </c>
       <c r="C139" t="inlineStr">
@@ -3487,7 +3487,7 @@
       </c>
       <c r="B140" t="inlineStr">
         <is>
-          <t>parameter found.</t>
+          <t>l:event:duration</t>
         </is>
       </c>
       <c r="C140" t="inlineStr">
@@ -3509,7 +3509,7 @@
       </c>
       <c r="B141" t="inlineStr">
         <is>
-          <t>parameter found.</t>
+          <t>l:event:prev_ts</t>
         </is>
       </c>
       <c r="C141" t="inlineStr">
@@ -3531,7 +3531,7 @@
       </c>
       <c r="B142" t="inlineStr">
         <is>
-          <t>parameter found.</t>
+          <t>l:event:ts</t>
         </is>
       </c>
       <c r="C142" t="inlineStr">
@@ -3553,7 +3553,7 @@
       </c>
       <c r="B143" t="inlineStr">
         <is>
-          <t>parameter found.</t>
+          <t>s:asset:name</t>
         </is>
       </c>
       <c r="C143" t="inlineStr">
@@ -3575,7 +3575,7 @@
       </c>
       <c r="B144" t="inlineStr">
         <is>
-          <t>parameter found.</t>
+          <t>l:asset:length</t>
         </is>
       </c>
       <c r="C144" t="inlineStr">
@@ -3597,7 +3597,7 @@
       </c>
       <c r="B145" t="inlineStr">
         <is>
-          <t>parameter found.</t>
+          <t>s:asset:publisher</t>
         </is>
       </c>
       <c r="C145" t="inlineStr">
@@ -3619,7 +3619,7 @@
       </c>
       <c r="B146" t="inlineStr">
         <is>
-          <t>parameter found.</t>
+          <t>s:asset:type</t>
         </is>
       </c>
       <c r="C146" t="inlineStr">
@@ -3641,7 +3641,7 @@
       </c>
       <c r="B147" t="inlineStr">
         <is>
-          <t>parameter found with value foxnewsglobalproduction. URL: http://foxnews.hb.omtrdc.net/?s:sc:rsid=foxnewsglobalproduction&amp;s:sc:tracking_server=smetrics.foxnews.com&amp;h:sc:ssl=1&amp;s:user:mid=69099319612994832056547930341105758682&amp;&amp;&amp;s:sp:ovp=Akamai&amp;s:sp:channel=Fox+News&amp;s:sp:player_name=Fox+News+Android+Player&amp;s:sp:hb_version=android-2.1.0.154-42fb90&amp;l:sp:hb_api_lvl=4&amp;s:event:sid=1673312989776217636246&amp;l:event:duration=9892&amp;l:event:playhead=11124&amp;l:event:prev_ts=1673312995088&amp;s:event:type=play&amp;l:event:ts=1673313004980&amp;s:asset:name=Biden+accused+of+mishandling+classified+documents&amp;l:asset:length=200&amp;s:asset:publisher=foxnews&amp;s:asset:type=main&amp;s:asset:video_id=6318425658112&amp;s:stream:type=vod&amp;l:stream:startup_time=0&amp;l:stream:fps=0&amp;l:stream:bitrate=0&amp;l:stream:dropped_frames=0.</t>
+          <t>s:sc:rsid</t>
         </is>
       </c>
       <c r="C147" t="inlineStr">
@@ -3663,7 +3663,7 @@
       </c>
       <c r="B148" t="inlineStr">
         <is>
-          <t>parameter found with value play. URL: http://foxnews.hb.omtrdc.net/?s:sc:rsid=foxnewsglobalproduction&amp;s:sc:tracking_server=smetrics.foxnews.com&amp;h:sc:ssl=1&amp;s:user:mid=69099319612994832056547930341105758682&amp;&amp;&amp;s:sp:ovp=Akamai&amp;s:sp:channel=Fox+News&amp;s:sp:player_name=Fox+News+Android+Player&amp;s:sp:hb_version=android-2.1.0.154-42fb90&amp;l:sp:hb_api_lvl=4&amp;s:event:sid=1673312989776217636246&amp;l:event:duration=9945&amp;l:event:playhead=21071&amp;l:event:prev_ts=1673313004980&amp;s:event:type=play&amp;l:event:ts=1673313014925&amp;s:asset:name=Biden+accused+of+mishandling+classified+documents&amp;l:asset:length=200&amp;s:asset:publisher=foxnews&amp;s:asset:type=main&amp;s:asset:video_id=6318425658112&amp;s:stream:type=vod&amp;l:stream:startup_time=0&amp;l:stream:fps=0&amp;l:stream:bitrate=0&amp;l:stream:dropped_frames=0.</t>
+          <t>s:event:type</t>
         </is>
       </c>
       <c r="C148" t="inlineStr">
@@ -3685,7 +3685,7 @@
       </c>
       <c r="B149" t="inlineStr">
         <is>
-          <t>parameter found with value play. URL: http://foxnews.hb.omtrdc.net/?s:sc:rsid=foxnewsglobalproduction&amp;s:sc:tracking_server=smetrics.foxnews.com&amp;h:sc:ssl=1&amp;s:user:mid=69099319612994832056547930341105758682&amp;&amp;&amp;s:sp:ovp=Akamai&amp;s:sp:channel=Fox+News&amp;s:sp:player_name=Fox+News+Android+Player&amp;s:sp:hb_version=android-2.1.0.154-42fb90&amp;l:sp:hb_api_lvl=4&amp;s:event:sid=1673312989776217636246&amp;l:event:duration=9945&amp;l:event:playhead=21071&amp;l:event:prev_ts=1673313004980&amp;s:event:type=play&amp;l:event:ts=1673313014925&amp;s:asset:name=Biden+accused+of+mishandling+classified+documents&amp;l:asset:length=200&amp;s:asset:publisher=foxnews&amp;s:asset:type=main&amp;s:asset:video_id=6318425658112&amp;s:stream:type=vod&amp;l:stream:startup_time=0&amp;l:stream:fps=0&amp;l:stream:bitrate=0&amp;l:stream:dropped_frames=0.</t>
+          <t>s:event:type</t>
         </is>
       </c>
       <c r="C149" t="inlineStr">
@@ -3707,7 +3707,7 @@
       </c>
       <c r="B150" t="inlineStr">
         <is>
-          <t>parameter found. URL: http://foxnews.hb.omtrdc.net/?s:sc:rsid=foxnewsglobalproduction&amp;s:sc:tracking_server=smetrics.foxnews.com&amp;h:sc:ssl=1&amp;s:user:mid=69099319612994832056547930341105758682&amp;&amp;&amp;s:sp:ovp=Akamai&amp;s:sp:channel=Fox+News&amp;s:sp:player_name=Fox+News+Android+Player&amp;s:sp:hb_version=android-2.1.0.154-42fb90&amp;l:sp:hb_api_lvl=4&amp;s:event:sid=1673312989776217636246&amp;l:event:duration=9945&amp;l:event:playhead=21071&amp;l:event:prev_ts=1673313004980&amp;s:event:type=play&amp;l:event:ts=1673313014925&amp;s:asset:name=Biden+accused+of+mishandling+classified+documents&amp;l:asset:length=200&amp;s:asset:publisher=foxnews&amp;s:asset:type=main&amp;s:asset:video_id=6318425658112&amp;s:stream:type=vod&amp;l:stream:startup_time=0&amp;l:stream:fps=0&amp;l:stream:bitrate=0&amp;l:stream:dropped_frames=0.</t>
+          <t>s:event:sid</t>
         </is>
       </c>
       <c r="C150" t="inlineStr">
@@ -3729,7 +3729,7 @@
       </c>
       <c r="B151" t="inlineStr">
         <is>
-          <t>parameter found.</t>
+          <t>l:event:duration</t>
         </is>
       </c>
       <c r="C151" t="inlineStr">
@@ -3751,7 +3751,7 @@
       </c>
       <c r="B152" t="inlineStr">
         <is>
-          <t>parameter found.</t>
+          <t>l:event:prev_ts</t>
         </is>
       </c>
       <c r="C152" t="inlineStr">
@@ -3773,7 +3773,7 @@
       </c>
       <c r="B153" t="inlineStr">
         <is>
-          <t>parameter found.</t>
+          <t>l:event:ts</t>
         </is>
       </c>
       <c r="C153" t="inlineStr">
@@ -3795,7 +3795,7 @@
       </c>
       <c r="B154" t="inlineStr">
         <is>
-          <t>parameter found.</t>
+          <t>s:asset:name</t>
         </is>
       </c>
       <c r="C154" t="inlineStr">
@@ -3817,7 +3817,7 @@
       </c>
       <c r="B155" t="inlineStr">
         <is>
-          <t>parameter found.</t>
+          <t>l:asset:length</t>
         </is>
       </c>
       <c r="C155" t="inlineStr">
@@ -3839,7 +3839,7 @@
       </c>
       <c r="B156" t="inlineStr">
         <is>
-          <t>parameter found.</t>
+          <t>s:asset:publisher</t>
         </is>
       </c>
       <c r="C156" t="inlineStr">
@@ -3861,7 +3861,7 @@
       </c>
       <c r="B157" t="inlineStr">
         <is>
-          <t>parameter found.</t>
+          <t>s:asset:type</t>
         </is>
       </c>
       <c r="C157" t="inlineStr">
@@ -3883,7 +3883,7 @@
       </c>
       <c r="B158" t="inlineStr">
         <is>
-          <t>parameter found with value foxnewsglobalproduction. URL: http://foxnews.hb.omtrdc.net/?s:sc:rsid=foxnewsglobalproduction&amp;s:sc:tracking_server=smetrics.foxnews.com&amp;h:sc:ssl=1&amp;s:user:mid=69099319612994832056547930341105758682&amp;&amp;&amp;s:sp:ovp=Akamai&amp;s:sp:channel=Fox+News&amp;s:sp:player_name=Fox+News+Android+Player&amp;s:sp:hb_version=android-2.1.0.154-42fb90&amp;l:sp:hb_api_lvl=4&amp;s:event:sid=1673312989776217636246&amp;l:event:duration=9945&amp;l:event:playhead=21071&amp;l:event:prev_ts=1673313004980&amp;s:event:type=play&amp;l:event:ts=1673313014925&amp;s:asset:name=Biden+accused+of+mishandling+classified+documents&amp;l:asset:length=200&amp;s:asset:publisher=foxnews&amp;s:asset:type=main&amp;s:asset:video_id=6318425658112&amp;s:stream:type=vod&amp;l:stream:startup_time=0&amp;l:stream:fps=0&amp;l:stream:bitrate=0&amp;l:stream:dropped_frames=0.</t>
+          <t>s:sc:rsid</t>
         </is>
       </c>
       <c r="C158" t="inlineStr">
@@ -3905,7 +3905,7 @@
       </c>
       <c r="B159" t="inlineStr">
         <is>
-          <t>parameter found with value play. URL: http://foxnews.hb.omtrdc.net/?s:sc:rsid=foxnewsglobalproduction&amp;s:sc:tracking_server=smetrics.foxnews.com&amp;h:sc:ssl=1&amp;s:user:mid=69099319612994832056547930341105758682&amp;&amp;&amp;s:sp:ovp=Akamai&amp;s:sp:channel=Fox+News&amp;s:sp:player_name=Fox+News+Android+Player&amp;s:sp:hb_version=android-2.1.0.154-42fb90&amp;l:sp:hb_api_lvl=4&amp;s:event:sid=1673312989776217636246&amp;l:event:duration=9909&amp;l:event:playhead=30711&amp;l:event:prev_ts=1673313014925&amp;s:event:type=play&amp;l:event:ts=1673313024834&amp;s:asset:name=Biden+accused+of+mishandling+classified+documents&amp;l:asset:length=200&amp;s:asset:publisher=foxnews&amp;s:asset:type=main&amp;s:asset:video_id=6318425658112&amp;s:stream:type=vod&amp;l:stream:startup_time=0&amp;l:stream:fps=0&amp;l:stream:bitrate=0&amp;l:stream:dropped_frames=0.</t>
+          <t>s:event:type</t>
         </is>
       </c>
       <c r="C159" t="inlineStr">
@@ -3927,7 +3927,7 @@
       </c>
       <c r="B160" t="inlineStr">
         <is>
-          <t>parameter found with value play. URL: http://foxnews.hb.omtrdc.net/?s:sc:rsid=foxnewsglobalproduction&amp;s:sc:tracking_server=smetrics.foxnews.com&amp;h:sc:ssl=1&amp;s:user:mid=69099319612994832056547930341105758682&amp;&amp;&amp;s:sp:ovp=Akamai&amp;s:sp:channel=Fox+News&amp;s:sp:player_name=Fox+News+Android+Player&amp;s:sp:hb_version=android-2.1.0.154-42fb90&amp;l:sp:hb_api_lvl=4&amp;s:event:sid=1673312989776217636246&amp;l:event:duration=9909&amp;l:event:playhead=30711&amp;l:event:prev_ts=1673313014925&amp;s:event:type=play&amp;l:event:ts=1673313024834&amp;s:asset:name=Biden+accused+of+mishandling+classified+documents&amp;l:asset:length=200&amp;s:asset:publisher=foxnews&amp;s:asset:type=main&amp;s:asset:video_id=6318425658112&amp;s:stream:type=vod&amp;l:stream:startup_time=0&amp;l:stream:fps=0&amp;l:stream:bitrate=0&amp;l:stream:dropped_frames=0.</t>
+          <t>s:event:type</t>
         </is>
       </c>
       <c r="C160" t="inlineStr">
@@ -3949,7 +3949,7 @@
       </c>
       <c r="B161" t="inlineStr">
         <is>
-          <t>parameter found. URL: http://foxnews.hb.omtrdc.net/?s:sc:rsid=foxnewsglobalproduction&amp;s:sc:tracking_server=smetrics.foxnews.com&amp;h:sc:ssl=1&amp;s:user:mid=69099319612994832056547930341105758682&amp;&amp;&amp;s:sp:ovp=Akamai&amp;s:sp:channel=Fox+News&amp;s:sp:player_name=Fox+News+Android+Player&amp;s:sp:hb_version=android-2.1.0.154-42fb90&amp;l:sp:hb_api_lvl=4&amp;s:event:sid=1673312989776217636246&amp;l:event:duration=9909&amp;l:event:playhead=30711&amp;l:event:prev_ts=1673313014925&amp;s:event:type=play&amp;l:event:ts=1673313024834&amp;s:asset:name=Biden+accused+of+mishandling+classified+documents&amp;l:asset:length=200&amp;s:asset:publisher=foxnews&amp;s:asset:type=main&amp;s:asset:video_id=6318425658112&amp;s:stream:type=vod&amp;l:stream:startup_time=0&amp;l:stream:fps=0&amp;l:stream:bitrate=0&amp;l:stream:dropped_frames=0.</t>
+          <t>s:event:sid</t>
         </is>
       </c>
       <c r="C161" t="inlineStr">
@@ -3971,7 +3971,7 @@
       </c>
       <c r="B162" t="inlineStr">
         <is>
-          <t>parameter found.</t>
+          <t>l:event:duration</t>
         </is>
       </c>
       <c r="C162" t="inlineStr">
@@ -3993,7 +3993,7 @@
       </c>
       <c r="B163" t="inlineStr">
         <is>
-          <t>parameter found.</t>
+          <t>l:event:prev_ts</t>
         </is>
       </c>
       <c r="C163" t="inlineStr">
@@ -4015,7 +4015,7 @@
       </c>
       <c r="B164" t="inlineStr">
         <is>
-          <t>parameter found.</t>
+          <t>l:event:ts</t>
         </is>
       </c>
       <c r="C164" t="inlineStr">
@@ -4037,7 +4037,7 @@
       </c>
       <c r="B165" t="inlineStr">
         <is>
-          <t>parameter found.</t>
+          <t>s:asset:name</t>
         </is>
       </c>
       <c r="C165" t="inlineStr">
@@ -4059,7 +4059,7 @@
       </c>
       <c r="B166" t="inlineStr">
         <is>
-          <t>parameter found.</t>
+          <t>l:asset:length</t>
         </is>
       </c>
       <c r="C166" t="inlineStr">
@@ -4081,7 +4081,7 @@
       </c>
       <c r="B167" t="inlineStr">
         <is>
-          <t>parameter found.</t>
+          <t>s:asset:publisher</t>
         </is>
       </c>
       <c r="C167" t="inlineStr">
@@ -4103,7 +4103,7 @@
       </c>
       <c r="B168" t="inlineStr">
         <is>
-          <t>parameter found.</t>
+          <t>s:asset:type</t>
         </is>
       </c>
       <c r="C168" t="inlineStr">
@@ -4125,7 +4125,7 @@
       </c>
       <c r="B169" t="inlineStr">
         <is>
-          <t>parameter found with value foxnewsglobalproduction. URL: http://foxnews.hb.omtrdc.net/?s:sc:rsid=foxnewsglobalproduction&amp;s:sc:tracking_server=smetrics.foxnews.com&amp;h:sc:ssl=1&amp;s:user:mid=69099319612994832056547930341105758682&amp;&amp;&amp;s:sp:ovp=Akamai&amp;s:sp:channel=Fox+News&amp;s:sp:player_name=Fox+News+Android+Player&amp;s:sp:hb_version=android-2.1.0.154-42fb90&amp;l:sp:hb_api_lvl=4&amp;s:event:sid=1673312989776217636246&amp;l:event:duration=9909&amp;l:event:playhead=30711&amp;l:event:prev_ts=1673313014925&amp;s:event:type=play&amp;l:event:ts=1673313024834&amp;s:asset:name=Biden+accused+of+mishandling+classified+documents&amp;l:asset:length=200&amp;s:asset:publisher=foxnews&amp;s:asset:type=main&amp;s:asset:video_id=6318425658112&amp;s:stream:type=vod&amp;l:stream:startup_time=0&amp;l:stream:fps=0&amp;l:stream:bitrate=0&amp;l:stream:dropped_frames=0.</t>
+          <t>s:sc:rsid</t>
         </is>
       </c>
       <c r="C169" t="inlineStr">
@@ -4147,7 +4147,7 @@
       </c>
       <c r="B170" t="inlineStr">
         <is>
-          <t>parameter found with value play. URL: http://foxnews.hb.omtrdc.net/?s:sc:rsid=foxnewsglobalproduction&amp;s:sc:tracking_server=smetrics.foxnews.com&amp;h:sc:ssl=1&amp;s:user:mid=69099319612994832056547930341105758682&amp;&amp;&amp;s:sp:ovp=Akamai&amp;s:sp:channel=Fox+News&amp;s:sp:player_name=Fox+News+Android+Player&amp;s:sp:hb_version=android-2.1.0.154-42fb90&amp;l:sp:hb_api_lvl=4&amp;s:event:sid=1673312989776217636246&amp;l:event:duration=10104&amp;l:event:playhead=40827&amp;l:event:prev_ts=1673313024834&amp;s:event:type=play&amp;l:event:ts=1673313034938&amp;s:asset:name=Biden+accused+of+mishandling+classified+documents&amp;l:asset:length=200&amp;s:asset:publisher=foxnews&amp;s:asset:type=main&amp;s:asset:video_id=6318425658112&amp;s:stream:type=vod&amp;l:stream:startup_time=0&amp;l:stream:fps=0&amp;l:stream:bitrate=0&amp;l:stream:dropped_frames=0.</t>
+          <t>s:event:type</t>
         </is>
       </c>
       <c r="C170" t="inlineStr">
@@ -4169,7 +4169,7 @@
       </c>
       <c r="B171" t="inlineStr">
         <is>
-          <t>parameter found with value play. URL: http://foxnews.hb.omtrdc.net/?s:sc:rsid=foxnewsglobalproduction&amp;s:sc:tracking_server=smetrics.foxnews.com&amp;h:sc:ssl=1&amp;s:user:mid=69099319612994832056547930341105758682&amp;&amp;&amp;s:sp:ovp=Akamai&amp;s:sp:channel=Fox+News&amp;s:sp:player_name=Fox+News+Android+Player&amp;s:sp:hb_version=android-2.1.0.154-42fb90&amp;l:sp:hb_api_lvl=4&amp;s:event:sid=1673312989776217636246&amp;l:event:duration=10104&amp;l:event:playhead=40827&amp;l:event:prev_ts=1673313024834&amp;s:event:type=play&amp;l:event:ts=1673313034938&amp;s:asset:name=Biden+accused+of+mishandling+classified+documents&amp;l:asset:length=200&amp;s:asset:publisher=foxnews&amp;s:asset:type=main&amp;s:asset:video_id=6318425658112&amp;s:stream:type=vod&amp;l:stream:startup_time=0&amp;l:stream:fps=0&amp;l:stream:bitrate=0&amp;l:stream:dropped_frames=0.</t>
+          <t>s:event:type</t>
         </is>
       </c>
       <c r="C171" t="inlineStr">
@@ -4191,7 +4191,7 @@
       </c>
       <c r="B172" t="inlineStr">
         <is>
-          <t>parameter found. URL: http://foxnews.hb.omtrdc.net/?s:sc:rsid=foxnewsglobalproduction&amp;s:sc:tracking_server=smetrics.foxnews.com&amp;h:sc:ssl=1&amp;s:user:mid=69099319612994832056547930341105758682&amp;&amp;&amp;s:sp:ovp=Akamai&amp;s:sp:channel=Fox+News&amp;s:sp:player_name=Fox+News+Android+Player&amp;s:sp:hb_version=android-2.1.0.154-42fb90&amp;l:sp:hb_api_lvl=4&amp;s:event:sid=1673312989776217636246&amp;l:event:duration=10104&amp;l:event:playhead=40827&amp;l:event:prev_ts=1673313024834&amp;s:event:type=play&amp;l:event:ts=1673313034938&amp;s:asset:name=Biden+accused+of+mishandling+classified+documents&amp;l:asset:length=200&amp;s:asset:publisher=foxnews&amp;s:asset:type=main&amp;s:asset:video_id=6318425658112&amp;s:stream:type=vod&amp;l:stream:startup_time=0&amp;l:stream:fps=0&amp;l:stream:bitrate=0&amp;l:stream:dropped_frames=0.</t>
+          <t>s:event:sid</t>
         </is>
       </c>
       <c r="C172" t="inlineStr">
@@ -4213,7 +4213,7 @@
       </c>
       <c r="B173" t="inlineStr">
         <is>
-          <t>parameter found.</t>
+          <t>l:event:duration</t>
         </is>
       </c>
       <c r="C173" t="inlineStr">
@@ -4235,7 +4235,7 @@
       </c>
       <c r="B174" t="inlineStr">
         <is>
-          <t>parameter found.</t>
+          <t>l:event:prev_ts</t>
         </is>
       </c>
       <c r="C174" t="inlineStr">
@@ -4257,7 +4257,7 @@
       </c>
       <c r="B175" t="inlineStr">
         <is>
-          <t>parameter found.</t>
+          <t>l:event:ts</t>
         </is>
       </c>
       <c r="C175" t="inlineStr">
@@ -4279,7 +4279,7 @@
       </c>
       <c r="B176" t="inlineStr">
         <is>
-          <t>parameter found.</t>
+          <t>s:asset:name</t>
         </is>
       </c>
       <c r="C176" t="inlineStr">
@@ -4301,7 +4301,7 @@
       </c>
       <c r="B177" t="inlineStr">
         <is>
-          <t>parameter found.</t>
+          <t>l:asset:length</t>
         </is>
       </c>
       <c r="C177" t="inlineStr">
@@ -4323,7 +4323,7 @@
       </c>
       <c r="B178" t="inlineStr">
         <is>
-          <t>parameter found.</t>
+          <t>s:asset:publisher</t>
         </is>
       </c>
       <c r="C178" t="inlineStr">
@@ -4345,7 +4345,7 @@
       </c>
       <c r="B179" t="inlineStr">
         <is>
-          <t>parameter found.</t>
+          <t>s:asset:type</t>
         </is>
       </c>
       <c r="C179" t="inlineStr">
@@ -4367,7 +4367,7 @@
       </c>
       <c r="B180" t="inlineStr">
         <is>
-          <t>parameter found with value foxnewsglobalproduction. URL: http://foxnews.hb.omtrdc.net/?s:sc:rsid=foxnewsglobalproduction&amp;s:sc:tracking_server=smetrics.foxnews.com&amp;h:sc:ssl=1&amp;s:user:mid=69099319612994832056547930341105758682&amp;&amp;&amp;s:sp:ovp=Akamai&amp;s:sp:channel=Fox+News&amp;s:sp:player_name=Fox+News+Android+Player&amp;s:sp:hb_version=android-2.1.0.154-42fb90&amp;l:sp:hb_api_lvl=4&amp;s:event:sid=1673312989776217636246&amp;l:event:duration=10104&amp;l:event:playhead=40827&amp;l:event:prev_ts=1673313024834&amp;s:event:type=play&amp;l:event:ts=1673313034938&amp;s:asset:name=Biden+accused+of+mishandling+classified+documents&amp;l:asset:length=200&amp;s:asset:publisher=foxnews&amp;s:asset:type=main&amp;s:asset:video_id=6318425658112&amp;s:stream:type=vod&amp;l:stream:startup_time=0&amp;l:stream:fps=0&amp;l:stream:bitrate=0&amp;l:stream:dropped_frames=0.</t>
+          <t>s:sc:rsid</t>
         </is>
       </c>
       <c r="C180" t="inlineStr">

</xml_diff>

<commit_message>
Update test results with analysis tab
</commit_message>
<xml_diff>
--- a/harmony_test_results.xlsx
+++ b/harmony_test_results.xlsx
@@ -8,6 +8,7 @@
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Test Results" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Analysis" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -4926,4 +4927,323 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B31"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Metric</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Value</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Total Calls</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Total Test Cases</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Total Passes</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Total Fails</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Pass Percentage</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>74.86%</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Fail Percentage</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>25.14%</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>URL Failures</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Count</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>https://smetrics.foxnews.com/id?mid=69099319612994832056547930341105758682&amp;mcorgid=foxnews</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>https://smetrics.foxnews.com/b/ss/foxnewsglobalproduction/0/JAVA-4.17.9-AN/s40450848</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>http://foxnews.hb.omtrdc.net/settings/foxnews.xml?r=1673312989724</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Dimension Failures</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Count</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>s:event:type</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>s:event:sid</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>l:event:duration</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>l:event:prev_ts</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>l:event:ts</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>s:asset:name</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>l:asset:length</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>s:asset:publisher</t>
+        </is>
+      </c>
+      <c r="B22" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>s:asset:type</t>
+        </is>
+      </c>
+      <c r="B23" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>app_build</t>
+        </is>
+      </c>
+      <c r="B24" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>app_name</t>
+        </is>
+      </c>
+      <c r="B25" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>app_version</t>
+        </is>
+      </c>
+      <c r="B26" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>l:event:playhead</t>
+        </is>
+      </c>
+      <c r="B27" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>page_type</t>
+        </is>
+      </c>
+      <c r="B28" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>primary_business_unit</t>
+        </is>
+      </c>
+      <c r="B29" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>user_fox_anonymous_profile_id</t>
+        </is>
+      </c>
+      <c r="B30" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>s:sc:rsid</t>
+        </is>
+      </c>
+      <c r="B31" t="n">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Chore: Remove README_CheatSheet as content is integrated into README
</commit_message>
<xml_diff>
--- a/harmony_test_results.xlsx
+++ b/harmony_test_results.xlsx
@@ -8,6 +8,7 @@
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Test Results" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Analysis" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -435,6 +436,321 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
+          <t>URL</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Parameter</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Result</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>URL Failures</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>Count</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>Dimension Failures</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>Count</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>https://example.com/test1</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>param1</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Pass</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>http://foxnews.hb.omtrdc.net/settings/foxnews.xml?r=1673312989724</t>
+        </is>
+      </c>
+      <c r="E2" t="n">
+        <v>11</v>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>s:event:type</t>
+        </is>
+      </c>
+      <c r="H2" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>https://example.com/test2</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>param2</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Fail</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>https://smetrics.foxnews.com/id?mid=69099319612994832056547930341105758682&amp;mcorgid=foxnews</t>
+        </is>
+      </c>
+      <c r="E3" t="n">
+        <v>17</v>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>s:event:sid</t>
+        </is>
+      </c>
+      <c r="H3" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>https://example.com/test3</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>param3</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Pass</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>https://smetrics.foxnews.com/b/ss/foxnewsglobalproduction/0/JAVA-4.17.9-AN/s40450848</t>
+        </is>
+      </c>
+      <c r="E4" t="n">
+        <v>17</v>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>l:event:duration</t>
+        </is>
+      </c>
+      <c r="H4" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>https://example.com/test4</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>param4</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Fail</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Details of test case 4</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>l:event:prev_ts</t>
+        </is>
+      </c>
+      <c r="H5" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>l:event:ts</t>
+        </is>
+      </c>
+      <c r="H6" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>s:asset:name</t>
+        </is>
+      </c>
+      <c r="H7" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>l:asset:length</t>
+        </is>
+      </c>
+      <c r="H8" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>s:asset:publisher</t>
+        </is>
+      </c>
+      <c r="H9" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>s:asset:type</t>
+        </is>
+      </c>
+      <c r="H10" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>s:sc:rsid</t>
+        </is>
+      </c>
+      <c r="H11" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>app_build</t>
+        </is>
+      </c>
+      <c r="H12" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>app_name</t>
+        </is>
+      </c>
+      <c r="H13" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>app_version</t>
+        </is>
+      </c>
+      <c r="H14" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>l:event:playhead</t>
+        </is>
+      </c>
+      <c r="H15" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>page_type</t>
+        </is>
+      </c>
+      <c r="H16" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>primary_business_unit</t>
+        </is>
+      </c>
+      <c r="H17" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>user_fox_anonymous_profile_id</t>
+        </is>
+      </c>
+      <c r="H18" t="n">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:H7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
           <t>Metric</t>
         </is>
       </c>
@@ -477,19 +793,19 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>http://foxnews.hb.omtrdc.net/settings/foxnews.xml?r=1673312989724</t>
+          <t>https://example.com/failure1</t>
         </is>
       </c>
       <c r="E2" t="n">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>s:event:type</t>
+          <t>example_dimension_1</t>
         </is>
       </c>
       <c r="H2" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3">
@@ -503,19 +819,19 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>https://smetrics.foxnews.com/id?mid=69099319612994832056547930341105758682&amp;mcorgid=foxnews</t>
+          <t>https://example.com/failure2</t>
         </is>
       </c>
       <c r="E3" t="n">
-        <v>17</v>
+        <v>3</v>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>s:event:sid</t>
+          <t>example_dimension_2</t>
         </is>
       </c>
       <c r="H3" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4">
@@ -527,22 +843,6 @@
       <c r="B4" t="n">
         <v>1</v>
       </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>https://smetrics.foxnews.com/b/ss/foxnewsglobalproduction/0/JAVA-4.17.9-AN/s40450848</t>
-        </is>
-      </c>
-      <c r="E4" t="n">
-        <v>17</v>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>l:event:duration</t>
-        </is>
-      </c>
-      <c r="H4" t="n">
-        <v>3</v>
-      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -553,14 +853,6 @@
       <c r="B5" t="n">
         <v>1</v>
       </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>l:event:prev_ts</t>
-        </is>
-      </c>
-      <c r="H5" t="n">
-        <v>3</v>
-      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -573,14 +865,6 @@
           <t>100%</t>
         </is>
       </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>l:event:ts</t>
-        </is>
-      </c>
-      <c r="H6" t="n">
-        <v>3</v>
-      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -592,140 +876,6 @@
         <is>
           <t>0%</t>
         </is>
-      </c>
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>s:asset:name</t>
-        </is>
-      </c>
-      <c r="H7" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>l:asset:length</t>
-        </is>
-      </c>
-      <c r="H8" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>https://example.com</t>
-        </is>
-      </c>
-      <c r="B9" t="n">
-        <v>1</v>
-      </c>
-      <c r="G9" t="inlineStr">
-        <is>
-          <t>s:asset:publisher</t>
-        </is>
-      </c>
-      <c r="H9" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="G10" t="inlineStr">
-        <is>
-          <t>s:asset:type</t>
-        </is>
-      </c>
-      <c r="H10" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>example_dimension</t>
-        </is>
-      </c>
-      <c r="B11" t="n">
-        <v>1</v>
-      </c>
-      <c r="G11" t="inlineStr">
-        <is>
-          <t>s:sc:rsid</t>
-        </is>
-      </c>
-      <c r="H11" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="G12" t="inlineStr">
-        <is>
-          <t>app_build</t>
-        </is>
-      </c>
-      <c r="H12" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="G13" t="inlineStr">
-        <is>
-          <t>app_name</t>
-        </is>
-      </c>
-      <c r="H13" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="G14" t="inlineStr">
-        <is>
-          <t>app_version</t>
-        </is>
-      </c>
-      <c r="H14" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="G15" t="inlineStr">
-        <is>
-          <t>l:event:playhead</t>
-        </is>
-      </c>
-      <c r="H15" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="G16" t="inlineStr">
-        <is>
-          <t>page_type</t>
-        </is>
-      </c>
-      <c r="H16" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="G17" t="inlineStr">
-        <is>
-          <t>primary_business_unit</t>
-        </is>
-      </c>
-      <c r="H17" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="G18" t="inlineStr">
-        <is>
-          <t>user_fox_anonymous_profile_id</t>
-        </is>
-      </c>
-      <c r="H18" t="n">
-        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix: Clear existing data in Test Results sheet before writing new data
</commit_message>
<xml_diff>
--- a/harmony_test_results.xlsx
+++ b/harmony_test_results.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H18"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -470,265 +470,10 @@
         </is>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>https://example.com/test1</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>param1</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>http://foxnews.hb.omtrdc.net/settings/foxnews.xml?r=1673312989724</t>
-        </is>
-      </c>
-      <c r="E2" t="n">
-        <v>11</v>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>s:event:type</t>
-        </is>
-      </c>
-      <c r="H2" t="n">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>https://example.com/test2</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>param2</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Fail</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>https://smetrics.foxnews.com/id?mid=69099319612994832056547930341105758682&amp;mcorgid=foxnews</t>
-        </is>
-      </c>
-      <c r="E3" t="n">
-        <v>17</v>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>s:event:sid</t>
-        </is>
-      </c>
-      <c r="H3" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>https://example.com/test3</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>param3</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>https://smetrics.foxnews.com/b/ss/foxnewsglobalproduction/0/JAVA-4.17.9-AN/s40450848</t>
-        </is>
-      </c>
-      <c r="E4" t="n">
-        <v>17</v>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>l:event:duration</t>
-        </is>
-      </c>
-      <c r="H4" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>https://example.com/test4</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>param4</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>Fail</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>Details of test case 4</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>l:event:prev_ts</t>
-        </is>
-      </c>
-      <c r="H5" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>l:event:ts</t>
-        </is>
-      </c>
-      <c r="H6" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>s:asset:name</t>
-        </is>
-      </c>
-      <c r="H7" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>l:asset:length</t>
-        </is>
-      </c>
-      <c r="H8" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="G9" t="inlineStr">
-        <is>
-          <t>s:asset:publisher</t>
-        </is>
-      </c>
-      <c r="H9" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="G10" t="inlineStr">
-        <is>
-          <t>s:asset:type</t>
-        </is>
-      </c>
-      <c r="H10" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="G11" t="inlineStr">
-        <is>
-          <t>s:sc:rsid</t>
-        </is>
-      </c>
-      <c r="H11" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="G12" t="inlineStr">
-        <is>
-          <t>app_build</t>
-        </is>
-      </c>
-      <c r="H12" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="G13" t="inlineStr">
-        <is>
-          <t>app_name</t>
-        </is>
-      </c>
-      <c r="H13" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="G14" t="inlineStr">
-        <is>
-          <t>app_version</t>
-        </is>
-      </c>
-      <c r="H14" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="G15" t="inlineStr">
-        <is>
-          <t>l:event:playhead</t>
-        </is>
-      </c>
-      <c r="H15" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="G16" t="inlineStr">
-        <is>
-          <t>page_type</t>
-        </is>
-      </c>
-      <c r="H16" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="G17" t="inlineStr">
-        <is>
-          <t>primary_business_unit</t>
-        </is>
-      </c>
-      <c r="H17" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="G18" t="inlineStr">
-        <is>
-          <t>user_fox_anonymous_profile_id</t>
-        </is>
-      </c>
-      <c r="H18" t="n">
-        <v>2</v>
-      </c>
-    </row>
+    <row r="2"/>
+    <row r="3"/>
+    <row r="4"/>
+    <row r="5"/>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>